<commit_message>
new new 22 aprile
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -680,12 +680,6 @@
     <t>850</t>
   </si>
   <si>
-    <t>3/4/2018</t>
-  </si>
-  <si>
-    <t>70</t>
-  </si>
-  <si>
     <t>9/4/2018</t>
   </si>
   <si>
@@ -699,6 +693,12 @@
   </si>
   <si>
     <t>500</t>
+  </si>
+  <si>
+    <t>22/4/2018</t>
+  </si>
+  <si>
+    <t>80</t>
   </si>
 </sst>
 </file>
@@ -1854,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IU149"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A112" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="C125" sqref="C125"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -2838,10 +2838,10 @@
         <v>28</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="D24" s="19"/>
       <c r="E24" s="19" t="s">
@@ -4414,14 +4414,14 @@
         <v>21</v>
       </c>
       <c r="F94" s="20">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G94" s="43">
         <v>2.9</v>
       </c>
       <c r="H94" s="46">
         <f t="shared" si="2"/>
-        <v>304.5</v>
+        <v>298.7</v>
       </c>
       <c r="I94" s="42"/>
     </row>
@@ -4619,7 +4619,7 @@
         <v>104</v>
       </c>
       <c r="B102" s="19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C102" s="19" t="s">
         <v>177</v>
@@ -5044,7 +5044,7 @@
         <v>121</v>
       </c>
       <c r="B119" s="19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C119" s="19" t="s">
         <v>172</v>
@@ -5155,10 +5155,10 @@
         <v>128</v>
       </c>
       <c r="B124" s="19" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C124" s="19" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D124" s="19" t="s">
         <v>13</v>
@@ -5182,10 +5182,10 @@
         <v>179</v>
       </c>
       <c r="B125" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C125" s="19" t="s">
         <v>224</v>
-      </c>
-      <c r="C125" s="19" t="s">
-        <v>226</v>
       </c>
       <c r="D125" s="19" t="s">
         <v>13</v>
@@ -5903,7 +5903,7 @@
     <row r="147" spans="1:8" ht="48.75" customHeight="1">
       <c r="H147" s="47">
         <f>SUM(H3:H146)</f>
-        <v>19312.921999999995</v>
+        <v>19307.121999999999</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="29.1" customHeight="1"/>

</xml_diff>

<commit_message>
new new 27 aprile
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -10,15 +10,15 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$146</definedName>
-    <definedName name="Excel_BuiltIn_Print_Area" localSheetId="0">Sheet1!$A$1:$H$130</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$147</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area" localSheetId="0">Sheet1!$A$1:$H$131</definedName>
   </definedNames>
   <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="230">
   <si>
     <t>PRODOTTO</t>
   </si>
@@ -699,6 +699,15 @@
   </si>
   <si>
     <t>80</t>
+  </si>
+  <si>
+    <t>Porta abiti lunghi soffietto</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>26/4/2018</t>
   </si>
 </sst>
 </file>
@@ -1852,10 +1861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IU149"/>
+  <dimension ref="A1:IU150"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -2606,14 +2615,14 @@
         <v>16</v>
       </c>
       <c r="F16" s="17">
-        <v>739</v>
+        <v>699</v>
       </c>
       <c r="G16" s="13">
         <v>1.8280000000000001</v>
       </c>
       <c r="H16" s="14">
         <f t="shared" si="0"/>
-        <v>1350.8920000000001</v>
+        <v>1277.7720000000002</v>
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
@@ -3610,14 +3619,14 @@
         <v>21</v>
       </c>
       <c r="F58" s="20">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G58" s="21">
         <v>0.44</v>
       </c>
       <c r="H58" s="14">
         <f t="shared" si="1"/>
-        <v>5.28</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3834,7 +3843,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="H68" s="14">
-        <f t="shared" ref="H68:H146" si="2">F68*G68</f>
+        <f t="shared" ref="H68:H147" si="2">F68*G68</f>
         <v>210.70000000000002</v>
       </c>
     </row>
@@ -4092,14 +4101,14 @@
         <v>21</v>
       </c>
       <c r="F80" s="20">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G80" s="21">
         <v>1.1000000000000001</v>
       </c>
       <c r="H80" s="14">
         <f t="shared" si="2"/>
-        <v>7.7000000000000011</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="81" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4182,14 +4191,14 @@
         <v>10</v>
       </c>
       <c r="F84" s="20">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G84" s="21">
         <v>12.5</v>
       </c>
       <c r="H84" s="14">
         <f t="shared" si="2"/>
-        <v>75</v>
+        <v>50</v>
       </c>
     </row>
     <row r="85" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4427,13 +4436,13 @@
     </row>
     <row r="95" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A95" s="18" t="s">
-        <v>98</v>
+        <v>227</v>
       </c>
       <c r="B95" s="19" t="s">
-        <v>184</v>
+        <v>229</v>
       </c>
       <c r="C95" s="19" t="s">
-        <v>182</v>
+        <v>228</v>
       </c>
       <c r="D95" s="19" t="s">
         <v>185</v>
@@ -4442,20 +4451,20 @@
         <v>21</v>
       </c>
       <c r="F95" s="20">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="G95" s="43">
-        <v>3.45</v>
+        <v>4.8</v>
       </c>
       <c r="H95" s="46">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>230.39999999999998</v>
       </c>
       <c r="I95" s="42"/>
     </row>
     <row r="96" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A96" s="18" t="s">
-        <v>191</v>
+        <v>98</v>
       </c>
       <c r="B96" s="19" t="s">
         <v>184</v>
@@ -4470,388 +4479,389 @@
         <v>21</v>
       </c>
       <c r="F96" s="20">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="G96" s="43">
-        <v>3.75</v>
+        <v>3.45</v>
       </c>
       <c r="H96" s="46">
         <f t="shared" si="2"/>
-        <v>183.75</v>
+        <v>0</v>
       </c>
       <c r="I96" s="42"/>
     </row>
     <row r="97" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A97" s="18" t="s">
-        <v>99</v>
+        <v>191</v>
       </c>
       <c r="B97" s="19" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C97" s="19" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="D97" s="19" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="E97" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F97" s="20">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="G97" s="43">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="H97" s="46">
         <f t="shared" si="2"/>
-        <v>48</v>
+        <v>183.75</v>
       </c>
       <c r="I97" s="42"/>
     </row>
     <row r="98" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A98" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C98" s="19" t="s">
         <v>172</v>
       </c>
       <c r="D98" s="19" t="s">
-        <v>29</v>
+        <v>202</v>
       </c>
       <c r="E98" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F98" s="20">
+        <v>12</v>
+      </c>
+      <c r="G98" s="43">
+        <v>4</v>
+      </c>
+      <c r="H98" s="46">
+        <f t="shared" si="2"/>
         <v>48</v>
-      </c>
-      <c r="G98" s="43">
-        <v>0.8</v>
-      </c>
-      <c r="H98" s="46">
-        <f t="shared" si="2"/>
-        <v>38.400000000000006</v>
       </c>
       <c r="I98" s="42"/>
     </row>
     <row r="99" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A99" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="C99" s="19" t="s">
-        <v>199</v>
+        <v>172</v>
       </c>
       <c r="D99" s="19" t="s">
-        <v>198</v>
+        <v>29</v>
       </c>
       <c r="E99" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F99" s="20">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="G99" s="43">
-        <v>11.7</v>
+        <v>0.8</v>
       </c>
       <c r="H99" s="46">
         <f t="shared" si="2"/>
-        <v>117</v>
-      </c>
+        <v>38.400000000000006</v>
+      </c>
+      <c r="I99" s="42"/>
     </row>
     <row r="100" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A100" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="B100" s="19"/>
-      <c r="C100" s="19"/>
+        <v>101</v>
+      </c>
+      <c r="B100" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="C100" s="19" t="s">
+        <v>199</v>
+      </c>
       <c r="D100" s="19" t="s">
-        <v>15</v>
+        <v>198</v>
       </c>
       <c r="E100" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F100" s="20">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="G100" s="43">
-        <v>2.4</v>
+        <v>11.7</v>
       </c>
       <c r="H100" s="46">
         <f t="shared" si="2"/>
-        <v>408</v>
+        <v>117</v>
       </c>
     </row>
     <row r="101" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A101" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="B101" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="C101" s="19" t="s">
-        <v>197</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="B101" s="19"/>
+      <c r="C101" s="19"/>
       <c r="D101" s="19" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="E101" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F101" s="20">
-        <v>30</v>
-      </c>
-      <c r="G101" s="21">
-        <v>0.83</v>
-      </c>
-      <c r="H101" s="45">
-        <f t="shared" si="2"/>
-        <v>24.9</v>
+        <v>170</v>
+      </c>
+      <c r="G101" s="43">
+        <v>2.4</v>
+      </c>
+      <c r="H101" s="46">
+        <f t="shared" si="2"/>
+        <v>408</v>
       </c>
     </row>
     <row r="102" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A102" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B102" s="19" t="s">
-        <v>220</v>
+        <v>195</v>
       </c>
       <c r="C102" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="D102" s="19"/>
+        <v>197</v>
+      </c>
+      <c r="D102" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="E102" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F102" s="20">
-        <v>139</v>
+        <v>30</v>
       </c>
       <c r="G102" s="21">
-        <v>4.7</v>
-      </c>
-      <c r="H102" s="14">
-        <f t="shared" si="2"/>
-        <v>653.30000000000007</v>
+        <v>0.83</v>
+      </c>
+      <c r="H102" s="45">
+        <f t="shared" si="2"/>
+        <v>24.9</v>
       </c>
     </row>
     <row r="103" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A103" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B103" s="19" t="s">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="C103" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="D103" s="19" t="s">
-        <v>158</v>
-      </c>
+      <c r="D103" s="19"/>
       <c r="E103" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F103" s="20">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="G103" s="21">
-        <v>2.5</v>
+        <v>4.7</v>
       </c>
       <c r="H103" s="14">
         <f t="shared" si="2"/>
-        <v>262.5</v>
+        <v>653.30000000000007</v>
       </c>
     </row>
     <row r="104" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A104" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="B104" s="19"/>
-      <c r="C104" s="19"/>
-      <c r="D104" s="34"/>
+        <v>105</v>
+      </c>
+      <c r="B104" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="C104" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="D104" s="19" t="s">
+        <v>158</v>
+      </c>
       <c r="E104" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F104" s="20">
-        <v>6</v>
+        <v>105</v>
       </c>
       <c r="G104" s="21">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="H104" s="14">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>262.5</v>
       </c>
     </row>
     <row r="105" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A105" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B105" s="19"/>
       <c r="C105" s="19"/>
-      <c r="D105" s="19"/>
+      <c r="D105" s="34"/>
       <c r="E105" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F105" s="20">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="G105" s="21">
         <v>2</v>
       </c>
       <c r="H105" s="14">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="106" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A106" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="B106" s="19" t="s">
-        <v>206</v>
-      </c>
-      <c r="C106" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="D106" s="19" t="s">
-        <v>175</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="B106" s="19"/>
+      <c r="C106" s="19"/>
+      <c r="D106" s="19"/>
       <c r="E106" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F106" s="20">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="G106" s="21">
-        <v>41.34</v>
+        <v>2</v>
       </c>
       <c r="H106" s="14">
         <f t="shared" si="2"/>
-        <v>289.38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="107" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A107" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="B107" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="C107" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="D107" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="E107" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F107" s="20">
+        <v>7</v>
+      </c>
+      <c r="G107" s="21">
+        <v>41.34</v>
+      </c>
+      <c r="H107" s="14">
+        <f t="shared" si="2"/>
+        <v>289.38</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A108" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="B107" s="19" t="s">
+      <c r="B108" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="C107" s="19" t="s">
+      <c r="C108" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="D107" s="19" t="s">
+      <c r="D108" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="E107" s="19" t="s">
+      <c r="E108" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="F107" s="20">
+      <c r="F108" s="20">
         <v>30</v>
       </c>
-      <c r="G107" s="21">
+      <c r="G108" s="21">
         <v>2.7</v>
       </c>
-      <c r="H107" s="14">
+      <c r="H108" s="14">
         <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
-    <row r="108" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A108" s="23" t="s">
+    <row r="109" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A109" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="B108" s="29">
+      <c r="B109" s="29">
         <v>43140</v>
       </c>
-      <c r="C108" s="11">
+      <c r="C109" s="11">
         <v>12</v>
       </c>
-      <c r="D108" s="11" t="s">
+      <c r="D109" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="E108" s="11" t="s">
+      <c r="E109" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="F108" s="24">
+      <c r="F109" s="24">
         <v>14</v>
       </c>
-      <c r="G108" s="25">
+      <c r="G109" s="25">
         <v>6</v>
       </c>
-      <c r="H108" s="14">
+      <c r="H109" s="14">
         <f t="shared" si="2"/>
         <v>84</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A109" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="B109" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="C109" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="D109" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="E109" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F109" s="20">
-        <v>1116</v>
-      </c>
-      <c r="G109" s="21">
-        <v>0.66</v>
-      </c>
-      <c r="H109" s="14">
-        <f t="shared" si="2"/>
-        <v>736.56000000000006</v>
       </c>
     </row>
     <row r="110" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A110" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="C110" s="19" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="D110" s="19" t="s">
-        <v>29</v>
+        <v>188</v>
       </c>
       <c r="E110" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F110" s="20">
-        <v>5</v>
+        <v>1116</v>
       </c>
       <c r="G110" s="21">
-        <v>2.85</v>
+        <v>0.66</v>
       </c>
       <c r="H110" s="14">
         <f t="shared" si="2"/>
-        <v>14.25</v>
+        <v>736.56000000000006</v>
       </c>
     </row>
     <row r="111" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A111" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B111" s="19" t="s">
-        <v>212</v>
+        <v>170</v>
       </c>
       <c r="C111" s="19" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="D111" s="19" t="s">
         <v>29</v>
@@ -4860,146 +4870,146 @@
         <v>21</v>
       </c>
       <c r="F111" s="20">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G111" s="21">
-        <v>1.72</v>
+        <v>2.85</v>
       </c>
       <c r="H111" s="14">
         <f t="shared" si="2"/>
-        <v>12.04</v>
+        <v>14.25</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A112" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B112" s="19" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="C112" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="D112" s="19"/>
+        <v>183</v>
+      </c>
+      <c r="D112" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="E112" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F112" s="20">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G112" s="21">
-        <v>2.9</v>
+        <v>1.72</v>
       </c>
       <c r="H112" s="14">
         <f t="shared" si="2"/>
-        <v>31.9</v>
+        <v>12.04</v>
       </c>
     </row>
     <row r="113" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A113" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B113" s="19" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="C113" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="D113" s="19" t="s">
-        <v>29</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="D113" s="19"/>
       <c r="E113" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F113" s="20">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G113" s="21">
-        <v>1.72</v>
+        <v>2.9</v>
       </c>
       <c r="H113" s="14">
         <f t="shared" si="2"/>
-        <v>5.16</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="114" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A114" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="B114" s="19"/>
-      <c r="C114" s="19"/>
-      <c r="D114" s="35"/>
+        <v>115</v>
+      </c>
+      <c r="B114" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="C114" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="D114" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="E114" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F114" s="20">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G114" s="21">
-        <v>5</v>
+        <v>1.72</v>
       </c>
       <c r="H114" s="14">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>5.16</v>
       </c>
     </row>
     <row r="115" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A115" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B115" s="19"/>
       <c r="C115" s="19"/>
-      <c r="D115" s="19"/>
+      <c r="D115" s="35"/>
       <c r="E115" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F115" s="20">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G115" s="21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H115" s="14">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="116" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A116" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="B116" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="C116" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="D116" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B116" s="19"/>
+      <c r="C116" s="19"/>
+      <c r="D116" s="19"/>
+      <c r="E116" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F116" s="20">
         <v>9</v>
       </c>
-      <c r="E116" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F116" s="20">
-        <v>169</v>
-      </c>
       <c r="G116" s="21">
-        <v>2.69</v>
+        <v>1</v>
       </c>
       <c r="H116" s="14">
         <f t="shared" si="2"/>
-        <v>454.61</v>
+        <v>9</v>
       </c>
     </row>
     <row r="117" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A117" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B117" s="19" t="s">
         <v>174</v>
       </c>
       <c r="C117" s="19" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D117" s="19" t="s">
         <v>9</v>
@@ -5008,88 +5018,94 @@
         <v>12</v>
       </c>
       <c r="F117" s="20">
-        <v>113</v>
+        <v>169</v>
       </c>
       <c r="G117" s="21">
-        <v>3.3</v>
+        <v>2.69</v>
       </c>
       <c r="H117" s="14">
         <f t="shared" si="2"/>
-        <v>372.9</v>
+        <v>454.61</v>
       </c>
     </row>
     <row r="118" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A118" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="B118" s="19"/>
-      <c r="C118" s="19"/>
-      <c r="D118" s="19"/>
+        <v>119</v>
+      </c>
+      <c r="B118" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="C118" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="D118" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="E118" s="19" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F118" s="20">
-        <v>5</v>
+        <v>113</v>
       </c>
       <c r="G118" s="21">
-        <v>2.87</v>
+        <v>3.3</v>
       </c>
       <c r="H118" s="14">
         <f t="shared" si="2"/>
-        <v>14.350000000000001</v>
+        <v>372.9</v>
       </c>
     </row>
     <row r="119" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A119" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B119" s="19"/>
+      <c r="C119" s="19"/>
+      <c r="D119" s="19"/>
+      <c r="E119" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F119" s="20">
+        <v>5</v>
+      </c>
+      <c r="G119" s="21">
+        <v>2.87</v>
+      </c>
+      <c r="H119" s="14">
+        <f t="shared" si="2"/>
+        <v>14.350000000000001</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A120" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="B119" s="19" t="s">
+      <c r="B120" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="C119" s="19" t="s">
+      <c r="C120" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="D119" s="19" t="s">
+      <c r="D120" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="E119" s="19" t="s">
+      <c r="E120" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="F119" s="20">
+      <c r="F120" s="20">
         <v>6</v>
       </c>
-      <c r="G119" s="21">
+      <c r="G120" s="21">
         <v>7</v>
       </c>
-      <c r="H119" s="14">
+      <c r="H120" s="14">
         <f t="shared" si="2"/>
         <v>42</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" s="36" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A120" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="B120" s="19"/>
-      <c r="C120" s="19"/>
-      <c r="D120" s="19"/>
-      <c r="E120" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F120" s="20">
-        <v>584</v>
-      </c>
-      <c r="G120" s="21">
-        <v>3</v>
-      </c>
-      <c r="H120" s="14">
-        <f t="shared" si="2"/>
-        <v>1752</v>
       </c>
     </row>
     <row r="121" spans="1:8" s="36" customFormat="1" ht="28.35" customHeight="1">
       <c r="A121" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B121" s="19"/>
       <c r="C121" s="19"/>
@@ -5098,94 +5114,88 @@
         <v>21</v>
       </c>
       <c r="F121" s="20">
+        <v>584</v>
+      </c>
+      <c r="G121" s="21">
+        <v>3</v>
+      </c>
+      <c r="H121" s="14">
+        <f t="shared" si="2"/>
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" s="36" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A122" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B122" s="19"/>
+      <c r="C122" s="19"/>
+      <c r="D122" s="19"/>
+      <c r="E122" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F122" s="20">
         <v>1</v>
       </c>
-      <c r="G121" s="21">
+      <c r="G122" s="21">
         <v>1.96</v>
       </c>
-      <c r="H121" s="14">
+      <c r="H122" s="14">
         <f t="shared" si="2"/>
         <v>1.96</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="28.35" customHeight="1">
-      <c r="A122" s="23" t="s">
+    <row r="123" spans="1:8" ht="28.35" customHeight="1">
+      <c r="A123" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="B122" s="11"/>
-      <c r="C122" s="11"/>
-      <c r="D122" s="11"/>
-      <c r="E122" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F122" s="24">
-        <v>7</v>
-      </c>
-      <c r="G122" s="25">
-        <v>1.97</v>
-      </c>
-      <c r="H122" s="14">
-        <f t="shared" si="2"/>
-        <v>13.79</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" ht="28.35" customHeight="1">
-      <c r="A123" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="B123" s="19"/>
-      <c r="C123" s="19"/>
-      <c r="D123" s="19"/>
+      <c r="B123" s="11"/>
+      <c r="C123" s="11"/>
+      <c r="D123" s="11"/>
       <c r="E123" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F123" s="20">
-        <v>95</v>
-      </c>
-      <c r="G123" s="21">
+      <c r="F123" s="24">
         <v>7</v>
       </c>
+      <c r="G123" s="25">
+        <v>1.97</v>
+      </c>
       <c r="H123" s="14">
         <f t="shared" si="2"/>
-        <v>665</v>
+        <v>13.79</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="28.35" customHeight="1">
       <c r="A124" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="B124" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="C124" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="D124" s="19" t="s">
-        <v>13</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="B124" s="19"/>
+      <c r="C124" s="19"/>
+      <c r="D124" s="19"/>
       <c r="E124" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F124" s="20">
-        <v>250</v>
+        <v>95</v>
       </c>
       <c r="G124" s="21">
-        <v>2.69</v>
+        <v>7</v>
       </c>
       <c r="H124" s="14">
         <f t="shared" si="2"/>
-        <v>672.5</v>
+        <v>665</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="28.35" customHeight="1">
       <c r="A125" s="18" t="s">
-        <v>179</v>
+        <v>128</v>
       </c>
       <c r="B125" s="19" t="s">
         <v>222</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D125" s="19" t="s">
         <v>13</v>
@@ -5194,61 +5204,67 @@
         <v>12</v>
       </c>
       <c r="F125" s="20">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="G125" s="21">
-        <v>2.21</v>
+        <v>2.69</v>
       </c>
       <c r="H125" s="14">
         <f t="shared" si="2"/>
-        <v>442</v>
+        <v>672.5</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="28.35" customHeight="1">
-      <c r="A126" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="B126" s="11"/>
-      <c r="C126" s="11"/>
-      <c r="D126" s="11"/>
+      <c r="A126" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="B126" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C126" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="D126" s="19" t="s">
+        <v>13</v>
+      </c>
       <c r="E126" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F126" s="24">
-        <v>100</v>
-      </c>
-      <c r="G126" s="25">
-        <v>1.43</v>
+      <c r="F126" s="20">
+        <v>200</v>
+      </c>
+      <c r="G126" s="21">
+        <v>2.21</v>
       </c>
       <c r="H126" s="14">
         <f t="shared" si="2"/>
-        <v>143</v>
+        <v>442</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="28.35" customHeight="1">
-      <c r="A127" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="B127" s="19"/>
-      <c r="C127" s="19"/>
-      <c r="D127" s="19"/>
+      <c r="A127" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="B127" s="11"/>
+      <c r="C127" s="11"/>
+      <c r="D127" s="11"/>
       <c r="E127" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F127" s="20">
-        <v>4</v>
-      </c>
-      <c r="G127" s="21">
-        <v>8.5</v>
+      <c r="F127" s="24">
+        <v>100</v>
+      </c>
+      <c r="G127" s="25">
+        <v>1.43</v>
       </c>
       <c r="H127" s="14">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>143</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="28.35" customHeight="1">
       <c r="A128" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B128" s="19"/>
       <c r="C128" s="19"/>
@@ -5257,373 +5273,373 @@
         <v>12</v>
       </c>
       <c r="F128" s="20">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="G128" s="21">
-        <v>5</v>
+        <v>8.5</v>
       </c>
       <c r="H128" s="14">
         <f t="shared" si="2"/>
-        <v>85</v>
+        <v>34</v>
       </c>
     </row>
     <row r="129" spans="1:255" ht="28.35" customHeight="1">
       <c r="A129" s="18" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="B129" s="19"/>
       <c r="C129" s="19"/>
-      <c r="D129" s="19" t="s">
-        <v>157</v>
-      </c>
+      <c r="D129" s="19"/>
       <c r="E129" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F129" s="20">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G129" s="21">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="H129" s="14">
         <f t="shared" si="2"/>
-        <v>564</v>
+        <v>85</v>
       </c>
     </row>
     <row r="130" spans="1:255" ht="28.35" customHeight="1">
-      <c r="A130" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="B130" s="11"/>
-      <c r="C130" s="11"/>
-      <c r="D130" s="11"/>
+      <c r="A130" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="B130" s="19"/>
+      <c r="C130" s="19"/>
+      <c r="D130" s="19" t="s">
+        <v>157</v>
+      </c>
       <c r="E130" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F130" s="24">
+      <c r="F130" s="20">
+        <v>12</v>
+      </c>
+      <c r="G130" s="21">
+        <v>47</v>
+      </c>
+      <c r="H130" s="14">
+        <f t="shared" si="2"/>
+        <v>564</v>
+      </c>
+    </row>
+    <row r="131" spans="1:255" ht="28.35" customHeight="1">
+      <c r="A131" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="B131" s="11"/>
+      <c r="C131" s="11"/>
+      <c r="D131" s="11"/>
+      <c r="E131" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F131" s="24">
         <v>22</v>
       </c>
-      <c r="G130" s="25">
+      <c r="G131" s="25">
         <v>2.97</v>
       </c>
-      <c r="H130" s="14">
+      <c r="H131" s="14">
         <f t="shared" si="2"/>
         <v>65.34</v>
       </c>
     </row>
-    <row r="131" spans="1:255" ht="28.35" customHeight="1">
-      <c r="A131" s="18" t="s">
+    <row r="132" spans="1:255" ht="28.35" customHeight="1">
+      <c r="A132" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="B131" s="19"/>
-      <c r="C131" s="19"/>
-      <c r="D131" s="19"/>
-      <c r="E131" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F131" s="20">
+      <c r="B132" s="19"/>
+      <c r="C132" s="19"/>
+      <c r="D132" s="19"/>
+      <c r="E132" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F132" s="20">
         <v>140</v>
       </c>
-      <c r="G131" s="21">
+      <c r="G132" s="21">
         <v>1.1299999999999999</v>
       </c>
-      <c r="H131" s="14">
+      <c r="H132" s="14">
         <f t="shared" si="2"/>
         <v>158.19999999999999</v>
       </c>
-      <c r="I131"/>
-      <c r="J131"/>
-      <c r="K131"/>
-      <c r="L131"/>
-      <c r="M131"/>
-      <c r="N131"/>
-      <c r="O131"/>
-      <c r="P131"/>
-      <c r="Q131"/>
-      <c r="R131"/>
-      <c r="S131"/>
-      <c r="T131"/>
-      <c r="U131"/>
-      <c r="V131"/>
-      <c r="W131"/>
-      <c r="X131"/>
-      <c r="Y131"/>
-      <c r="Z131"/>
-      <c r="AA131"/>
-      <c r="AB131"/>
-      <c r="AC131"/>
-      <c r="AD131"/>
-      <c r="AE131"/>
-      <c r="AF131"/>
-      <c r="AG131"/>
-      <c r="AH131"/>
-      <c r="AI131"/>
-      <c r="AJ131"/>
-      <c r="AK131"/>
-      <c r="AL131"/>
-      <c r="AM131"/>
-      <c r="AN131"/>
-      <c r="AO131"/>
-      <c r="AP131"/>
-      <c r="AQ131"/>
-      <c r="AR131"/>
-      <c r="AS131"/>
-      <c r="AT131"/>
-      <c r="AU131"/>
-      <c r="AV131"/>
-      <c r="AW131"/>
-      <c r="AX131"/>
-      <c r="AY131"/>
-      <c r="AZ131"/>
-      <c r="BA131"/>
-      <c r="BB131"/>
-      <c r="BC131"/>
-      <c r="BD131"/>
-      <c r="BE131"/>
-      <c r="BF131"/>
-      <c r="BG131"/>
-      <c r="BH131"/>
-      <c r="BI131"/>
-      <c r="BJ131"/>
-      <c r="BK131"/>
-      <c r="BL131"/>
-      <c r="BM131"/>
-      <c r="BN131"/>
-      <c r="BO131"/>
-      <c r="BP131"/>
-      <c r="BQ131"/>
-      <c r="BR131"/>
-      <c r="BS131"/>
-      <c r="BT131"/>
-      <c r="BU131"/>
-      <c r="BV131"/>
-      <c r="BW131"/>
-      <c r="BX131"/>
-      <c r="BY131"/>
-      <c r="BZ131"/>
-      <c r="CA131"/>
-      <c r="CB131"/>
-      <c r="CC131"/>
-      <c r="CD131"/>
-      <c r="CE131"/>
-      <c r="CF131"/>
-      <c r="CG131"/>
-      <c r="CH131"/>
-      <c r="CI131"/>
-      <c r="CJ131"/>
-      <c r="CK131"/>
-      <c r="CL131"/>
-      <c r="CM131"/>
-      <c r="CN131"/>
-      <c r="CO131"/>
-      <c r="CP131"/>
-      <c r="CQ131"/>
-      <c r="CR131"/>
-      <c r="CS131"/>
-      <c r="CT131"/>
-      <c r="CU131"/>
-      <c r="CV131"/>
-      <c r="CW131"/>
-      <c r="CX131"/>
-      <c r="CY131"/>
-      <c r="CZ131"/>
-      <c r="DA131"/>
-      <c r="DB131"/>
-      <c r="DC131"/>
-      <c r="DD131"/>
-      <c r="DE131"/>
-      <c r="DF131"/>
-      <c r="DG131"/>
-      <c r="DH131"/>
-      <c r="DI131"/>
-      <c r="DJ131"/>
-      <c r="DK131"/>
-      <c r="DL131"/>
-      <c r="DM131"/>
-      <c r="DN131"/>
-      <c r="DO131"/>
-      <c r="DP131"/>
-      <c r="DQ131"/>
-      <c r="DR131"/>
-      <c r="DS131"/>
-      <c r="DT131"/>
-      <c r="DU131"/>
-      <c r="DV131"/>
-      <c r="DW131"/>
-      <c r="DX131"/>
-      <c r="DY131"/>
-      <c r="DZ131"/>
-      <c r="EA131"/>
-      <c r="EB131"/>
-      <c r="EC131"/>
-      <c r="ED131"/>
-      <c r="EE131"/>
-      <c r="EF131"/>
-      <c r="EG131"/>
-      <c r="EH131"/>
-      <c r="EI131"/>
-      <c r="EJ131"/>
-      <c r="EK131"/>
-      <c r="EL131"/>
-      <c r="EM131"/>
-      <c r="EN131"/>
-      <c r="EO131"/>
-      <c r="EP131"/>
-      <c r="EQ131"/>
-      <c r="ER131"/>
-      <c r="ES131"/>
-      <c r="ET131"/>
-      <c r="EU131"/>
-      <c r="EV131"/>
-      <c r="EW131"/>
-      <c r="EX131"/>
-      <c r="EY131"/>
-      <c r="EZ131"/>
-      <c r="FA131"/>
-      <c r="FB131"/>
-      <c r="FC131"/>
-      <c r="FD131"/>
-      <c r="FE131"/>
-      <c r="FF131"/>
-      <c r="FG131"/>
-      <c r="FH131"/>
-      <c r="FI131"/>
-      <c r="FJ131"/>
-      <c r="FK131"/>
-      <c r="FL131"/>
-      <c r="FM131"/>
-      <c r="FN131"/>
-      <c r="FO131"/>
-      <c r="FP131"/>
-      <c r="FQ131"/>
-      <c r="FR131"/>
-      <c r="FS131"/>
-      <c r="FT131"/>
-      <c r="FU131"/>
-      <c r="FV131"/>
-      <c r="FW131"/>
-      <c r="FX131"/>
-      <c r="FY131"/>
-      <c r="FZ131"/>
-      <c r="GA131"/>
-      <c r="GB131"/>
-      <c r="GC131"/>
-      <c r="GD131"/>
-      <c r="GE131"/>
-      <c r="GF131"/>
-      <c r="GG131"/>
-      <c r="GH131"/>
-      <c r="GI131"/>
-      <c r="GJ131"/>
-      <c r="GK131"/>
-      <c r="GL131"/>
-      <c r="GM131"/>
-      <c r="GN131"/>
-      <c r="GO131"/>
-      <c r="GP131"/>
-      <c r="GQ131"/>
-      <c r="GR131"/>
-      <c r="GS131"/>
-      <c r="GT131"/>
-      <c r="GU131"/>
-      <c r="GV131"/>
-      <c r="GW131"/>
-      <c r="GX131"/>
-      <c r="GY131"/>
-      <c r="GZ131"/>
-      <c r="HA131"/>
-      <c r="HB131"/>
-      <c r="HC131"/>
-      <c r="HD131"/>
-      <c r="HE131"/>
-      <c r="HF131"/>
-      <c r="HG131"/>
-      <c r="HH131"/>
-      <c r="HI131"/>
-      <c r="HJ131"/>
-      <c r="HK131"/>
-      <c r="HL131"/>
-      <c r="HM131"/>
-      <c r="HN131"/>
-      <c r="HO131"/>
-      <c r="HP131"/>
-      <c r="HQ131"/>
-      <c r="HR131"/>
-      <c r="HS131"/>
-      <c r="HT131"/>
-      <c r="HU131"/>
-      <c r="HV131"/>
-      <c r="HW131"/>
-      <c r="HX131"/>
-      <c r="HY131"/>
-      <c r="HZ131"/>
-      <c r="IA131"/>
-      <c r="IB131"/>
-      <c r="IC131"/>
-      <c r="ID131"/>
-      <c r="IE131"/>
-      <c r="IF131"/>
-      <c r="IG131"/>
-      <c r="IH131"/>
-      <c r="II131"/>
-      <c r="IJ131"/>
-      <c r="IK131"/>
-      <c r="IL131"/>
-      <c r="IM131"/>
-      <c r="IN131"/>
-      <c r="IO131"/>
-      <c r="IP131"/>
-      <c r="IQ131"/>
-      <c r="IR131"/>
-      <c r="IS131"/>
-      <c r="IT131"/>
-      <c r="IU131"/>
-    </row>
-    <row r="132" spans="1:255" ht="28.35" customHeight="1">
-      <c r="A132" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="B132" s="11"/>
-      <c r="C132" s="11"/>
-      <c r="D132" s="11"/>
-      <c r="E132" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F132" s="24">
-        <v>25</v>
-      </c>
-      <c r="G132" s="25">
-        <v>5</v>
-      </c>
-      <c r="H132" s="14">
-        <f t="shared" si="2"/>
-        <v>125</v>
-      </c>
+      <c r="I132"/>
+      <c r="J132"/>
+      <c r="K132"/>
+      <c r="L132"/>
+      <c r="M132"/>
+      <c r="N132"/>
+      <c r="O132"/>
+      <c r="P132"/>
+      <c r="Q132"/>
+      <c r="R132"/>
+      <c r="S132"/>
+      <c r="T132"/>
+      <c r="U132"/>
+      <c r="V132"/>
+      <c r="W132"/>
+      <c r="X132"/>
+      <c r="Y132"/>
+      <c r="Z132"/>
+      <c r="AA132"/>
+      <c r="AB132"/>
+      <c r="AC132"/>
+      <c r="AD132"/>
+      <c r="AE132"/>
+      <c r="AF132"/>
+      <c r="AG132"/>
+      <c r="AH132"/>
+      <c r="AI132"/>
+      <c r="AJ132"/>
+      <c r="AK132"/>
+      <c r="AL132"/>
+      <c r="AM132"/>
+      <c r="AN132"/>
+      <c r="AO132"/>
+      <c r="AP132"/>
+      <c r="AQ132"/>
+      <c r="AR132"/>
+      <c r="AS132"/>
+      <c r="AT132"/>
+      <c r="AU132"/>
+      <c r="AV132"/>
+      <c r="AW132"/>
+      <c r="AX132"/>
+      <c r="AY132"/>
+      <c r="AZ132"/>
+      <c r="BA132"/>
+      <c r="BB132"/>
+      <c r="BC132"/>
+      <c r="BD132"/>
+      <c r="BE132"/>
+      <c r="BF132"/>
+      <c r="BG132"/>
+      <c r="BH132"/>
+      <c r="BI132"/>
+      <c r="BJ132"/>
+      <c r="BK132"/>
+      <c r="BL132"/>
+      <c r="BM132"/>
+      <c r="BN132"/>
+      <c r="BO132"/>
+      <c r="BP132"/>
+      <c r="BQ132"/>
+      <c r="BR132"/>
+      <c r="BS132"/>
+      <c r="BT132"/>
+      <c r="BU132"/>
+      <c r="BV132"/>
+      <c r="BW132"/>
+      <c r="BX132"/>
+      <c r="BY132"/>
+      <c r="BZ132"/>
+      <c r="CA132"/>
+      <c r="CB132"/>
+      <c r="CC132"/>
+      <c r="CD132"/>
+      <c r="CE132"/>
+      <c r="CF132"/>
+      <c r="CG132"/>
+      <c r="CH132"/>
+      <c r="CI132"/>
+      <c r="CJ132"/>
+      <c r="CK132"/>
+      <c r="CL132"/>
+      <c r="CM132"/>
+      <c r="CN132"/>
+      <c r="CO132"/>
+      <c r="CP132"/>
+      <c r="CQ132"/>
+      <c r="CR132"/>
+      <c r="CS132"/>
+      <c r="CT132"/>
+      <c r="CU132"/>
+      <c r="CV132"/>
+      <c r="CW132"/>
+      <c r="CX132"/>
+      <c r="CY132"/>
+      <c r="CZ132"/>
+      <c r="DA132"/>
+      <c r="DB132"/>
+      <c r="DC132"/>
+      <c r="DD132"/>
+      <c r="DE132"/>
+      <c r="DF132"/>
+      <c r="DG132"/>
+      <c r="DH132"/>
+      <c r="DI132"/>
+      <c r="DJ132"/>
+      <c r="DK132"/>
+      <c r="DL132"/>
+      <c r="DM132"/>
+      <c r="DN132"/>
+      <c r="DO132"/>
+      <c r="DP132"/>
+      <c r="DQ132"/>
+      <c r="DR132"/>
+      <c r="DS132"/>
+      <c r="DT132"/>
+      <c r="DU132"/>
+      <c r="DV132"/>
+      <c r="DW132"/>
+      <c r="DX132"/>
+      <c r="DY132"/>
+      <c r="DZ132"/>
+      <c r="EA132"/>
+      <c r="EB132"/>
+      <c r="EC132"/>
+      <c r="ED132"/>
+      <c r="EE132"/>
+      <c r="EF132"/>
+      <c r="EG132"/>
+      <c r="EH132"/>
+      <c r="EI132"/>
+      <c r="EJ132"/>
+      <c r="EK132"/>
+      <c r="EL132"/>
+      <c r="EM132"/>
+      <c r="EN132"/>
+      <c r="EO132"/>
+      <c r="EP132"/>
+      <c r="EQ132"/>
+      <c r="ER132"/>
+      <c r="ES132"/>
+      <c r="ET132"/>
+      <c r="EU132"/>
+      <c r="EV132"/>
+      <c r="EW132"/>
+      <c r="EX132"/>
+      <c r="EY132"/>
+      <c r="EZ132"/>
+      <c r="FA132"/>
+      <c r="FB132"/>
+      <c r="FC132"/>
+      <c r="FD132"/>
+      <c r="FE132"/>
+      <c r="FF132"/>
+      <c r="FG132"/>
+      <c r="FH132"/>
+      <c r="FI132"/>
+      <c r="FJ132"/>
+      <c r="FK132"/>
+      <c r="FL132"/>
+      <c r="FM132"/>
+      <c r="FN132"/>
+      <c r="FO132"/>
+      <c r="FP132"/>
+      <c r="FQ132"/>
+      <c r="FR132"/>
+      <c r="FS132"/>
+      <c r="FT132"/>
+      <c r="FU132"/>
+      <c r="FV132"/>
+      <c r="FW132"/>
+      <c r="FX132"/>
+      <c r="FY132"/>
+      <c r="FZ132"/>
+      <c r="GA132"/>
+      <c r="GB132"/>
+      <c r="GC132"/>
+      <c r="GD132"/>
+      <c r="GE132"/>
+      <c r="GF132"/>
+      <c r="GG132"/>
+      <c r="GH132"/>
+      <c r="GI132"/>
+      <c r="GJ132"/>
+      <c r="GK132"/>
+      <c r="GL132"/>
+      <c r="GM132"/>
+      <c r="GN132"/>
+      <c r="GO132"/>
+      <c r="GP132"/>
+      <c r="GQ132"/>
+      <c r="GR132"/>
+      <c r="GS132"/>
+      <c r="GT132"/>
+      <c r="GU132"/>
+      <c r="GV132"/>
+      <c r="GW132"/>
+      <c r="GX132"/>
+      <c r="GY132"/>
+      <c r="GZ132"/>
+      <c r="HA132"/>
+      <c r="HB132"/>
+      <c r="HC132"/>
+      <c r="HD132"/>
+      <c r="HE132"/>
+      <c r="HF132"/>
+      <c r="HG132"/>
+      <c r="HH132"/>
+      <c r="HI132"/>
+      <c r="HJ132"/>
+      <c r="HK132"/>
+      <c r="HL132"/>
+      <c r="HM132"/>
+      <c r="HN132"/>
+      <c r="HO132"/>
+      <c r="HP132"/>
+      <c r="HQ132"/>
+      <c r="HR132"/>
+      <c r="HS132"/>
+      <c r="HT132"/>
+      <c r="HU132"/>
+      <c r="HV132"/>
+      <c r="HW132"/>
+      <c r="HX132"/>
+      <c r="HY132"/>
+      <c r="HZ132"/>
+      <c r="IA132"/>
+      <c r="IB132"/>
+      <c r="IC132"/>
+      <c r="ID132"/>
+      <c r="IE132"/>
+      <c r="IF132"/>
+      <c r="IG132"/>
+      <c r="IH132"/>
+      <c r="II132"/>
+      <c r="IJ132"/>
+      <c r="IK132"/>
+      <c r="IL132"/>
+      <c r="IM132"/>
+      <c r="IN132"/>
+      <c r="IO132"/>
+      <c r="IP132"/>
+      <c r="IQ132"/>
+      <c r="IR132"/>
+      <c r="IS132"/>
+      <c r="IT132"/>
+      <c r="IU132"/>
     </row>
     <row r="133" spans="1:255" ht="28.35" customHeight="1">
       <c r="A133" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B133" s="11"/>
       <c r="C133" s="11"/>
       <c r="D133" s="11"/>
       <c r="E133" s="11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F133" s="24">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="G133" s="25">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H133" s="14">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>125</v>
       </c>
     </row>
     <row r="134" spans="1:255" ht="28.35" customHeight="1">
       <c r="A134" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B134" s="11"/>
       <c r="C134" s="11"/>
@@ -5632,40 +5648,40 @@
         <v>21</v>
       </c>
       <c r="F134" s="24">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G134" s="25">
-        <v>1.36</v>
+        <v>12</v>
       </c>
       <c r="H134" s="14">
         <f t="shared" si="2"/>
-        <v>10.88</v>
+        <v>12</v>
       </c>
     </row>
     <row r="135" spans="1:255" ht="28.35" customHeight="1">
       <c r="A135" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="B135" s="29"/>
+        <v>136</v>
+      </c>
+      <c r="B135" s="11"/>
       <c r="C135" s="11"/>
       <c r="D135" s="11"/>
       <c r="E135" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F135" s="24">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="G135" s="25">
-        <v>2.2000000000000002</v>
+        <v>1.36</v>
       </c>
       <c r="H135" s="14">
         <f t="shared" si="2"/>
-        <v>55.000000000000007</v>
+        <v>10.88</v>
       </c>
     </row>
     <row r="136" spans="1:255" ht="28.35" customHeight="1">
       <c r="A136" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B136" s="29"/>
       <c r="C136" s="11"/>
@@ -5674,19 +5690,19 @@
         <v>21</v>
       </c>
       <c r="F136" s="24">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G136" s="25">
-        <v>5.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H136" s="14">
         <f t="shared" si="2"/>
-        <v>203.5</v>
+        <v>55.000000000000007</v>
       </c>
     </row>
     <row r="137" spans="1:255" ht="28.35" customHeight="1">
       <c r="A137" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B137" s="29"/>
       <c r="C137" s="11"/>
@@ -5695,61 +5711,61 @@
         <v>21</v>
       </c>
       <c r="F137" s="24">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="G137" s="25">
-        <v>0.4</v>
+        <v>5.5</v>
       </c>
       <c r="H137" s="14">
         <f t="shared" si="2"/>
-        <v>8.8000000000000007</v>
+        <v>203.5</v>
       </c>
     </row>
     <row r="138" spans="1:255" ht="28.35" customHeight="1">
       <c r="A138" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="B138" s="11"/>
+        <v>139</v>
+      </c>
+      <c r="B138" s="29"/>
       <c r="C138" s="11"/>
       <c r="D138" s="11"/>
       <c r="E138" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F138" s="24">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="G138" s="25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H138" s="14">
         <f t="shared" si="2"/>
-        <v>3.5</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="139" spans="1:255" ht="28.35" customHeight="1">
       <c r="A139" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="B139" s="29"/>
+        <v>140</v>
+      </c>
+      <c r="B139" s="11"/>
       <c r="C139" s="11"/>
       <c r="D139" s="11"/>
       <c r="E139" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F139" s="24">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="G139" s="25">
-        <v>1.1000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="H139" s="14">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="140" spans="1:255" ht="28.35" customHeight="1">
       <c r="A140" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B140" s="29"/>
       <c r="C140" s="11"/>
@@ -5758,19 +5774,19 @@
         <v>21</v>
       </c>
       <c r="F140" s="24">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="G140" s="25">
-        <v>0.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H140" s="14">
         <f t="shared" si="2"/>
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="141" spans="1:255" ht="28.35" customHeight="1">
       <c r="A141" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B141" s="29"/>
       <c r="C141" s="11"/>
@@ -5779,19 +5795,19 @@
         <v>21</v>
       </c>
       <c r="F141" s="24">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="G141" s="25">
-        <v>2.85</v>
+        <v>0.9</v>
       </c>
       <c r="H141" s="14">
         <f t="shared" si="2"/>
-        <v>85.5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="142" spans="1:255" ht="28.35" customHeight="1">
       <c r="A142" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B142" s="29"/>
       <c r="C142" s="11"/>
@@ -5800,86 +5816,84 @@
         <v>21</v>
       </c>
       <c r="F142" s="24">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="G142" s="25">
-        <v>3.4</v>
+        <v>2.85</v>
       </c>
       <c r="H142" s="14">
         <f t="shared" si="2"/>
-        <v>40.799999999999997</v>
+        <v>85.5</v>
       </c>
     </row>
     <row r="143" spans="1:255" ht="28.35" customHeight="1">
       <c r="A143" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="B143" s="11"/>
+        <v>144</v>
+      </c>
+      <c r="B143" s="29"/>
       <c r="C143" s="11"/>
       <c r="D143" s="11"/>
       <c r="E143" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F143" s="24">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G143" s="25">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="H143" s="14">
         <f t="shared" si="2"/>
-        <v>78</v>
+        <v>40.799999999999997</v>
       </c>
     </row>
     <row r="144" spans="1:255" ht="28.35" customHeight="1">
       <c r="A144" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="B144" s="29"/>
+        <v>145</v>
+      </c>
+      <c r="B144" s="11"/>
       <c r="C144" s="11"/>
-      <c r="D144" s="11" t="s">
-        <v>147</v>
-      </c>
+      <c r="D144" s="11"/>
       <c r="E144" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F144" s="24">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G144" s="25">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="H144" s="14">
         <f t="shared" si="2"/>
-        <v>357</v>
+        <v>78</v>
       </c>
     </row>
     <row r="145" spans="1:8" ht="28.35" customHeight="1">
       <c r="A145" s="23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B145" s="29"/>
       <c r="C145" s="11"/>
       <c r="D145" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E145" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F145" s="24">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="G145" s="25">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H145" s="14">
         <f t="shared" si="2"/>
-        <v>1000</v>
+        <v>357</v>
       </c>
     </row>
     <row r="146" spans="1:8" ht="28.35" customHeight="1">
       <c r="A146" s="23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B146" s="29"/>
       <c r="C146" s="11"/>
@@ -5890,30 +5904,53 @@
         <v>21</v>
       </c>
       <c r="F146" s="24">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="G146" s="25">
         <v>10</v>
       </c>
       <c r="H146" s="14">
         <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="28.35" customHeight="1">
+      <c r="A147" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="B147" s="29"/>
+      <c r="C147" s="11"/>
+      <c r="D147" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="E147" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F147" s="24">
+        <v>9</v>
+      </c>
+      <c r="G147" s="25">
+        <v>10</v>
+      </c>
+      <c r="H147" s="14">
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="48.75" customHeight="1">
-      <c r="H147" s="47">
-        <f>SUM(H3:H146)</f>
-        <v>19093.221999999998</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" ht="29.1" customHeight="1"/>
-    <row r="149" spans="1:8" ht="30" customHeight="1"/>
+    <row r="148" spans="1:8" ht="48.75" customHeight="1">
+      <c r="H148" s="47">
+        <f>SUM(H3:H147)</f>
+        <v>19206.601999999999</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" ht="29.1" customHeight="1"/>
+    <row r="150" spans="1:8" ht="30" customHeight="1"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="F110:F112 F21:F25 F80 F18:F19">
+  <conditionalFormatting sqref="F111:F113 F21:F25 F80 F18:F19">
     <cfRule type="cellIs" dxfId="21" priority="2" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>2</formula>
     </cfRule>
@@ -5948,7 +5985,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F45 F81:F82 F100 F86:F87">
+  <conditionalFormatting sqref="F45 F81:F82 F101 F86:F87">
     <cfRule type="cellIs" dxfId="14" priority="12" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>1</formula>
     </cfRule>
@@ -5978,32 +6015,32 @@
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F96 F92:F93">
+  <conditionalFormatting sqref="F97 F92:F93">
     <cfRule type="cellIs" dxfId="8" priority="24" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F113 F101">
+  <conditionalFormatting sqref="F114 F102">
     <cfRule type="cellIs" dxfId="7" priority="25" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>150</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F103:F106">
+  <conditionalFormatting sqref="F104:F107">
     <cfRule type="cellIs" dxfId="6" priority="28" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F99">
+  <conditionalFormatting sqref="F100">
     <cfRule type="cellIs" dxfId="5" priority="31" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F95">
+  <conditionalFormatting sqref="F96">
     <cfRule type="cellIs" dxfId="4" priority="33" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F94">
+  <conditionalFormatting sqref="F94:F95">
     <cfRule type="cellIs" dxfId="3" priority="34" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>10</formula>
     </cfRule>

</xml_diff>

<commit_message>
new new 28 aprile
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IU150"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="A113" sqref="A113"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -2665,14 +2665,14 @@
         <v>10</v>
       </c>
       <c r="F17" s="17">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G17" s="13">
         <v>2</v>
       </c>
       <c r="H17" s="14">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
@@ -5940,7 +5940,7 @@
     <row r="148" spans="1:8" ht="48.75" customHeight="1">
       <c r="H148" s="47">
         <f>SUM(H3:H147)</f>
-        <v>19206.601999999999</v>
+        <v>19202.601999999999</v>
       </c>
     </row>
     <row r="149" spans="1:8" ht="29.1" customHeight="1"/>

</xml_diff>

<commit_message>
new new 2 maggio
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -10,15 +10,15 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$147</definedName>
-    <definedName name="Excel_BuiltIn_Print_Area" localSheetId="0">Sheet1!$A$1:$H$131</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$146</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area" localSheetId="0">Sheet1!$A$1:$H$130</definedName>
   </definedNames>
   <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="229">
   <si>
     <t>PRODOTTO</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>Buste Plastica forate f.to 22x30</t>
-  </si>
-  <si>
-    <t>Buste porta cd TRASPARENTI</t>
   </si>
   <si>
     <t>Calicot   panna (cencio della nonna)</t>
@@ -1861,10 +1858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IU150"/>
+  <dimension ref="A1:IU149"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="J117" sqref="J117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -1881,7 +1878,7 @@
   <sheetData>
     <row r="1" spans="1:35" s="5" customFormat="1" ht="60.75" customHeight="1">
       <c r="A1" s="48" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -2046,7 +2043,7 @@
     </row>
     <row r="5" spans="1:35" ht="24.95" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -2094,7 +2091,7 @@
     </row>
     <row r="6" spans="1:35" ht="24.2" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
@@ -2142,7 +2139,7 @@
     </row>
     <row r="7" spans="1:35" ht="25.35" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="16"/>
@@ -2192,7 +2189,7 @@
     </row>
     <row r="8" spans="1:35" ht="23.25" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B8" s="10">
         <v>43174</v>
@@ -2246,7 +2243,7 @@
     </row>
     <row r="9" spans="1:35" ht="23.25" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="16"/>
@@ -2296,7 +2293,7 @@
     </row>
     <row r="10" spans="1:35" ht="28.35" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B10" s="10">
         <v>43174</v>
@@ -2350,15 +2347,15 @@
     </row>
     <row r="11" spans="1:35" ht="28.35" customHeight="1">
       <c r="A11" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F11" s="17">
         <v>72</v>
@@ -2400,15 +2397,15 @@
     </row>
     <row r="12" spans="1:35" ht="28.35" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F12" s="17">
         <v>10</v>
@@ -2604,12 +2601,12 @@
     </row>
     <row r="16" spans="1:35" ht="28.35" customHeight="1">
       <c r="A16" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>16</v>
@@ -2707,13 +2704,13 @@
         <v>22</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>21</v>
@@ -2725,7 +2722,7 @@
         <v>3</v>
       </c>
       <c r="H18" s="14">
-        <f t="shared" ref="H18:H67" si="1">F18*G18</f>
+        <f t="shared" ref="H18:H66" si="1">F18*G18</f>
         <v>6</v>
       </c>
     </row>
@@ -2734,14 +2731,14 @@
         <v>23</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F19" s="20">
         <v>250</v>
@@ -2756,7 +2753,7 @@
     </row>
     <row r="20" spans="1:35" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A20" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -2774,237 +2771,237 @@
       </c>
     </row>
     <row r="21" spans="1:35" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21" s="20">
-        <v>100</v>
-      </c>
-      <c r="G21" s="21">
-        <v>0</v>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="24">
+        <v>25</v>
+      </c>
+      <c r="G21" s="25">
+        <v>1.1399999999999999</v>
       </c>
       <c r="H21" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>28.499999999999996</v>
       </c>
     </row>
     <row r="22" spans="1:35" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="24">
-        <v>25</v>
-      </c>
-      <c r="G22" s="25">
-        <v>1.1399999999999999</v>
+      <c r="B22" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="20">
+        <v>4</v>
+      </c>
+      <c r="G22" s="21">
+        <v>8.5</v>
       </c>
       <c r="H22" s="14">
         <f t="shared" si="1"/>
-        <v>28.499999999999996</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:35" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A23" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>27</v>
-      </c>
       <c r="F23" s="20">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G23" s="21">
-        <v>8.5</v>
+        <v>25.13</v>
       </c>
       <c r="H23" s="14">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>251.29999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:35" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A24" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="D24" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="19" t="s">
-        <v>225</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>226</v>
-      </c>
-      <c r="D24" s="19"/>
       <c r="E24" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F24" s="20">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G24" s="21">
-        <v>25.13</v>
+        <v>17</v>
       </c>
       <c r="H24" s="14">
         <f t="shared" si="1"/>
-        <v>251.29999999999998</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:35" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A25" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
       <c r="E25" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F25" s="20">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G25" s="21">
-        <v>17</v>
+        <v>7.9</v>
       </c>
       <c r="H25" s="14">
         <f t="shared" si="1"/>
-        <v>102</v>
+        <v>23.700000000000003</v>
       </c>
     </row>
     <row r="26" spans="1:35" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A26" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
+      <c r="B26" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E26" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F26" s="20">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="G26" s="21">
-        <v>7.9</v>
+        <v>2.76</v>
       </c>
       <c r="H26" s="14">
         <f t="shared" si="1"/>
-        <v>23.700000000000003</v>
+        <v>41.4</v>
       </c>
     </row>
     <row r="27" spans="1:35" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="20">
-        <v>15</v>
+      <c r="B27" s="27"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="12">
+        <v>0</v>
       </c>
       <c r="G27" s="21">
-        <v>2.76</v>
+        <v>9.75</v>
       </c>
       <c r="H27" s="14">
         <f t="shared" si="1"/>
-        <v>41.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:35" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="12">
-        <v>0</v>
+      <c r="B28" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="20">
+        <v>25</v>
       </c>
       <c r="G28" s="21">
-        <v>9.75</v>
+        <v>2.6</v>
       </c>
       <c r="H28" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:35" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A29" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>175</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
       <c r="E29" s="19" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="F29" s="20">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G29" s="21">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
       <c r="H29" s="14">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:35" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="20">
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="12">
         <v>0</v>
       </c>
-      <c r="G30" s="21">
-        <v>2.7</v>
+      <c r="G30" s="11">
+        <v>3.68</v>
       </c>
       <c r="H30" s="14">
         <f t="shared" si="1"/>
@@ -3012,20 +3009,22 @@
       </c>
     </row>
     <row r="31" spans="1:35" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E31" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F31" s="12">
+      <c r="F31" s="20">
         <v>0</v>
       </c>
-      <c r="G31" s="11">
-        <v>3.68</v>
+      <c r="G31" s="21">
+        <v>0.1</v>
       </c>
       <c r="H31" s="14">
         <f t="shared" si="1"/>
@@ -3038,21 +3037,19 @@
       </c>
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
-      <c r="D32" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="D32" s="19"/>
       <c r="E32" s="28" t="s">
         <v>21</v>
       </c>
       <c r="F32" s="20">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G32" s="21">
-        <v>0.1</v>
+        <v>3</v>
       </c>
       <c r="H32" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3066,14 +3063,14 @@
         <v>21</v>
       </c>
       <c r="F33" s="20">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G33" s="21">
-        <v>3</v>
+        <v>0.25</v>
       </c>
       <c r="H33" s="14">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3087,14 +3084,14 @@
         <v>21</v>
       </c>
       <c r="F34" s="20">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G34" s="21">
-        <v>0.25</v>
+        <v>85</v>
       </c>
       <c r="H34" s="14">
         <f t="shared" si="1"/>
-        <v>12.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3111,7 +3108,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="21">
-        <v>85</v>
+        <v>177</v>
       </c>
       <c r="H35" s="14">
         <f t="shared" si="1"/>
@@ -3132,7 +3129,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="21">
-        <v>177</v>
+        <v>110</v>
       </c>
       <c r="H36" s="14">
         <f t="shared" si="1"/>
@@ -3150,14 +3147,14 @@
         <v>21</v>
       </c>
       <c r="F37" s="20">
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="G37" s="21">
-        <v>110</v>
+        <v>1.18</v>
       </c>
       <c r="H37" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>200.6</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3171,104 +3168,104 @@
         <v>21</v>
       </c>
       <c r="F38" s="20">
-        <v>100</v>
+        <v>575</v>
       </c>
       <c r="G38" s="21">
-        <v>1.18</v>
+        <v>0.35</v>
       </c>
       <c r="H38" s="14">
         <f t="shared" si="1"/>
-        <v>118</v>
+        <v>201.25</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A39" s="18" t="s">
-        <v>45</v>
+        <v>154</v>
       </c>
       <c r="B39" s="19"/>
       <c r="C39" s="19"/>
       <c r="D39" s="19"/>
       <c r="E39" s="28" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F39" s="20">
-        <v>575</v>
-      </c>
-      <c r="G39" s="21">
-        <v>0.35</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="G39" s="21"/>
       <c r="H39" s="14">
         <f t="shared" si="1"/>
-        <v>201.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A40" s="18" t="s">
-        <v>155</v>
+        <v>45</v>
       </c>
       <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
+      <c r="C40" s="19" t="s">
+        <v>201</v>
+      </c>
       <c r="D40" s="19"/>
       <c r="E40" s="28" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F40" s="20">
-        <v>60</v>
-      </c>
-      <c r="G40" s="21"/>
+        <v>3</v>
+      </c>
+      <c r="G40" s="21">
+        <v>1</v>
+      </c>
       <c r="H40" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A41" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="19"/>
+      <c r="B41" s="19" t="s">
+        <v>204</v>
+      </c>
       <c r="C41" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="D41" s="19"/>
+        <v>203</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E41" s="28" t="s">
         <v>21</v>
       </c>
       <c r="F41" s="20">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G41" s="21">
-        <v>1</v>
+        <v>1.75</v>
       </c>
       <c r="H41" s="14">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A42" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="C42" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
       <c r="E42" s="28" t="s">
         <v>21</v>
       </c>
       <c r="F42" s="20">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="G42" s="21">
-        <v>1.75</v>
+        <v>0.72</v>
       </c>
       <c r="H42" s="14">
         <f t="shared" si="1"/>
-        <v>24.5</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3277,42 +3274,42 @@
       </c>
       <c r="B43" s="19"/>
       <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
+      <c r="D43" s="19" t="s">
+        <v>49</v>
+      </c>
       <c r="E43" s="28" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F43" s="20">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="G43" s="21">
-        <v>0.72</v>
+        <v>3</v>
       </c>
       <c r="H43" s="14">
         <f t="shared" si="1"/>
-        <v>0.72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A44" s="18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B44" s="19"/>
       <c r="C44" s="19"/>
-      <c r="D44" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E44" s="28" t="s">
+      <c r="D44" s="19"/>
+      <c r="E44" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F44" s="20">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G44" s="21">
-        <v>3</v>
+        <v>1.8</v>
       </c>
       <c r="H44" s="14">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3326,14 +3323,14 @@
         <v>12</v>
       </c>
       <c r="F45" s="20">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G45" s="21">
-        <v>1.8</v>
+        <v>1</v>
       </c>
       <c r="H45" s="14">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3342,37 +3339,39 @@
       </c>
       <c r="B46" s="19"/>
       <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19" t="s">
-        <v>12</v>
+      <c r="D46" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="F46" s="20">
-        <v>14</v>
+        <v>600</v>
       </c>
       <c r="G46" s="21">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="H46" s="14">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A47" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B47" s="19"/>
+      <c r="A47" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" s="11"/>
       <c r="C47" s="19"/>
-      <c r="D47" s="19" t="s">
-        <v>54</v>
-      </c>
+      <c r="D47" s="19"/>
       <c r="E47" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F47" s="20">
-        <v>1000</v>
-      </c>
-      <c r="G47" s="21"/>
+        <v>0</v>
+      </c>
+      <c r="G47" s="21">
+        <v>0.22</v>
+      </c>
       <c r="H47" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3383,8 +3382,8 @@
         <v>55</v>
       </c>
       <c r="B48" s="11"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
       <c r="E48" s="11" t="s">
         <v>21</v>
       </c>
@@ -3392,7 +3391,7 @@
         <v>0</v>
       </c>
       <c r="G48" s="21">
-        <v>0.22</v>
+        <v>2.13</v>
       </c>
       <c r="H48" s="14">
         <f t="shared" si="1"/>
@@ -3400,47 +3399,53 @@
       </c>
     </row>
     <row r="49" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E49" s="11" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="F49" s="20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G49" s="21">
-        <v>2.13</v>
+        <v>5.95</v>
       </c>
       <c r="H49" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A50" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
+      <c r="B50" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>170</v>
+      </c>
       <c r="D50" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F50" s="20">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G50" s="21">
-        <v>5.95</v>
+        <v>0.7</v>
       </c>
       <c r="H50" s="14">
         <f t="shared" si="1"/>
-        <v>11.9</v>
+        <v>4.1999999999999993</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3448,53 +3453,47 @@
         <v>58</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F51" s="20">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="G51" s="21">
-        <v>0.7</v>
+        <v>1.5</v>
       </c>
       <c r="H51" s="14">
         <f t="shared" si="1"/>
-        <v>4.1999999999999993</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A52" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="B52" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="C52" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
       <c r="E52" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F52" s="20">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G52" s="21">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="H52" s="14">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3508,14 +3507,14 @@
         <v>21</v>
       </c>
       <c r="F53" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53" s="21">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="H53" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3529,14 +3528,14 @@
         <v>21</v>
       </c>
       <c r="F54" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54" s="21">
-        <v>1.5</v>
+        <v>5.35</v>
       </c>
       <c r="H54" s="14">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3550,125 +3549,125 @@
         <v>21</v>
       </c>
       <c r="F55" s="20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G55" s="21">
-        <v>5.35</v>
+        <v>2</v>
       </c>
       <c r="H55" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A56" s="18" t="s">
-        <v>63</v>
+        <v>159</v>
       </c>
       <c r="B56" s="19"/>
       <c r="C56" s="19"/>
-      <c r="D56" s="19"/>
+      <c r="D56" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="E56" s="11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F56" s="20">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="G56" s="21">
-        <v>2</v>
+        <v>1.98</v>
       </c>
       <c r="H56" s="14">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>43.56</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A57" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="B57" s="19"/>
-      <c r="C57" s="19"/>
-      <c r="D57" s="19" t="s">
-        <v>9</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="C57" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="D57" s="19"/>
       <c r="E57" s="11" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F57" s="20">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="G57" s="21">
-        <v>1.98</v>
+        <v>0.44</v>
       </c>
       <c r="H57" s="14">
         <f t="shared" si="1"/>
-        <v>43.56</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="58" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A58" s="18" t="s">
+      <c r="A58" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="B58" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="C58" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="D58" s="19"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
       <c r="E58" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F58" s="20">
-        <v>7</v>
-      </c>
-      <c r="G58" s="21">
-        <v>0.44</v>
+        <v>12</v>
+      </c>
+      <c r="F58" s="24">
+        <v>12</v>
+      </c>
+      <c r="G58" s="25">
+        <v>4.8499999999999996</v>
       </c>
       <c r="H58" s="14">
         <f t="shared" si="1"/>
-        <v>3.08</v>
+        <v>58.199999999999996</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A59" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="B59" s="11"/>
+      <c r="B59" s="29"/>
       <c r="C59" s="11"/>
       <c r="D59" s="11"/>
       <c r="E59" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F59" s="24">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="G59" s="25">
-        <v>4.8499999999999996</v>
+        <v>5.04</v>
       </c>
       <c r="H59" s="14">
         <f t="shared" si="1"/>
-        <v>58.199999999999996</v>
+        <v>151.19999999999999</v>
       </c>
     </row>
     <row r="60" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A60" s="23" t="s">
+      <c r="A60" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B60" s="29"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19"/>
       <c r="E60" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F60" s="24">
-        <v>30</v>
-      </c>
-      <c r="G60" s="25">
-        <v>5.04</v>
+      <c r="F60" s="20">
+        <v>25</v>
+      </c>
+      <c r="G60" s="21">
+        <v>8.3000000000000007</v>
       </c>
       <c r="H60" s="14">
         <f t="shared" si="1"/>
-        <v>151.19999999999999</v>
+        <v>207.50000000000003</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3678,66 +3677,66 @@
       <c r="B61" s="19"/>
       <c r="C61" s="19"/>
       <c r="D61" s="19"/>
-      <c r="E61" s="11" t="s">
+      <c r="E61" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F61" s="20">
         <v>12</v>
       </c>
-      <c r="F61" s="20">
-        <v>25</v>
-      </c>
       <c r="G61" s="21">
-        <v>8.3000000000000007</v>
+        <v>0.75</v>
       </c>
       <c r="H61" s="14">
         <f t="shared" si="1"/>
-        <v>207.50000000000003</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A62" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="B62" s="19"/>
-      <c r="C62" s="19"/>
-      <c r="D62" s="19"/>
+      <c r="B62" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C62" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>157</v>
+      </c>
       <c r="E62" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F62" s="20">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="G62" s="21">
-        <v>0.75</v>
+        <v>3</v>
       </c>
       <c r="H62" s="14">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>174</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A63" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B63" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="C63" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="D63" s="19" t="s">
-        <v>158</v>
-      </c>
+      <c r="B63" s="19"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
       <c r="E63" s="19" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F63" s="20">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="G63" s="21">
         <v>3</v>
       </c>
       <c r="H63" s="14">
         <f t="shared" si="1"/>
-        <v>174</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3746,42 +3745,42 @@
       </c>
       <c r="B64" s="19"/>
       <c r="C64" s="19"/>
-      <c r="D64" s="19"/>
+      <c r="D64" s="19" t="s">
+        <v>150</v>
+      </c>
       <c r="E64" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F64" s="20">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="G64" s="21">
         <v>3</v>
       </c>
       <c r="H64" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A65" s="18" t="s">
+      <c r="A65" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="B65" s="19"/>
-      <c r="C65" s="19"/>
-      <c r="D65" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="E65" s="19" t="s">
+      <c r="B65" s="31"/>
+      <c r="C65" s="31"/>
+      <c r="D65" s="31"/>
+      <c r="E65" s="31" t="s">
         <v>12</v>
       </c>
       <c r="F65" s="20">
-        <v>35</v>
-      </c>
-      <c r="G65" s="21">
+        <v>18</v>
+      </c>
+      <c r="G65" s="32">
         <v>3</v>
       </c>
-      <c r="H65" s="14">
+      <c r="H65" s="33">
         <f t="shared" si="1"/>
-        <v>105</v>
+        <v>54</v>
       </c>
     </row>
     <row r="66" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3795,35 +3794,35 @@
         <v>12</v>
       </c>
       <c r="F66" s="20">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G66" s="32">
         <v>3</v>
       </c>
       <c r="H66" s="33">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>21</v>
       </c>
     </row>
     <row r="67" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A67" s="30" t="s">
+      <c r="A67" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="B67" s="31"/>
-      <c r="C67" s="31"/>
-      <c r="D67" s="31"/>
-      <c r="E67" s="31" t="s">
+      <c r="B67" s="19"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F67" s="20">
-        <v>7</v>
-      </c>
-      <c r="G67" s="32">
-        <v>3</v>
-      </c>
-      <c r="H67" s="33">
-        <f t="shared" si="1"/>
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="G67" s="21">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="H67" s="14">
+        <f t="shared" ref="H67:H146" si="2">F67*G67</f>
+        <v>210.70000000000002</v>
       </c>
     </row>
     <row r="68" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3834,17 +3833,17 @@
       <c r="C68" s="19"/>
       <c r="D68" s="19"/>
       <c r="E68" s="19" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F68" s="20">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="G68" s="21">
-        <v>4.9000000000000004</v>
+        <v>33.5</v>
       </c>
       <c r="H68" s="14">
-        <f t="shared" ref="H68:H147" si="2">F68*G68</f>
-        <v>210.70000000000002</v>
+        <f t="shared" si="2"/>
+        <v>2043.5</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3858,14 +3857,14 @@
         <v>21</v>
       </c>
       <c r="F69" s="20">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="G69" s="21">
-        <v>33.5</v>
+        <v>2</v>
       </c>
       <c r="H69" s="14">
         <f t="shared" si="2"/>
-        <v>2043.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3879,14 +3878,14 @@
         <v>21</v>
       </c>
       <c r="F70" s="20">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="G70" s="21">
-        <v>2</v>
+        <v>4.3</v>
       </c>
       <c r="H70" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>81.7</v>
       </c>
     </row>
     <row r="71" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3895,19 +3894,21 @@
       </c>
       <c r="B71" s="19"/>
       <c r="C71" s="19"/>
-      <c r="D71" s="19"/>
+      <c r="D71" s="19" t="s">
+        <v>49</v>
+      </c>
       <c r="E71" s="19" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F71" s="20">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="G71" s="21">
-        <v>4.3</v>
+        <v>8.5</v>
       </c>
       <c r="H71" s="14">
         <f t="shared" si="2"/>
-        <v>81.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3917,20 +3918,20 @@
       <c r="B72" s="19"/>
       <c r="C72" s="19"/>
       <c r="D72" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E72" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F72" s="20">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G72" s="21">
         <v>8.5</v>
       </c>
       <c r="H72" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>102</v>
       </c>
     </row>
     <row r="73" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3940,20 +3941,20 @@
       <c r="B73" s="19"/>
       <c r="C73" s="19"/>
       <c r="D73" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E73" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F73" s="20">
-        <v>12</v>
+        <v>1.5</v>
       </c>
       <c r="G73" s="21">
-        <v>8.5</v>
+        <v>5</v>
       </c>
       <c r="H73" s="14">
         <f t="shared" si="2"/>
-        <v>102</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="74" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3962,21 +3963,19 @@
       </c>
       <c r="B74" s="19"/>
       <c r="C74" s="19"/>
-      <c r="D74" s="19" t="s">
-        <v>50</v>
-      </c>
+      <c r="D74" s="19"/>
       <c r="E74" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F74" s="20">
-        <v>1.5</v>
+        <v>20</v>
       </c>
       <c r="G74" s="21">
         <v>5</v>
       </c>
       <c r="H74" s="14">
         <f t="shared" si="2"/>
-        <v>7.5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="75" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3990,40 +3989,40 @@
         <v>12</v>
       </c>
       <c r="F75" s="20">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="G75" s="21">
         <v>5</v>
       </c>
       <c r="H75" s="14">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>15</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A76" s="18" t="s">
-        <v>82</v>
+        <v>151</v>
       </c>
       <c r="B76" s="19"/>
       <c r="C76" s="19"/>
-      <c r="D76" s="19"/>
+      <c r="D76" s="19" t="s">
+        <v>13</v>
+      </c>
       <c r="E76" s="19" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
       <c r="F76" s="20">
-        <v>3</v>
-      </c>
-      <c r="G76" s="21">
-        <v>5</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="G76" s="21"/>
       <c r="H76" s="14">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A77" s="18" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B77" s="19"/>
       <c r="C77" s="19"/>
@@ -4031,7 +4030,7 @@
         <v>13</v>
       </c>
       <c r="E77" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F77" s="20">
         <v>150</v>
@@ -4044,71 +4043,71 @@
     </row>
     <row r="78" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A78" s="18" t="s">
-        <v>154</v>
+        <v>82</v>
       </c>
       <c r="B78" s="19"/>
       <c r="C78" s="19"/>
-      <c r="D78" s="19" t="s">
-        <v>13</v>
-      </c>
+      <c r="D78" s="19"/>
       <c r="E78" s="19" t="s">
-        <v>153</v>
+        <v>21</v>
       </c>
       <c r="F78" s="20">
-        <v>150</v>
-      </c>
-      <c r="G78" s="21"/>
+        <v>9</v>
+      </c>
+      <c r="G78" s="21">
+        <v>0.8</v>
+      </c>
       <c r="H78" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A79" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B79" s="19"/>
-      <c r="C79" s="19"/>
-      <c r="D79" s="19"/>
+      <c r="B79" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="C79" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="D79" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E79" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F79" s="20">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G79" s="21">
-        <v>0.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H79" s="14">
         <f t="shared" si="2"/>
-        <v>7.2</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A80" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="B80" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="C80" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="D80" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="B80" s="19"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="19"/>
       <c r="E80" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F80" s="20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G80" s="21">
-        <v>1.1000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="H80" s="14">
         <f t="shared" si="2"/>
-        <v>5.5</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="81" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4122,14 +4121,14 @@
         <v>21</v>
       </c>
       <c r="F81" s="20">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G81" s="21">
-        <v>0.9</v>
+        <v>1.5</v>
       </c>
       <c r="H81" s="14">
         <f t="shared" si="2"/>
-        <v>3.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4143,62 +4142,62 @@
         <v>21</v>
       </c>
       <c r="F82" s="20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G82" s="21">
         <v>1.5</v>
       </c>
       <c r="H82" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="83" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A83" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="B83" s="19"/>
-      <c r="C83" s="19"/>
-      <c r="D83" s="19"/>
+      <c r="B83" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="C83" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="D83" s="19" t="s">
+        <v>189</v>
+      </c>
       <c r="E83" s="19" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F83" s="20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G83" s="21">
-        <v>1.5</v>
+        <v>12.5</v>
       </c>
       <c r="H83" s="14">
         <f t="shared" si="2"/>
-        <v>4.5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="84" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A84" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="B84" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="C84" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="D84" s="19" t="s">
-        <v>190</v>
-      </c>
+      <c r="B84" s="19"/>
+      <c r="C84" s="19"/>
+      <c r="D84" s="19"/>
       <c r="E84" s="19" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F84" s="20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G84" s="21">
-        <v>12.5</v>
+        <v>2.5</v>
       </c>
       <c r="H84" s="14">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4212,14 +4211,14 @@
         <v>21</v>
       </c>
       <c r="F85" s="20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G85" s="21">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="H85" s="14">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4247,21 +4246,25 @@
       <c r="A87" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B87" s="19"/>
-      <c r="C87" s="19"/>
+      <c r="B87" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="C87" s="19" t="s">
+        <v>181</v>
+      </c>
       <c r="D87" s="19"/>
       <c r="E87" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F87" s="20">
-        <v>0</v>
-      </c>
-      <c r="G87" s="21">
-        <v>1</v>
-      </c>
-      <c r="H87" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>50</v>
+      </c>
+      <c r="G87" s="38">
+        <v>0.19</v>
+      </c>
+      <c r="H87" s="44">
+        <f t="shared" si="2"/>
+        <v>9.5</v>
       </c>
     </row>
     <row r="88" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4269,22 +4272,22 @@
         <v>92</v>
       </c>
       <c r="B88" s="19" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C88" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D88" s="19"/>
       <c r="E88" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F88" s="20">
+      <c r="F88" s="37">
         <v>50</v>
       </c>
-      <c r="G88" s="38">
+      <c r="G88" s="40">
         <v>0.19</v>
       </c>
-      <c r="H88" s="44">
+      <c r="H88" s="46">
         <f t="shared" si="2"/>
         <v>9.5</v>
       </c>
@@ -4293,25 +4296,21 @@
       <c r="A89" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="B89" s="19" t="s">
-        <v>212</v>
-      </c>
-      <c r="C89" s="19" t="s">
-        <v>182</v>
-      </c>
+      <c r="B89" s="19"/>
+      <c r="C89" s="19"/>
       <c r="D89" s="19"/>
       <c r="E89" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F89" s="37">
-        <v>50</v>
-      </c>
-      <c r="G89" s="40">
-        <v>0.19</v>
-      </c>
-      <c r="H89" s="46">
-        <f t="shared" si="2"/>
-        <v>9.5</v>
+      <c r="F89" s="20">
+        <v>3</v>
+      </c>
+      <c r="G89" s="39">
+        <v>1.2</v>
+      </c>
+      <c r="H89" s="45">
+        <f t="shared" si="2"/>
+        <v>3.5999999999999996</v>
       </c>
     </row>
     <row r="90" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4325,14 +4324,14 @@
         <v>21</v>
       </c>
       <c r="F90" s="20">
-        <v>3</v>
-      </c>
-      <c r="G90" s="39">
-        <v>1.2</v>
-      </c>
-      <c r="H90" s="45">
-        <f t="shared" si="2"/>
-        <v>3.5999999999999996</v>
+        <v>0</v>
+      </c>
+      <c r="G90" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="H90" s="44">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4346,175 +4345,182 @@
         <v>21</v>
       </c>
       <c r="F91" s="20">
-        <v>0</v>
-      </c>
-      <c r="G91" s="21">
-        <v>0.2</v>
-      </c>
-      <c r="H91" s="44">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G91" s="43">
+        <v>1</v>
+      </c>
+      <c r="H91" s="46">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="I91" s="41"/>
     </row>
     <row r="92" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A92" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="B92" s="19"/>
-      <c r="C92" s="19"/>
-      <c r="D92" s="19"/>
+        <v>191</v>
+      </c>
+      <c r="B92" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C92" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="D92" s="19" t="s">
+        <v>184</v>
+      </c>
       <c r="E92" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F92" s="20">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="G92" s="43">
-        <v>1</v>
+        <v>3.45</v>
       </c>
       <c r="H92" s="46">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="I92" s="41"/>
+        <f>F92*G92</f>
+        <v>358.8</v>
+      </c>
+      <c r="I92" s="42"/>
     </row>
     <row r="93" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A93" s="18" t="s">
-        <v>192</v>
+        <v>96</v>
       </c>
       <c r="B93" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C93" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="D93" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="C93" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="D93" s="19" t="s">
-        <v>185</v>
-      </c>
       <c r="E93" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F93" s="20">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G93" s="43">
-        <v>3.45</v>
+        <v>2.9</v>
       </c>
       <c r="H93" s="46">
-        <f>F93*G93</f>
-        <v>358.8</v>
+        <f t="shared" si="2"/>
+        <v>295.8</v>
       </c>
       <c r="I93" s="42"/>
     </row>
     <row r="94" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A94" s="18" t="s">
-        <v>97</v>
+        <v>226</v>
       </c>
       <c r="B94" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C94" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="D94" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="C94" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="D94" s="19" t="s">
-        <v>185</v>
-      </c>
       <c r="E94" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F94" s="20">
-        <v>102</v>
+        <v>48</v>
       </c>
       <c r="G94" s="43">
-        <v>2.9</v>
+        <v>4.8</v>
       </c>
       <c r="H94" s="46">
         <f t="shared" si="2"/>
-        <v>295.8</v>
+        <v>230.39999999999998</v>
       </c>
       <c r="I94" s="42"/>
     </row>
     <row r="95" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A95" s="18" t="s">
-        <v>227</v>
+        <v>97</v>
       </c>
       <c r="B95" s="19" t="s">
-        <v>229</v>
+        <v>183</v>
       </c>
       <c r="C95" s="19" t="s">
-        <v>228</v>
+        <v>181</v>
       </c>
       <c r="D95" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E95" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F95" s="20">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="G95" s="43">
-        <v>4.8</v>
+        <v>3.45</v>
       </c>
       <c r="H95" s="46">
         <f t="shared" si="2"/>
-        <v>230.39999999999998</v>
+        <v>0</v>
       </c>
       <c r="I95" s="42"/>
     </row>
     <row r="96" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A96" s="18" t="s">
-        <v>98</v>
+        <v>190</v>
       </c>
       <c r="B96" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C96" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="D96" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="C96" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="D96" s="19" t="s">
-        <v>185</v>
-      </c>
       <c r="E96" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F96" s="20">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="G96" s="43">
-        <v>3.45</v>
+        <v>3.75</v>
       </c>
       <c r="H96" s="46">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>183.75</v>
       </c>
       <c r="I96" s="42"/>
     </row>
     <row r="97" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A97" s="18" t="s">
-        <v>191</v>
+        <v>98</v>
       </c>
       <c r="B97" s="19" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="C97" s="19" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="D97" s="19" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="E97" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F97" s="20">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="G97" s="43">
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="H97" s="46">
         <f t="shared" si="2"/>
-        <v>183.75</v>
+        <v>48</v>
       </c>
       <c r="I97" s="42"/>
     </row>
@@ -4523,26 +4529,26 @@
         <v>99</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C98" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D98" s="19" t="s">
-        <v>202</v>
+        <v>28</v>
       </c>
       <c r="E98" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F98" s="20">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="G98" s="43">
-        <v>4</v>
+        <v>0.8</v>
       </c>
       <c r="H98" s="46">
         <f t="shared" si="2"/>
-        <v>48</v>
+        <v>38.400000000000006</v>
       </c>
       <c r="I98" s="42"/>
     </row>
@@ -4551,77 +4557,76 @@
         <v>100</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C99" s="19" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="D99" s="19" t="s">
-        <v>29</v>
+        <v>197</v>
       </c>
       <c r="E99" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F99" s="20">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="G99" s="43">
-        <v>0.8</v>
+        <v>11.7</v>
       </c>
       <c r="H99" s="46">
         <f t="shared" si="2"/>
-        <v>38.400000000000006</v>
-      </c>
-      <c r="I99" s="42"/>
+        <v>117</v>
+      </c>
     </row>
     <row r="100" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A100" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="B100" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="C100" s="19" t="s">
-        <v>199</v>
-      </c>
+      <c r="B100" s="19"/>
+      <c r="C100" s="19"/>
       <c r="D100" s="19" t="s">
-        <v>198</v>
+        <v>15</v>
       </c>
       <c r="E100" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F100" s="20">
-        <v>10</v>
+        <v>170</v>
       </c>
       <c r="G100" s="43">
-        <v>11.7</v>
+        <v>2.4</v>
       </c>
       <c r="H100" s="46">
         <f t="shared" si="2"/>
-        <v>117</v>
+        <v>408</v>
       </c>
     </row>
     <row r="101" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A101" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="B101" s="19"/>
-      <c r="C101" s="19"/>
+      <c r="B101" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="C101" s="19" t="s">
+        <v>196</v>
+      </c>
       <c r="D101" s="19" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E101" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F101" s="20">
-        <v>170</v>
-      </c>
-      <c r="G101" s="43">
-        <v>2.4</v>
-      </c>
-      <c r="H101" s="46">
-        <f t="shared" si="2"/>
-        <v>408</v>
+        <v>30</v>
+      </c>
+      <c r="G101" s="21">
+        <v>0.83</v>
+      </c>
+      <c r="H101" s="45">
+        <f t="shared" si="2"/>
+        <v>24.9</v>
       </c>
     </row>
     <row r="102" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4629,26 +4634,24 @@
         <v>103</v>
       </c>
       <c r="B102" s="19" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="C102" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="D102" s="19" t="s">
-        <v>29</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="D102" s="19"/>
       <c r="E102" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F102" s="20">
-        <v>30</v>
+        <v>139</v>
       </c>
       <c r="G102" s="21">
-        <v>0.83</v>
-      </c>
-      <c r="H102" s="45">
-        <f t="shared" si="2"/>
-        <v>24.9</v>
+        <v>4.7</v>
+      </c>
+      <c r="H102" s="14">
+        <f t="shared" si="2"/>
+        <v>653.30000000000007</v>
       </c>
     </row>
     <row r="103" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4656,51 +4659,47 @@
         <v>104</v>
       </c>
       <c r="B103" s="19" t="s">
-        <v>220</v>
+        <v>179</v>
       </c>
       <c r="C103" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="D103" s="19"/>
+        <v>176</v>
+      </c>
+      <c r="D103" s="19" t="s">
+        <v>157</v>
+      </c>
       <c r="E103" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F103" s="20">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="G103" s="21">
-        <v>4.7</v>
+        <v>2.5</v>
       </c>
       <c r="H103" s="14">
         <f t="shared" si="2"/>
-        <v>653.30000000000007</v>
+        <v>262.5</v>
       </c>
     </row>
     <row r="104" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A104" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="B104" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="C104" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="D104" s="19" t="s">
-        <v>158</v>
-      </c>
+      <c r="B104" s="19"/>
+      <c r="C104" s="19"/>
+      <c r="D104" s="34"/>
       <c r="E104" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F104" s="20">
-        <v>105</v>
+        <v>6</v>
       </c>
       <c r="G104" s="21">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="H104" s="14">
         <f t="shared" si="2"/>
-        <v>262.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="105" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4709,121 +4708,127 @@
       </c>
       <c r="B105" s="19"/>
       <c r="C105" s="19"/>
-      <c r="D105" s="34"/>
+      <c r="D105" s="19"/>
       <c r="E105" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F105" s="20">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="G105" s="21">
         <v>2</v>
       </c>
       <c r="H105" s="14">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="106" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A106" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="B106" s="19"/>
-      <c r="C106" s="19"/>
-      <c r="D106" s="19"/>
+        <v>206</v>
+      </c>
+      <c r="B106" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="C106" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="D106" s="19" t="s">
+        <v>174</v>
+      </c>
       <c r="E106" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F106" s="20">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="G106" s="21">
-        <v>2</v>
+        <v>41.34</v>
       </c>
       <c r="H106" s="14">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>289.38</v>
       </c>
     </row>
     <row r="107" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A107" s="18" t="s">
-        <v>207</v>
+        <v>107</v>
       </c>
       <c r="B107" s="19" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C107" s="19" t="s">
-        <v>171</v>
+        <v>200</v>
       </c>
       <c r="D107" s="19" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="E107" s="19" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="F107" s="20">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="G107" s="21">
-        <v>41.34</v>
+        <v>2.7</v>
       </c>
       <c r="H107" s="14">
         <f t="shared" si="2"/>
-        <v>289.38</v>
+        <v>81</v>
       </c>
     </row>
     <row r="108" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A108" s="18" t="s">
+      <c r="A108" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="B108" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="C108" s="19" t="s">
-        <v>201</v>
-      </c>
-      <c r="D108" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="E108" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="F108" s="20">
-        <v>30</v>
-      </c>
-      <c r="G108" s="21">
-        <v>2.7</v>
+      <c r="B108" s="29">
+        <v>43140</v>
+      </c>
+      <c r="C108" s="11">
+        <v>36</v>
+      </c>
+      <c r="D108" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E108" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F108" s="24">
+        <v>15</v>
+      </c>
+      <c r="G108" s="14">
+        <v>6</v>
       </c>
       <c r="H108" s="14">
         <f t="shared" si="2"/>
-        <v>81</v>
+        <v>90</v>
       </c>
     </row>
     <row r="109" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A109" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="B109" s="29">
-        <v>43140</v>
-      </c>
-      <c r="C109" s="11">
-        <v>12</v>
-      </c>
-      <c r="D109" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="E109" s="11" t="s">
+      <c r="A109" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="F109" s="24">
-        <v>14</v>
-      </c>
-      <c r="G109" s="25">
-        <v>6</v>
+      <c r="B109" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="C109" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="D109" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="E109" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F109" s="20">
+        <v>1116</v>
+      </c>
+      <c r="G109" s="21">
+        <v>0.66</v>
       </c>
       <c r="H109" s="14">
         <f t="shared" si="2"/>
-        <v>84</v>
+        <v>736.56000000000006</v>
       </c>
     </row>
     <row r="110" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4831,26 +4836,26 @@
         <v>111</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="C110" s="19" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="D110" s="19" t="s">
-        <v>188</v>
+        <v>28</v>
       </c>
       <c r="E110" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F110" s="20">
-        <v>1116</v>
+        <v>5</v>
       </c>
       <c r="G110" s="21">
-        <v>0.66</v>
+        <v>2.85</v>
       </c>
       <c r="H110" s="14">
         <f t="shared" si="2"/>
-        <v>736.56000000000006</v>
+        <v>14.25</v>
       </c>
     </row>
     <row r="111" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4858,26 +4863,26 @@
         <v>112</v>
       </c>
       <c r="B111" s="19" t="s">
-        <v>170</v>
+        <v>211</v>
       </c>
       <c r="C111" s="19" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="D111" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E111" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F111" s="20">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G111" s="21">
-        <v>2.85</v>
+        <v>1.72</v>
       </c>
       <c r="H111" s="14">
         <f t="shared" si="2"/>
-        <v>14.25</v>
+        <v>12.04</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4885,26 +4890,24 @@
         <v>113</v>
       </c>
       <c r="B112" s="19" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C112" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="D112" s="19" t="s">
-        <v>29</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="D112" s="19"/>
       <c r="E112" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F112" s="20">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G112" s="21">
-        <v>1.72</v>
+        <v>2.9</v>
       </c>
       <c r="H112" s="14">
         <f t="shared" si="2"/>
-        <v>12.04</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="113" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4912,51 +4915,47 @@
         <v>114</v>
       </c>
       <c r="B113" s="19" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="C113" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="D113" s="19"/>
+        <v>180</v>
+      </c>
+      <c r="D113" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E113" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F113" s="20">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G113" s="21">
-        <v>2.9</v>
+        <v>1.72</v>
       </c>
       <c r="H113" s="14">
         <f t="shared" si="2"/>
-        <v>17.399999999999999</v>
+        <v>5.16</v>
       </c>
     </row>
     <row r="114" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A114" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="B114" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="C114" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="D114" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="B114" s="19"/>
+      <c r="C114" s="19"/>
+      <c r="D114" s="35"/>
       <c r="E114" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F114" s="20">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G114" s="21">
-        <v>1.72</v>
+        <v>5</v>
       </c>
       <c r="H114" s="14">
         <f t="shared" si="2"/>
-        <v>5.16</v>
+        <v>35</v>
       </c>
     </row>
     <row r="115" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4965,40 +4964,46 @@
       </c>
       <c r="B115" s="19"/>
       <c r="C115" s="19"/>
-      <c r="D115" s="35"/>
+      <c r="D115" s="19"/>
       <c r="E115" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F115" s="20">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G115" s="21">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H115" s="14">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="116" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A116" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="B116" s="19"/>
-      <c r="C116" s="19"/>
-      <c r="D116" s="19"/>
+      <c r="B116" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="C116" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="D116" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="E116" s="19" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F116" s="20">
-        <v>9</v>
+        <v>169</v>
       </c>
       <c r="G116" s="21">
-        <v>1</v>
+        <v>2.69</v>
       </c>
       <c r="H116" s="14">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>454.61</v>
       </c>
     </row>
     <row r="117" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -5006,10 +5011,10 @@
         <v>118</v>
       </c>
       <c r="B117" s="19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C117" s="19" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D117" s="19" t="s">
         <v>9</v>
@@ -5018,89 +5023,83 @@
         <v>12</v>
       </c>
       <c r="F117" s="20">
-        <v>169</v>
+        <v>113</v>
       </c>
       <c r="G117" s="21">
-        <v>2.69</v>
+        <v>3.3</v>
       </c>
       <c r="H117" s="14">
         <f t="shared" si="2"/>
-        <v>454.61</v>
+        <v>372.9</v>
       </c>
     </row>
     <row r="118" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A118" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="B118" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="C118" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="D118" s="19" t="s">
-        <v>9</v>
-      </c>
+      <c r="B118" s="19"/>
+      <c r="C118" s="19"/>
+      <c r="D118" s="19"/>
       <c r="E118" s="19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F118" s="20">
-        <v>113</v>
+        <v>5</v>
       </c>
       <c r="G118" s="21">
-        <v>3.3</v>
+        <v>2.87</v>
       </c>
       <c r="H118" s="14">
         <f t="shared" si="2"/>
-        <v>372.9</v>
+        <v>14.350000000000001</v>
       </c>
     </row>
     <row r="119" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A119" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="B119" s="19"/>
-      <c r="C119" s="19"/>
-      <c r="D119" s="19"/>
+      <c r="B119" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C119" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="D119" s="19" t="s">
+        <v>121</v>
+      </c>
       <c r="E119" s="19" t="s">
-        <v>10</v>
+        <v>122</v>
       </c>
       <c r="F119" s="20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G119" s="21">
-        <v>2.87</v>
+        <v>7</v>
       </c>
       <c r="H119" s="14">
         <f t="shared" si="2"/>
-        <v>14.350000000000001</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" s="36" customFormat="1" ht="28.35" customHeight="1">
       <c r="A120" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="B120" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="C120" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="D120" s="19" t="s">
-        <v>122</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="B120" s="19"/>
+      <c r="C120" s="19"/>
+      <c r="D120" s="19"/>
       <c r="E120" s="19" t="s">
-        <v>123</v>
+        <v>21</v>
       </c>
       <c r="F120" s="20">
-        <v>6</v>
+        <v>584</v>
       </c>
       <c r="G120" s="21">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H120" s="14">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>1752</v>
       </c>
     </row>
     <row r="121" spans="1:8" s="36" customFormat="1" ht="28.35" customHeight="1">
@@ -5114,85 +5113,91 @@
         <v>21</v>
       </c>
       <c r="F121" s="20">
-        <v>584</v>
+        <v>1</v>
       </c>
       <c r="G121" s="21">
-        <v>3</v>
+        <v>1.96</v>
       </c>
       <c r="H121" s="14">
         <f t="shared" si="2"/>
-        <v>1752</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" s="36" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A122" s="18" t="s">
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="28.35" customHeight="1">
+      <c r="A122" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="B122" s="19"/>
-      <c r="C122" s="19"/>
-      <c r="D122" s="19"/>
-      <c r="E122" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F122" s="20">
-        <v>1</v>
-      </c>
-      <c r="G122" s="21">
-        <v>1.96</v>
+      <c r="B122" s="11"/>
+      <c r="C122" s="11"/>
+      <c r="D122" s="11"/>
+      <c r="E122" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F122" s="24">
+        <v>7</v>
+      </c>
+      <c r="G122" s="25">
+        <v>1.97</v>
       </c>
       <c r="H122" s="14">
         <f t="shared" si="2"/>
-        <v>1.96</v>
+        <v>13.79</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="28.35" customHeight="1">
-      <c r="A123" s="23" t="s">
+      <c r="A123" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="B123" s="11"/>
-      <c r="C123" s="11"/>
-      <c r="D123" s="11"/>
+      <c r="B123" s="19"/>
+      <c r="C123" s="19"/>
+      <c r="D123" s="19"/>
       <c r="E123" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F123" s="24">
+      <c r="F123" s="20">
+        <v>95</v>
+      </c>
+      <c r="G123" s="21">
         <v>7</v>
       </c>
-      <c r="G123" s="25">
-        <v>1.97</v>
-      </c>
       <c r="H123" s="14">
         <f t="shared" si="2"/>
-        <v>13.79</v>
+        <v>665</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="28.35" customHeight="1">
       <c r="A124" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="B124" s="19"/>
-      <c r="C124" s="19"/>
-      <c r="D124" s="19"/>
+      <c r="B124" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C124" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="D124" s="19" t="s">
+        <v>13</v>
+      </c>
       <c r="E124" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F124" s="20">
-        <v>95</v>
+        <v>250</v>
       </c>
       <c r="G124" s="21">
-        <v>7</v>
+        <v>2.69</v>
       </c>
       <c r="H124" s="14">
         <f t="shared" si="2"/>
-        <v>665</v>
+        <v>672.5</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="28.35" customHeight="1">
       <c r="A125" s="18" t="s">
-        <v>128</v>
+        <v>178</v>
       </c>
       <c r="B125" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C125" s="19" t="s">
         <v>223</v>
@@ -5204,62 +5209,56 @@
         <v>12</v>
       </c>
       <c r="F125" s="20">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="G125" s="21">
-        <v>2.69</v>
+        <v>2.21</v>
       </c>
       <c r="H125" s="14">
         <f t="shared" si="2"/>
-        <v>672.5</v>
+        <v>442</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="28.35" customHeight="1">
-      <c r="A126" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="B126" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="C126" s="19" t="s">
-        <v>224</v>
-      </c>
-      <c r="D126" s="19" t="s">
-        <v>13</v>
-      </c>
+      <c r="A126" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="B126" s="11"/>
+      <c r="C126" s="11"/>
+      <c r="D126" s="11"/>
       <c r="E126" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F126" s="20">
-        <v>200</v>
-      </c>
-      <c r="G126" s="21">
-        <v>2.21</v>
+      <c r="F126" s="24">
+        <v>100</v>
+      </c>
+      <c r="G126" s="25">
+        <v>1.43</v>
       </c>
       <c r="H126" s="14">
         <f t="shared" si="2"/>
-        <v>442</v>
+        <v>143</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="28.35" customHeight="1">
-      <c r="A127" s="23" t="s">
+      <c r="A127" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="B127" s="11"/>
-      <c r="C127" s="11"/>
-      <c r="D127" s="11"/>
+      <c r="B127" s="19"/>
+      <c r="C127" s="19"/>
+      <c r="D127" s="19"/>
       <c r="E127" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F127" s="24">
-        <v>100</v>
-      </c>
-      <c r="G127" s="25">
-        <v>1.43</v>
+      <c r="F127" s="20">
+        <v>4</v>
+      </c>
+      <c r="G127" s="21">
+        <v>8.5</v>
       </c>
       <c r="H127" s="14">
         <f t="shared" si="2"/>
-        <v>143</v>
+        <v>34</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="28.35" customHeight="1">
@@ -5273,348 +5272,348 @@
         <v>12</v>
       </c>
       <c r="F128" s="20">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="G128" s="21">
-        <v>8.5</v>
+        <v>5</v>
       </c>
       <c r="H128" s="14">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>85</v>
       </c>
     </row>
     <row r="129" spans="1:255" ht="28.35" customHeight="1">
       <c r="A129" s="18" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="B129" s="19"/>
       <c r="C129" s="19"/>
-      <c r="D129" s="19"/>
+      <c r="D129" s="19" t="s">
+        <v>156</v>
+      </c>
       <c r="E129" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F129" s="20">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G129" s="21">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="H129" s="14">
         <f t="shared" si="2"/>
-        <v>85</v>
+        <v>564</v>
       </c>
     </row>
     <row r="130" spans="1:255" ht="28.35" customHeight="1">
-      <c r="A130" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="B130" s="19"/>
-      <c r="C130" s="19"/>
-      <c r="D130" s="19" t="s">
-        <v>157</v>
-      </c>
+      <c r="A130" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="B130" s="11"/>
+      <c r="C130" s="11"/>
+      <c r="D130" s="11"/>
       <c r="E130" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F130" s="20">
+      <c r="F130" s="24">
+        <v>22</v>
+      </c>
+      <c r="G130" s="25">
+        <v>2.97</v>
+      </c>
+      <c r="H130" s="14">
+        <f t="shared" si="2"/>
+        <v>65.34</v>
+      </c>
+    </row>
+    <row r="131" spans="1:255" ht="28.35" customHeight="1">
+      <c r="A131" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="B131" s="19"/>
+      <c r="C131" s="19"/>
+      <c r="D131" s="19"/>
+      <c r="E131" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F131" s="20">
+        <v>140</v>
+      </c>
+      <c r="G131" s="21">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="H131" s="14">
+        <f t="shared" si="2"/>
+        <v>158.19999999999999</v>
+      </c>
+      <c r="I131"/>
+      <c r="J131"/>
+      <c r="K131"/>
+      <c r="L131"/>
+      <c r="M131"/>
+      <c r="N131"/>
+      <c r="O131"/>
+      <c r="P131"/>
+      <c r="Q131"/>
+      <c r="R131"/>
+      <c r="S131"/>
+      <c r="T131"/>
+      <c r="U131"/>
+      <c r="V131"/>
+      <c r="W131"/>
+      <c r="X131"/>
+      <c r="Y131"/>
+      <c r="Z131"/>
+      <c r="AA131"/>
+      <c r="AB131"/>
+      <c r="AC131"/>
+      <c r="AD131"/>
+      <c r="AE131"/>
+      <c r="AF131"/>
+      <c r="AG131"/>
+      <c r="AH131"/>
+      <c r="AI131"/>
+      <c r="AJ131"/>
+      <c r="AK131"/>
+      <c r="AL131"/>
+      <c r="AM131"/>
+      <c r="AN131"/>
+      <c r="AO131"/>
+      <c r="AP131"/>
+      <c r="AQ131"/>
+      <c r="AR131"/>
+      <c r="AS131"/>
+      <c r="AT131"/>
+      <c r="AU131"/>
+      <c r="AV131"/>
+      <c r="AW131"/>
+      <c r="AX131"/>
+      <c r="AY131"/>
+      <c r="AZ131"/>
+      <c r="BA131"/>
+      <c r="BB131"/>
+      <c r="BC131"/>
+      <c r="BD131"/>
+      <c r="BE131"/>
+      <c r="BF131"/>
+      <c r="BG131"/>
+      <c r="BH131"/>
+      <c r="BI131"/>
+      <c r="BJ131"/>
+      <c r="BK131"/>
+      <c r="BL131"/>
+      <c r="BM131"/>
+      <c r="BN131"/>
+      <c r="BO131"/>
+      <c r="BP131"/>
+      <c r="BQ131"/>
+      <c r="BR131"/>
+      <c r="BS131"/>
+      <c r="BT131"/>
+      <c r="BU131"/>
+      <c r="BV131"/>
+      <c r="BW131"/>
+      <c r="BX131"/>
+      <c r="BY131"/>
+      <c r="BZ131"/>
+      <c r="CA131"/>
+      <c r="CB131"/>
+      <c r="CC131"/>
+      <c r="CD131"/>
+      <c r="CE131"/>
+      <c r="CF131"/>
+      <c r="CG131"/>
+      <c r="CH131"/>
+      <c r="CI131"/>
+      <c r="CJ131"/>
+      <c r="CK131"/>
+      <c r="CL131"/>
+      <c r="CM131"/>
+      <c r="CN131"/>
+      <c r="CO131"/>
+      <c r="CP131"/>
+      <c r="CQ131"/>
+      <c r="CR131"/>
+      <c r="CS131"/>
+      <c r="CT131"/>
+      <c r="CU131"/>
+      <c r="CV131"/>
+      <c r="CW131"/>
+      <c r="CX131"/>
+      <c r="CY131"/>
+      <c r="CZ131"/>
+      <c r="DA131"/>
+      <c r="DB131"/>
+      <c r="DC131"/>
+      <c r="DD131"/>
+      <c r="DE131"/>
+      <c r="DF131"/>
+      <c r="DG131"/>
+      <c r="DH131"/>
+      <c r="DI131"/>
+      <c r="DJ131"/>
+      <c r="DK131"/>
+      <c r="DL131"/>
+      <c r="DM131"/>
+      <c r="DN131"/>
+      <c r="DO131"/>
+      <c r="DP131"/>
+      <c r="DQ131"/>
+      <c r="DR131"/>
+      <c r="DS131"/>
+      <c r="DT131"/>
+      <c r="DU131"/>
+      <c r="DV131"/>
+      <c r="DW131"/>
+      <c r="DX131"/>
+      <c r="DY131"/>
+      <c r="DZ131"/>
+      <c r="EA131"/>
+      <c r="EB131"/>
+      <c r="EC131"/>
+      <c r="ED131"/>
+      <c r="EE131"/>
+      <c r="EF131"/>
+      <c r="EG131"/>
+      <c r="EH131"/>
+      <c r="EI131"/>
+      <c r="EJ131"/>
+      <c r="EK131"/>
+      <c r="EL131"/>
+      <c r="EM131"/>
+      <c r="EN131"/>
+      <c r="EO131"/>
+      <c r="EP131"/>
+      <c r="EQ131"/>
+      <c r="ER131"/>
+      <c r="ES131"/>
+      <c r="ET131"/>
+      <c r="EU131"/>
+      <c r="EV131"/>
+      <c r="EW131"/>
+      <c r="EX131"/>
+      <c r="EY131"/>
+      <c r="EZ131"/>
+      <c r="FA131"/>
+      <c r="FB131"/>
+      <c r="FC131"/>
+      <c r="FD131"/>
+      <c r="FE131"/>
+      <c r="FF131"/>
+      <c r="FG131"/>
+      <c r="FH131"/>
+      <c r="FI131"/>
+      <c r="FJ131"/>
+      <c r="FK131"/>
+      <c r="FL131"/>
+      <c r="FM131"/>
+      <c r="FN131"/>
+      <c r="FO131"/>
+      <c r="FP131"/>
+      <c r="FQ131"/>
+      <c r="FR131"/>
+      <c r="FS131"/>
+      <c r="FT131"/>
+      <c r="FU131"/>
+      <c r="FV131"/>
+      <c r="FW131"/>
+      <c r="FX131"/>
+      <c r="FY131"/>
+      <c r="FZ131"/>
+      <c r="GA131"/>
+      <c r="GB131"/>
+      <c r="GC131"/>
+      <c r="GD131"/>
+      <c r="GE131"/>
+      <c r="GF131"/>
+      <c r="GG131"/>
+      <c r="GH131"/>
+      <c r="GI131"/>
+      <c r="GJ131"/>
+      <c r="GK131"/>
+      <c r="GL131"/>
+      <c r="GM131"/>
+      <c r="GN131"/>
+      <c r="GO131"/>
+      <c r="GP131"/>
+      <c r="GQ131"/>
+      <c r="GR131"/>
+      <c r="GS131"/>
+      <c r="GT131"/>
+      <c r="GU131"/>
+      <c r="GV131"/>
+      <c r="GW131"/>
+      <c r="GX131"/>
+      <c r="GY131"/>
+      <c r="GZ131"/>
+      <c r="HA131"/>
+      <c r="HB131"/>
+      <c r="HC131"/>
+      <c r="HD131"/>
+      <c r="HE131"/>
+      <c r="HF131"/>
+      <c r="HG131"/>
+      <c r="HH131"/>
+      <c r="HI131"/>
+      <c r="HJ131"/>
+      <c r="HK131"/>
+      <c r="HL131"/>
+      <c r="HM131"/>
+      <c r="HN131"/>
+      <c r="HO131"/>
+      <c r="HP131"/>
+      <c r="HQ131"/>
+      <c r="HR131"/>
+      <c r="HS131"/>
+      <c r="HT131"/>
+      <c r="HU131"/>
+      <c r="HV131"/>
+      <c r="HW131"/>
+      <c r="HX131"/>
+      <c r="HY131"/>
+      <c r="HZ131"/>
+      <c r="IA131"/>
+      <c r="IB131"/>
+      <c r="IC131"/>
+      <c r="ID131"/>
+      <c r="IE131"/>
+      <c r="IF131"/>
+      <c r="IG131"/>
+      <c r="IH131"/>
+      <c r="II131"/>
+      <c r="IJ131"/>
+      <c r="IK131"/>
+      <c r="IL131"/>
+      <c r="IM131"/>
+      <c r="IN131"/>
+      <c r="IO131"/>
+      <c r="IP131"/>
+      <c r="IQ131"/>
+      <c r="IR131"/>
+      <c r="IS131"/>
+      <c r="IT131"/>
+      <c r="IU131"/>
+    </row>
+    <row r="132" spans="1:255" ht="28.35" customHeight="1">
+      <c r="A132" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="B132" s="11"/>
+      <c r="C132" s="11"/>
+      <c r="D132" s="11"/>
+      <c r="E132" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G130" s="21">
-        <v>47</v>
-      </c>
-      <c r="H130" s="14">
-        <f t="shared" si="2"/>
-        <v>564</v>
-      </c>
-    </row>
-    <row r="131" spans="1:255" ht="28.35" customHeight="1">
-      <c r="A131" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="B131" s="11"/>
-      <c r="C131" s="11"/>
-      <c r="D131" s="11"/>
-      <c r="E131" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F131" s="24">
-        <v>22</v>
-      </c>
-      <c r="G131" s="25">
-        <v>2.97</v>
-      </c>
-      <c r="H131" s="14">
-        <f t="shared" si="2"/>
-        <v>65.34</v>
-      </c>
-    </row>
-    <row r="132" spans="1:255" ht="28.35" customHeight="1">
-      <c r="A132" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="B132" s="19"/>
-      <c r="C132" s="19"/>
-      <c r="D132" s="19"/>
-      <c r="E132" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F132" s="20">
-        <v>140</v>
-      </c>
-      <c r="G132" s="21">
-        <v>1.1299999999999999</v>
+      <c r="F132" s="24">
+        <v>25</v>
+      </c>
+      <c r="G132" s="25">
+        <v>5</v>
       </c>
       <c r="H132" s="14">
         <f t="shared" si="2"/>
-        <v>158.19999999999999</v>
-      </c>
-      <c r="I132"/>
-      <c r="J132"/>
-      <c r="K132"/>
-      <c r="L132"/>
-      <c r="M132"/>
-      <c r="N132"/>
-      <c r="O132"/>
-      <c r="P132"/>
-      <c r="Q132"/>
-      <c r="R132"/>
-      <c r="S132"/>
-      <c r="T132"/>
-      <c r="U132"/>
-      <c r="V132"/>
-      <c r="W132"/>
-      <c r="X132"/>
-      <c r="Y132"/>
-      <c r="Z132"/>
-      <c r="AA132"/>
-      <c r="AB132"/>
-      <c r="AC132"/>
-      <c r="AD132"/>
-      <c r="AE132"/>
-      <c r="AF132"/>
-      <c r="AG132"/>
-      <c r="AH132"/>
-      <c r="AI132"/>
-      <c r="AJ132"/>
-      <c r="AK132"/>
-      <c r="AL132"/>
-      <c r="AM132"/>
-      <c r="AN132"/>
-      <c r="AO132"/>
-      <c r="AP132"/>
-      <c r="AQ132"/>
-      <c r="AR132"/>
-      <c r="AS132"/>
-      <c r="AT132"/>
-      <c r="AU132"/>
-      <c r="AV132"/>
-      <c r="AW132"/>
-      <c r="AX132"/>
-      <c r="AY132"/>
-      <c r="AZ132"/>
-      <c r="BA132"/>
-      <c r="BB132"/>
-      <c r="BC132"/>
-      <c r="BD132"/>
-      <c r="BE132"/>
-      <c r="BF132"/>
-      <c r="BG132"/>
-      <c r="BH132"/>
-      <c r="BI132"/>
-      <c r="BJ132"/>
-      <c r="BK132"/>
-      <c r="BL132"/>
-      <c r="BM132"/>
-      <c r="BN132"/>
-      <c r="BO132"/>
-      <c r="BP132"/>
-      <c r="BQ132"/>
-      <c r="BR132"/>
-      <c r="BS132"/>
-      <c r="BT132"/>
-      <c r="BU132"/>
-      <c r="BV132"/>
-      <c r="BW132"/>
-      <c r="BX132"/>
-      <c r="BY132"/>
-      <c r="BZ132"/>
-      <c r="CA132"/>
-      <c r="CB132"/>
-      <c r="CC132"/>
-      <c r="CD132"/>
-      <c r="CE132"/>
-      <c r="CF132"/>
-      <c r="CG132"/>
-      <c r="CH132"/>
-      <c r="CI132"/>
-      <c r="CJ132"/>
-      <c r="CK132"/>
-      <c r="CL132"/>
-      <c r="CM132"/>
-      <c r="CN132"/>
-      <c r="CO132"/>
-      <c r="CP132"/>
-      <c r="CQ132"/>
-      <c r="CR132"/>
-      <c r="CS132"/>
-      <c r="CT132"/>
-      <c r="CU132"/>
-      <c r="CV132"/>
-      <c r="CW132"/>
-      <c r="CX132"/>
-      <c r="CY132"/>
-      <c r="CZ132"/>
-      <c r="DA132"/>
-      <c r="DB132"/>
-      <c r="DC132"/>
-      <c r="DD132"/>
-      <c r="DE132"/>
-      <c r="DF132"/>
-      <c r="DG132"/>
-      <c r="DH132"/>
-      <c r="DI132"/>
-      <c r="DJ132"/>
-      <c r="DK132"/>
-      <c r="DL132"/>
-      <c r="DM132"/>
-      <c r="DN132"/>
-      <c r="DO132"/>
-      <c r="DP132"/>
-      <c r="DQ132"/>
-      <c r="DR132"/>
-      <c r="DS132"/>
-      <c r="DT132"/>
-      <c r="DU132"/>
-      <c r="DV132"/>
-      <c r="DW132"/>
-      <c r="DX132"/>
-      <c r="DY132"/>
-      <c r="DZ132"/>
-      <c r="EA132"/>
-      <c r="EB132"/>
-      <c r="EC132"/>
-      <c r="ED132"/>
-      <c r="EE132"/>
-      <c r="EF132"/>
-      <c r="EG132"/>
-      <c r="EH132"/>
-      <c r="EI132"/>
-      <c r="EJ132"/>
-      <c r="EK132"/>
-      <c r="EL132"/>
-      <c r="EM132"/>
-      <c r="EN132"/>
-      <c r="EO132"/>
-      <c r="EP132"/>
-      <c r="EQ132"/>
-      <c r="ER132"/>
-      <c r="ES132"/>
-      <c r="ET132"/>
-      <c r="EU132"/>
-      <c r="EV132"/>
-      <c r="EW132"/>
-      <c r="EX132"/>
-      <c r="EY132"/>
-      <c r="EZ132"/>
-      <c r="FA132"/>
-      <c r="FB132"/>
-      <c r="FC132"/>
-      <c r="FD132"/>
-      <c r="FE132"/>
-      <c r="FF132"/>
-      <c r="FG132"/>
-      <c r="FH132"/>
-      <c r="FI132"/>
-      <c r="FJ132"/>
-      <c r="FK132"/>
-      <c r="FL132"/>
-      <c r="FM132"/>
-      <c r="FN132"/>
-      <c r="FO132"/>
-      <c r="FP132"/>
-      <c r="FQ132"/>
-      <c r="FR132"/>
-      <c r="FS132"/>
-      <c r="FT132"/>
-      <c r="FU132"/>
-      <c r="FV132"/>
-      <c r="FW132"/>
-      <c r="FX132"/>
-      <c r="FY132"/>
-      <c r="FZ132"/>
-      <c r="GA132"/>
-      <c r="GB132"/>
-      <c r="GC132"/>
-      <c r="GD132"/>
-      <c r="GE132"/>
-      <c r="GF132"/>
-      <c r="GG132"/>
-      <c r="GH132"/>
-      <c r="GI132"/>
-      <c r="GJ132"/>
-      <c r="GK132"/>
-      <c r="GL132"/>
-      <c r="GM132"/>
-      <c r="GN132"/>
-      <c r="GO132"/>
-      <c r="GP132"/>
-      <c r="GQ132"/>
-      <c r="GR132"/>
-      <c r="GS132"/>
-      <c r="GT132"/>
-      <c r="GU132"/>
-      <c r="GV132"/>
-      <c r="GW132"/>
-      <c r="GX132"/>
-      <c r="GY132"/>
-      <c r="GZ132"/>
-      <c r="HA132"/>
-      <c r="HB132"/>
-      <c r="HC132"/>
-      <c r="HD132"/>
-      <c r="HE132"/>
-      <c r="HF132"/>
-      <c r="HG132"/>
-      <c r="HH132"/>
-      <c r="HI132"/>
-      <c r="HJ132"/>
-      <c r="HK132"/>
-      <c r="HL132"/>
-      <c r="HM132"/>
-      <c r="HN132"/>
-      <c r="HO132"/>
-      <c r="HP132"/>
-      <c r="HQ132"/>
-      <c r="HR132"/>
-      <c r="HS132"/>
-      <c r="HT132"/>
-      <c r="HU132"/>
-      <c r="HV132"/>
-      <c r="HW132"/>
-      <c r="HX132"/>
-      <c r="HY132"/>
-      <c r="HZ132"/>
-      <c r="IA132"/>
-      <c r="IB132"/>
-      <c r="IC132"/>
-      <c r="ID132"/>
-      <c r="IE132"/>
-      <c r="IF132"/>
-      <c r="IG132"/>
-      <c r="IH132"/>
-      <c r="II132"/>
-      <c r="IJ132"/>
-      <c r="IK132"/>
-      <c r="IL132"/>
-      <c r="IM132"/>
-      <c r="IN132"/>
-      <c r="IO132"/>
-      <c r="IP132"/>
-      <c r="IQ132"/>
-      <c r="IR132"/>
-      <c r="IS132"/>
-      <c r="IT132"/>
-      <c r="IU132"/>
+        <v>125</v>
+      </c>
     </row>
     <row r="133" spans="1:255" ht="28.35" customHeight="1">
       <c r="A133" s="23" t="s">
@@ -5624,17 +5623,17 @@
       <c r="C133" s="11"/>
       <c r="D133" s="11"/>
       <c r="E133" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F133" s="24">
+        <v>1</v>
+      </c>
+      <c r="G133" s="25">
         <v>12</v>
       </c>
-      <c r="F133" s="24">
-        <v>25</v>
-      </c>
-      <c r="G133" s="25">
-        <v>5</v>
-      </c>
       <c r="H133" s="14">
         <f t="shared" si="2"/>
-        <v>125</v>
+        <v>12</v>
       </c>
     </row>
     <row r="134" spans="1:255" ht="28.35" customHeight="1">
@@ -5648,35 +5647,35 @@
         <v>21</v>
       </c>
       <c r="F134" s="24">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G134" s="25">
-        <v>12</v>
+        <v>1.36</v>
       </c>
       <c r="H134" s="14">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>10.88</v>
       </c>
     </row>
     <row r="135" spans="1:255" ht="28.35" customHeight="1">
       <c r="A135" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="B135" s="11"/>
+      <c r="B135" s="29"/>
       <c r="C135" s="11"/>
       <c r="D135" s="11"/>
       <c r="E135" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F135" s="24">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="G135" s="25">
-        <v>1.36</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H135" s="14">
         <f t="shared" si="2"/>
-        <v>10.88</v>
+        <v>55.000000000000007</v>
       </c>
     </row>
     <row r="136" spans="1:255" ht="28.35" customHeight="1">
@@ -5690,14 +5689,14 @@
         <v>21</v>
       </c>
       <c r="F136" s="24">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="G136" s="25">
-        <v>2.2000000000000002</v>
+        <v>5.5</v>
       </c>
       <c r="H136" s="14">
         <f t="shared" si="2"/>
-        <v>55.000000000000007</v>
+        <v>203.5</v>
       </c>
     </row>
     <row r="137" spans="1:255" ht="28.35" customHeight="1">
@@ -5711,56 +5710,56 @@
         <v>21</v>
       </c>
       <c r="F137" s="24">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G137" s="25">
-        <v>5.5</v>
+        <v>0.4</v>
       </c>
       <c r="H137" s="14">
         <f t="shared" si="2"/>
-        <v>203.5</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="138" spans="1:255" ht="28.35" customHeight="1">
       <c r="A138" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="B138" s="29"/>
+      <c r="B138" s="11"/>
       <c r="C138" s="11"/>
       <c r="D138" s="11"/>
       <c r="E138" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F138" s="24">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="G138" s="25">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H138" s="14">
         <f t="shared" si="2"/>
-        <v>8.8000000000000007</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="139" spans="1:255" ht="28.35" customHeight="1">
       <c r="A139" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="B139" s="11"/>
+      <c r="B139" s="29"/>
       <c r="C139" s="11"/>
       <c r="D139" s="11"/>
       <c r="E139" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F139" s="24">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="G139" s="25">
-        <v>0.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H139" s="14">
         <f t="shared" si="2"/>
-        <v>3.5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="140" spans="1:255" ht="28.35" customHeight="1">
@@ -5774,14 +5773,14 @@
         <v>21</v>
       </c>
       <c r="F140" s="24">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="G140" s="25">
-        <v>1.1000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="H140" s="14">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>54</v>
       </c>
     </row>
     <row r="141" spans="1:255" ht="28.35" customHeight="1">
@@ -5795,14 +5794,14 @@
         <v>21</v>
       </c>
       <c r="F141" s="24">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="G141" s="25">
-        <v>0.9</v>
+        <v>2.85</v>
       </c>
       <c r="H141" s="14">
         <f t="shared" si="2"/>
-        <v>54</v>
+        <v>85.5</v>
       </c>
     </row>
     <row r="142" spans="1:255" ht="28.35" customHeight="1">
@@ -5816,252 +5815,231 @@
         <v>21</v>
       </c>
       <c r="F142" s="24">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G142" s="25">
-        <v>2.85</v>
+        <v>3.4</v>
       </c>
       <c r="H142" s="14">
         <f t="shared" si="2"/>
-        <v>85.5</v>
+        <v>40.799999999999997</v>
       </c>
     </row>
     <row r="143" spans="1:255" ht="28.35" customHeight="1">
       <c r="A143" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="B143" s="29"/>
+      <c r="B143" s="11"/>
       <c r="C143" s="11"/>
       <c r="D143" s="11"/>
       <c r="E143" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F143" s="24">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="G143" s="25">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="H143" s="14">
         <f t="shared" si="2"/>
-        <v>40.799999999999997</v>
+        <v>78</v>
       </c>
     </row>
     <row r="144" spans="1:255" ht="28.35" customHeight="1">
       <c r="A144" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="B144" s="11"/>
+      <c r="B144" s="29"/>
       <c r="C144" s="11"/>
-      <c r="D144" s="11"/>
+      <c r="D144" s="11" t="s">
+        <v>146</v>
+      </c>
       <c r="E144" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F144" s="24">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G144" s="25">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="H144" s="14">
         <f t="shared" si="2"/>
-        <v>78</v>
+        <v>357</v>
       </c>
     </row>
     <row r="145" spans="1:8" ht="28.35" customHeight="1">
       <c r="A145" s="23" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B145" s="29"/>
       <c r="C145" s="11"/>
       <c r="D145" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E145" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F145" s="24">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="G145" s="25">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H145" s="14">
         <f t="shared" si="2"/>
-        <v>357</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="146" spans="1:8" ht="28.35" customHeight="1">
       <c r="A146" s="23" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B146" s="29"/>
       <c r="C146" s="11"/>
       <c r="D146" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E146" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F146" s="24">
-        <v>100</v>
+        <v>9</v>
       </c>
       <c r="G146" s="25">
         <v>10</v>
       </c>
       <c r="H146" s="14">
         <f t="shared" si="2"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" ht="28.35" customHeight="1">
-      <c r="A147" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="B147" s="29"/>
-      <c r="C147" s="11"/>
-      <c r="D147" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="E147" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F147" s="24">
-        <v>9</v>
-      </c>
-      <c r="G147" s="25">
-        <v>10</v>
-      </c>
-      <c r="H147" s="14">
-        <f t="shared" si="2"/>
         <v>90</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="48.75" customHeight="1">
-      <c r="H148" s="47">
-        <f>SUM(H3:H147)</f>
-        <v>19202.601999999999</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" ht="29.1" customHeight="1"/>
-    <row r="150" spans="1:8" ht="30" customHeight="1"/>
+    <row r="147" spans="1:8" ht="48.75" customHeight="1">
+      <c r="H147" s="47">
+        <f>SUM(H3:H146)</f>
+        <v>19381.201999999997</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="29.1" customHeight="1"/>
+    <row r="149" spans="1:8" ht="30" customHeight="1"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="F111:F113 F21:F25 F80 F18:F19">
+  <conditionalFormatting sqref="F110:F112 F79 F21:F24 F18:F19">
     <cfRule type="cellIs" dxfId="21" priority="2" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F26:F27 F36:F37 F83:F85">
+  <conditionalFormatting sqref="F25:F26 F35:F36 F82:F84">
     <cfRule type="cellIs" dxfId="20" priority="4" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F28:F29">
+  <conditionalFormatting sqref="F27:F28">
     <cfRule type="cellIs" dxfId="19" priority="5" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F33:F34">
+  <conditionalFormatting sqref="F32:F33">
     <cfRule type="cellIs" dxfId="18" priority="6" stopIfTrue="1" operator="lessThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F35">
+  <conditionalFormatting sqref="F34">
     <cfRule type="cellIs" dxfId="17" priority="8" stopIfTrue="1" operator="lessThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F39:F40">
+  <conditionalFormatting sqref="F38:F39">
     <cfRule type="cellIs" dxfId="16" priority="10" stopIfTrue="1" operator="lessThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F41">
+  <conditionalFormatting sqref="F40">
     <cfRule type="cellIs" dxfId="15" priority="11" stopIfTrue="1" operator="lessThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F45 F81:F82 F101 F86:F87">
+  <conditionalFormatting sqref="F44 F80:F81 F100 F85:F86">
     <cfRule type="cellIs" dxfId="14" priority="12" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F49">
+  <conditionalFormatting sqref="F48">
     <cfRule type="cellIs" dxfId="13" priority="13" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F54 F69:F79">
+  <conditionalFormatting sqref="F53 F68:F78">
     <cfRule type="cellIs" dxfId="12" priority="14" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F58">
+  <conditionalFormatting sqref="F57">
     <cfRule type="cellIs" dxfId="11" priority="15" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F63">
+  <conditionalFormatting sqref="F62">
     <cfRule type="cellIs" dxfId="10" priority="16" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>35</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F64">
+  <conditionalFormatting sqref="F63">
     <cfRule type="cellIs" dxfId="9" priority="17" stopIfTrue="1" operator="lessThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F97 F92:F93">
+  <conditionalFormatting sqref="F96 F91:F92">
     <cfRule type="cellIs" dxfId="8" priority="24" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F114 F102">
+  <conditionalFormatting sqref="F113 F101">
     <cfRule type="cellIs" dxfId="7" priority="25" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>150</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F104:F107">
+  <conditionalFormatting sqref="F103:F106">
     <cfRule type="cellIs" dxfId="6" priority="28" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F100">
+  <conditionalFormatting sqref="F99">
     <cfRule type="cellIs" dxfId="5" priority="31" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F96">
+  <conditionalFormatting sqref="F95">
     <cfRule type="cellIs" dxfId="4" priority="33" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F94:F95">
+  <conditionalFormatting sqref="F93:F94">
     <cfRule type="cellIs" dxfId="3" priority="34" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F91">
+  <conditionalFormatting sqref="F90">
     <cfRule type="cellIs" dxfId="2" priority="36" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F89:F90">
+  <conditionalFormatting sqref="F88:F89">
     <cfRule type="cellIs" dxfId="1" priority="38" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F93">
+  <conditionalFormatting sqref="F92">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup paperSize="8" scale="70" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="8" scale="70" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new new 3 maggio
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -1860,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IU149"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="J117" sqref="J117"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="J84" sqref="J84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -3237,14 +3237,14 @@
         <v>21</v>
       </c>
       <c r="F41" s="20">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G41" s="21">
         <v>1.75</v>
       </c>
       <c r="H41" s="14">
         <f t="shared" si="1"/>
-        <v>24.5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4052,14 +4052,14 @@
         <v>21</v>
       </c>
       <c r="F78" s="20">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G78" s="21">
         <v>0.8</v>
       </c>
       <c r="H78" s="14">
         <f t="shared" si="2"/>
-        <v>7.2</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4079,14 +4079,14 @@
         <v>21</v>
       </c>
       <c r="F79" s="20">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G79" s="21">
         <v>1.1000000000000001</v>
       </c>
       <c r="H79" s="14">
         <f t="shared" si="2"/>
-        <v>5.5</v>
+        <v>13.200000000000001</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -5668,14 +5668,14 @@
         <v>21</v>
       </c>
       <c r="F135" s="24">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G135" s="25">
         <v>2.2000000000000002</v>
       </c>
       <c r="H135" s="14">
         <f t="shared" si="2"/>
-        <v>55.000000000000007</v>
+        <v>50.6</v>
       </c>
     </row>
     <row r="136" spans="1:255" ht="28.35" customHeight="1">
@@ -5710,14 +5710,14 @@
         <v>21</v>
       </c>
       <c r="F137" s="24">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G137" s="25">
         <v>0.4</v>
       </c>
       <c r="H137" s="14">
         <f t="shared" si="2"/>
-        <v>8.8000000000000007</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="138" spans="1:255" ht="28.35" customHeight="1">
@@ -5731,14 +5731,14 @@
         <v>21</v>
       </c>
       <c r="F138" s="24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G138" s="25">
         <v>0.5</v>
       </c>
       <c r="H138" s="14">
         <f t="shared" si="2"/>
-        <v>3.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139" spans="1:255" ht="28.35" customHeight="1">
@@ -5918,7 +5918,7 @@
     <row r="147" spans="1:8" ht="48.75" customHeight="1">
       <c r="H147" s="47">
         <f>SUM(H3:H146)</f>
-        <v>19381.201999999997</v>
+        <v>19386.301999999996</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="29.1" customHeight="1"/>

</xml_diff>

<commit_message>
new new 7 maggio
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="230">
   <si>
     <t>PRODOTTO</t>
   </si>
@@ -251,9 +251,6 @@
     <t>Kit scatole vuote</t>
   </si>
   <si>
-    <t>tessuto lana stock (10)</t>
-  </si>
-  <si>
     <t>tessuto lana stock (9)</t>
   </si>
   <si>
@@ -705,6 +702,12 @@
   </si>
   <si>
     <t>26/4/2018</t>
+  </si>
+  <si>
+    <t>tessuto lana quadretti</t>
+  </si>
+  <si>
+    <t>4/5/2018</t>
   </si>
 </sst>
 </file>
@@ -1860,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IU149"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="J84" sqref="J84"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A54" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -1878,7 +1881,7 @@
   <sheetData>
     <row r="1" spans="1:35" s="5" customFormat="1" ht="60.75" customHeight="1">
       <c r="A1" s="48" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -2043,7 +2046,7 @@
     </row>
     <row r="5" spans="1:35" ht="24.95" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -2091,7 +2094,7 @@
     </row>
     <row r="6" spans="1:35" ht="24.2" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
@@ -2139,7 +2142,7 @@
     </row>
     <row r="7" spans="1:35" ht="25.35" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="16"/>
@@ -2189,7 +2192,7 @@
     </row>
     <row r="8" spans="1:35" ht="23.25" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B8" s="10">
         <v>43174</v>
@@ -2243,7 +2246,7 @@
     </row>
     <row r="9" spans="1:35" ht="23.25" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="16"/>
@@ -2293,7 +2296,7 @@
     </row>
     <row r="10" spans="1:35" ht="28.35" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B10" s="10">
         <v>43174</v>
@@ -2347,15 +2350,15 @@
     </row>
     <row r="11" spans="1:35" ht="28.35" customHeight="1">
       <c r="A11" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F11" s="17">
         <v>72</v>
@@ -2397,15 +2400,15 @@
     </row>
     <row r="12" spans="1:35" ht="28.35" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F12" s="17">
         <v>10</v>
@@ -2601,12 +2604,12 @@
     </row>
     <row r="16" spans="1:35" ht="28.35" customHeight="1">
       <c r="A16" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>16</v>
@@ -2704,10 +2707,10 @@
         <v>22</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>28</v>
@@ -2731,10 +2734,10 @@
         <v>23</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="19" t="s">
@@ -2753,7 +2756,7 @@
     </row>
     <row r="20" spans="1:35" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A20" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -2796,10 +2799,10 @@
         <v>25</v>
       </c>
       <c r="B22" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>215</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>216</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>28</v>
@@ -2823,10 +2826,10 @@
         <v>27</v>
       </c>
       <c r="B23" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>224</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>225</v>
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="19" t="s">
@@ -2848,10 +2851,10 @@
         <v>29</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>28</v>
@@ -2896,10 +2899,10 @@
         <v>31</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>28</v>
@@ -2944,13 +2947,13 @@
         <v>33</v>
       </c>
       <c r="B28" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="C28" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="C28" s="19" t="s">
-        <v>214</v>
-      </c>
       <c r="D28" s="19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E28" s="19" t="s">
         <v>34</v>
@@ -3180,7 +3183,7 @@
     </row>
     <row r="39" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A39" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B39" s="19"/>
       <c r="C39" s="19"/>
@@ -3203,7 +3206,7 @@
       </c>
       <c r="B40" s="19"/>
       <c r="C40" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D40" s="19"/>
       <c r="E40" s="28" t="s">
@@ -3225,10 +3228,10 @@
         <v>46</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D41" s="19" t="s">
         <v>28</v>
@@ -3426,10 +3429,10 @@
         <v>57</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D50" s="19" t="s">
         <v>28</v>
@@ -3453,10 +3456,10 @@
         <v>58</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D51" s="19" t="s">
         <v>28</v>
@@ -3561,7 +3564,7 @@
     </row>
     <row r="56" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A56" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B56" s="19"/>
       <c r="C56" s="19"/>
@@ -3587,10 +3590,10 @@
         <v>63</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D57" s="19"/>
       <c r="E57" s="11" t="s">
@@ -3696,26 +3699,26 @@
         <v>68</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D62" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E62" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F62" s="20">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G62" s="21">
         <v>3</v>
       </c>
       <c r="H62" s="14">
         <f t="shared" si="1"/>
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3746,7 +3749,7 @@
       <c r="B64" s="19"/>
       <c r="C64" s="19"/>
       <c r="D64" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E64" s="19" t="s">
         <v>12</v>
@@ -3890,9 +3893,11 @@
     </row>
     <row r="71" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A71" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="B71" s="19"/>
+        <v>228</v>
+      </c>
+      <c r="B71" s="19" t="s">
+        <v>229</v>
+      </c>
       <c r="C71" s="19"/>
       <c r="D71" s="19" t="s">
         <v>49</v>
@@ -3901,19 +3906,19 @@
         <v>12</v>
       </c>
       <c r="F71" s="20">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G71" s="21">
         <v>8.5</v>
       </c>
       <c r="H71" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>204</v>
       </c>
     </row>
     <row r="72" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A72" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B72" s="19"/>
       <c r="C72" s="19"/>
@@ -3936,7 +3941,7 @@
     </row>
     <row r="73" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A73" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B73" s="19"/>
       <c r="C73" s="19"/>
@@ -3959,7 +3964,7 @@
     </row>
     <row r="74" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A74" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B74" s="19"/>
       <c r="C74" s="19"/>
@@ -3980,7 +3985,7 @@
     </row>
     <row r="75" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A75" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B75" s="19"/>
       <c r="C75" s="19"/>
@@ -4001,7 +4006,7 @@
     </row>
     <row r="76" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A76" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B76" s="19"/>
       <c r="C76" s="19"/>
@@ -4009,7 +4014,7 @@
         <v>13</v>
       </c>
       <c r="E76" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F76" s="20">
         <v>150</v>
@@ -4022,7 +4027,7 @@
     </row>
     <row r="77" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A77" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B77" s="19"/>
       <c r="C77" s="19"/>
@@ -4030,7 +4035,7 @@
         <v>13</v>
       </c>
       <c r="E77" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F77" s="20">
         <v>150</v>
@@ -4043,7 +4048,7 @@
     </row>
     <row r="78" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A78" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B78" s="19"/>
       <c r="C78" s="19"/>
@@ -4064,13 +4069,13 @@
     </row>
     <row r="79" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A79" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B79" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D79" s="19" t="s">
         <v>28</v>
@@ -4091,7 +4096,7 @@
     </row>
     <row r="80" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A80" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B80" s="19"/>
       <c r="C80" s="19"/>
@@ -4112,7 +4117,7 @@
     </row>
     <row r="81" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A81" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B81" s="19"/>
       <c r="C81" s="19"/>
@@ -4133,7 +4138,7 @@
     </row>
     <row r="82" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A82" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B82" s="19"/>
       <c r="C82" s="19"/>
@@ -4154,16 +4159,16 @@
     </row>
     <row r="83" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A83" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B83" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="C83" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="D83" s="19" t="s">
         <v>188</v>
-      </c>
-      <c r="C83" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="D83" s="19" t="s">
-        <v>189</v>
       </c>
       <c r="E83" s="19" t="s">
         <v>10</v>
@@ -4181,7 +4186,7 @@
     </row>
     <row r="84" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A84" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B84" s="19"/>
       <c r="C84" s="19"/>
@@ -4202,7 +4207,7 @@
     </row>
     <row r="85" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A85" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B85" s="19"/>
       <c r="C85" s="19"/>
@@ -4223,7 +4228,7 @@
     </row>
     <row r="86" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A86" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B86" s="19"/>
       <c r="C86" s="19"/>
@@ -4244,13 +4249,13 @@
     </row>
     <row r="87" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A87" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B87" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C87" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D87" s="19"/>
       <c r="E87" s="19" t="s">
@@ -4269,13 +4274,13 @@
     </row>
     <row r="88" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A88" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B88" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C88" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D88" s="19"/>
       <c r="E88" s="19" t="s">
@@ -4294,7 +4299,7 @@
     </row>
     <row r="89" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A89" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B89" s="19"/>
       <c r="C89" s="19"/>
@@ -4315,7 +4320,7 @@
     </row>
     <row r="90" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A90" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B90" s="19"/>
       <c r="C90" s="19"/>
@@ -4336,7 +4341,7 @@
     </row>
     <row r="91" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A91" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B91" s="19"/>
       <c r="C91" s="19"/>
@@ -4358,16 +4363,16 @@
     </row>
     <row r="92" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A92" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B92" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="C92" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="D92" s="19" t="s">
         <v>183</v>
-      </c>
-      <c r="C92" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="D92" s="19" t="s">
-        <v>184</v>
       </c>
       <c r="E92" s="19" t="s">
         <v>21</v>
@@ -4386,72 +4391,72 @@
     </row>
     <row r="93" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A93" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B93" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="C93" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="D93" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="C93" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="D93" s="19" t="s">
-        <v>184</v>
-      </c>
       <c r="E93" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F93" s="20">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G93" s="43">
         <v>2.9</v>
       </c>
       <c r="H93" s="46">
         <f t="shared" si="2"/>
-        <v>295.8</v>
+        <v>292.89999999999998</v>
       </c>
       <c r="I93" s="42"/>
     </row>
     <row r="94" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A94" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="B94" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="C94" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="B94" s="19" t="s">
-        <v>228</v>
-      </c>
-      <c r="C94" s="19" t="s">
-        <v>227</v>
-      </c>
       <c r="D94" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E94" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F94" s="20">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G94" s="43">
         <v>4.8</v>
       </c>
       <c r="H94" s="46">
         <f t="shared" si="2"/>
-        <v>230.39999999999998</v>
+        <v>220.79999999999998</v>
       </c>
       <c r="I94" s="42"/>
     </row>
     <row r="95" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A95" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B95" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="C95" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="D95" s="19" t="s">
         <v>183</v>
-      </c>
-      <c r="C95" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="D95" s="19" t="s">
-        <v>184</v>
       </c>
       <c r="E95" s="19" t="s">
         <v>21</v>
@@ -4470,16 +4475,16 @@
     </row>
     <row r="96" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A96" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B96" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="C96" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="D96" s="19" t="s">
         <v>183</v>
-      </c>
-      <c r="C96" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="D96" s="19" t="s">
-        <v>184</v>
       </c>
       <c r="E96" s="19" t="s">
         <v>21</v>
@@ -4498,16 +4503,16 @@
     </row>
     <row r="97" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A97" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B97" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C97" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D97" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E97" s="19" t="s">
         <v>21</v>
@@ -4526,13 +4531,13 @@
     </row>
     <row r="98" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A98" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C98" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D98" s="19" t="s">
         <v>28</v>
@@ -4554,16 +4559,16 @@
     </row>
     <row r="99" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A99" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C99" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D99" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E99" s="19" t="s">
         <v>21</v>
@@ -4581,7 +4586,7 @@
     </row>
     <row r="100" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A100" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B100" s="19"/>
       <c r="C100" s="19"/>
@@ -4604,13 +4609,13 @@
     </row>
     <row r="101" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A101" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B101" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C101" s="19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D101" s="19" t="s">
         <v>28</v>
@@ -4631,13 +4636,13 @@
     </row>
     <row r="102" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A102" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B102" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C102" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D102" s="19"/>
       <c r="E102" s="19" t="s">
@@ -4656,16 +4661,16 @@
     </row>
     <row r="103" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A103" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B103" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C103" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D103" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E103" s="19" t="s">
         <v>21</v>
@@ -4683,7 +4688,7 @@
     </row>
     <row r="104" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A104" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B104" s="19"/>
       <c r="C104" s="19"/>
@@ -4704,7 +4709,7 @@
     </row>
     <row r="105" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A105" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B105" s="19"/>
       <c r="C105" s="19"/>
@@ -4725,16 +4730,16 @@
     </row>
     <row r="106" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A106" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B106" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C106" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D106" s="19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E106" s="19" t="s">
         <v>21</v>
@@ -4752,16 +4757,16 @@
     </row>
     <row r="107" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A107" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B107" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="C107" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="C107" s="19" t="s">
-        <v>200</v>
-      </c>
       <c r="D107" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E107" s="19" t="s">
         <v>34</v>
@@ -4779,7 +4784,7 @@
     </row>
     <row r="108" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A108" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B108" s="29">
         <v>43140</v>
@@ -4788,10 +4793,10 @@
         <v>36</v>
       </c>
       <c r="D108" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E108" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F108" s="24">
         <v>15</v>
@@ -4806,16 +4811,16 @@
     </row>
     <row r="109" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A109" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B109" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="C109" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="C109" s="19" t="s">
+      <c r="D109" s="19" t="s">
         <v>186</v>
-      </c>
-      <c r="D109" s="19" t="s">
-        <v>187</v>
       </c>
       <c r="E109" s="19" t="s">
         <v>21</v>
@@ -4833,13 +4838,13 @@
     </row>
     <row r="110" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A110" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C110" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D110" s="19" t="s">
         <v>28</v>
@@ -4860,13 +4865,13 @@
     </row>
     <row r="111" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A111" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B111" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C111" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D111" s="19" t="s">
         <v>28</v>
@@ -4887,13 +4892,13 @@
     </row>
     <row r="112" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A112" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B112" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="C112" s="19" t="s">
         <v>202</v>
-      </c>
-      <c r="C112" s="19" t="s">
-        <v>203</v>
       </c>
       <c r="D112" s="19"/>
       <c r="E112" s="19" t="s">
@@ -4912,13 +4917,13 @@
     </row>
     <row r="113" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A113" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B113" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C113" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D113" s="19" t="s">
         <v>28</v>
@@ -4939,7 +4944,7 @@
     </row>
     <row r="114" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A114" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B114" s="19"/>
       <c r="C114" s="19"/>
@@ -4960,7 +4965,7 @@
     </row>
     <row r="115" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A115" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B115" s="19"/>
       <c r="C115" s="19"/>
@@ -4981,13 +4986,13 @@
     </row>
     <row r="116" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A116" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C116" s="19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D116" s="19" t="s">
         <v>9</v>
@@ -5008,13 +5013,13 @@
     </row>
     <row r="117" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A117" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B117" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C117" s="19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D117" s="19" t="s">
         <v>9</v>
@@ -5035,7 +5040,7 @@
     </row>
     <row r="118" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A118" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B118" s="19"/>
       <c r="C118" s="19"/>
@@ -5056,19 +5061,19 @@
     </row>
     <row r="119" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A119" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B119" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C119" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="D119" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="B119" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="C119" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="D119" s="19" t="s">
+      <c r="E119" s="19" t="s">
         <v>121</v>
-      </c>
-      <c r="E119" s="19" t="s">
-        <v>122</v>
       </c>
       <c r="F119" s="20">
         <v>6</v>
@@ -5083,7 +5088,7 @@
     </row>
     <row r="120" spans="1:8" s="36" customFormat="1" ht="28.35" customHeight="1">
       <c r="A120" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B120" s="19"/>
       <c r="C120" s="19"/>
@@ -5092,19 +5097,19 @@
         <v>21</v>
       </c>
       <c r="F120" s="20">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="G120" s="21">
         <v>3</v>
       </c>
       <c r="H120" s="14">
         <f t="shared" si="2"/>
-        <v>1752</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="121" spans="1:8" s="36" customFormat="1" ht="28.35" customHeight="1">
       <c r="A121" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B121" s="19"/>
       <c r="C121" s="19"/>
@@ -5125,7 +5130,7 @@
     </row>
     <row r="122" spans="1:8" ht="28.35" customHeight="1">
       <c r="A122" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B122" s="11"/>
       <c r="C122" s="11"/>
@@ -5146,7 +5151,7 @@
     </row>
     <row r="123" spans="1:8" ht="28.35" customHeight="1">
       <c r="A123" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B123" s="19"/>
       <c r="C123" s="19"/>
@@ -5167,13 +5172,13 @@
     </row>
     <row r="124" spans="1:8" ht="28.35" customHeight="1">
       <c r="A124" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B124" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C124" s="19" t="s">
         <v>221</v>
-      </c>
-      <c r="C124" s="19" t="s">
-        <v>222</v>
       </c>
       <c r="D124" s="19" t="s">
         <v>13</v>
@@ -5194,13 +5199,13 @@
     </row>
     <row r="125" spans="1:8" ht="28.35" customHeight="1">
       <c r="A125" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B125" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D125" s="19" t="s">
         <v>13</v>
@@ -5221,7 +5226,7 @@
     </row>
     <row r="126" spans="1:8" ht="28.35" customHeight="1">
       <c r="A126" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B126" s="11"/>
       <c r="C126" s="11"/>
@@ -5242,7 +5247,7 @@
     </row>
     <row r="127" spans="1:8" ht="28.35" customHeight="1">
       <c r="A127" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B127" s="19"/>
       <c r="C127" s="19"/>
@@ -5263,7 +5268,7 @@
     </row>
     <row r="128" spans="1:8" ht="28.35" customHeight="1">
       <c r="A128" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B128" s="19"/>
       <c r="C128" s="19"/>
@@ -5284,12 +5289,12 @@
     </row>
     <row r="129" spans="1:255" ht="28.35" customHeight="1">
       <c r="A129" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B129" s="19"/>
       <c r="C129" s="19"/>
       <c r="D129" s="19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E129" s="11" t="s">
         <v>12</v>
@@ -5307,7 +5312,7 @@
     </row>
     <row r="130" spans="1:255" ht="28.35" customHeight="1">
       <c r="A130" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B130" s="11"/>
       <c r="C130" s="11"/>
@@ -5328,7 +5333,7 @@
     </row>
     <row r="131" spans="1:255" ht="28.35" customHeight="1">
       <c r="A131" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B131" s="19"/>
       <c r="C131" s="19"/>
@@ -5596,7 +5601,7 @@
     </row>
     <row r="132" spans="1:255" ht="28.35" customHeight="1">
       <c r="A132" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B132" s="11"/>
       <c r="C132" s="11"/>
@@ -5617,7 +5622,7 @@
     </row>
     <row r="133" spans="1:255" ht="28.35" customHeight="1">
       <c r="A133" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B133" s="11"/>
       <c r="C133" s="11"/>
@@ -5638,7 +5643,7 @@
     </row>
     <row r="134" spans="1:255" ht="28.35" customHeight="1">
       <c r="A134" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B134" s="11"/>
       <c r="C134" s="11"/>
@@ -5659,7 +5664,7 @@
     </row>
     <row r="135" spans="1:255" ht="28.35" customHeight="1">
       <c r="A135" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B135" s="29"/>
       <c r="C135" s="11"/>
@@ -5668,19 +5673,19 @@
         <v>21</v>
       </c>
       <c r="F135" s="24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G135" s="25">
         <v>2.2000000000000002</v>
       </c>
       <c r="H135" s="14">
         <f t="shared" si="2"/>
-        <v>50.6</v>
+        <v>48.400000000000006</v>
       </c>
     </row>
     <row r="136" spans="1:255" ht="28.35" customHeight="1">
       <c r="A136" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B136" s="29"/>
       <c r="C136" s="11"/>
@@ -5701,11 +5706,13 @@
     </row>
     <row r="137" spans="1:255" ht="28.35" customHeight="1">
       <c r="A137" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B137" s="29"/>
       <c r="C137" s="11"/>
-      <c r="D137" s="11"/>
+      <c r="D137" s="11">
+        <v>47</v>
+      </c>
       <c r="E137" s="11" t="s">
         <v>21</v>
       </c>
@@ -5722,7 +5729,7 @@
     </row>
     <row r="138" spans="1:255" ht="28.35" customHeight="1">
       <c r="A138" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B138" s="11"/>
       <c r="C138" s="11"/>
@@ -5731,19 +5738,19 @@
         <v>21</v>
       </c>
       <c r="F138" s="24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G138" s="25">
         <v>0.5</v>
       </c>
       <c r="H138" s="14">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="139" spans="1:255" ht="28.35" customHeight="1">
       <c r="A139" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B139" s="29"/>
       <c r="C139" s="11"/>
@@ -5752,19 +5759,19 @@
         <v>21</v>
       </c>
       <c r="F139" s="24">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G139" s="25">
         <v>1.1000000000000001</v>
       </c>
       <c r="H139" s="14">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>31.900000000000002</v>
       </c>
     </row>
     <row r="140" spans="1:255" ht="28.35" customHeight="1">
       <c r="A140" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B140" s="29"/>
       <c r="C140" s="11"/>
@@ -5785,7 +5792,7 @@
     </row>
     <row r="141" spans="1:255" ht="28.35" customHeight="1">
       <c r="A141" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B141" s="29"/>
       <c r="C141" s="11"/>
@@ -5806,7 +5813,7 @@
     </row>
     <row r="142" spans="1:255" ht="28.35" customHeight="1">
       <c r="A142" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B142" s="29"/>
       <c r="C142" s="11"/>
@@ -5827,7 +5834,7 @@
     </row>
     <row r="143" spans="1:255" ht="28.35" customHeight="1">
       <c r="A143" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B143" s="11"/>
       <c r="C143" s="11"/>
@@ -5848,12 +5855,12 @@
     </row>
     <row r="144" spans="1:255" ht="28.35" customHeight="1">
       <c r="A144" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B144" s="29"/>
       <c r="C144" s="11"/>
       <c r="D144" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E144" s="11" t="s">
         <v>21</v>
@@ -5871,12 +5878,12 @@
     </row>
     <row r="145" spans="1:8" ht="28.35" customHeight="1">
       <c r="A145" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B145" s="29"/>
       <c r="C145" s="11"/>
       <c r="D145" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E145" s="11" t="s">
         <v>21</v>
@@ -5894,12 +5901,12 @@
     </row>
     <row r="146" spans="1:8" ht="28.35" customHeight="1">
       <c r="A146" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B146" s="29"/>
       <c r="C146" s="11"/>
       <c r="D146" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E146" s="11" t="s">
         <v>21</v>
@@ -5918,7 +5925,7 @@
     <row r="147" spans="1:8" ht="48.75" customHeight="1">
       <c r="H147" s="47">
         <f>SUM(H3:H146)</f>
-        <v>19386.301999999996</v>
+        <v>19563.002</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="29.1" customHeight="1"/>

</xml_diff>

<commit_message>
new new 8 maggio
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IU149"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A54" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -2257,14 +2257,14 @@
         <v>12</v>
       </c>
       <c r="F9" s="17">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G9" s="13">
         <v>3</v>
       </c>
       <c r="H9" s="14">
         <f t="shared" si="0"/>
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -5694,14 +5694,14 @@
         <v>21</v>
       </c>
       <c r="F136" s="24">
-        <v>37</v>
+        <v>3625</v>
       </c>
       <c r="G136" s="25">
         <v>5.5</v>
       </c>
       <c r="H136" s="14">
         <f t="shared" si="2"/>
-        <v>203.5</v>
+        <v>19937.5</v>
       </c>
     </row>
     <row r="137" spans="1:255" ht="28.35" customHeight="1">
@@ -5843,14 +5843,14 @@
         <v>21</v>
       </c>
       <c r="F143" s="24">
-        <v>26</v>
+        <v>259</v>
       </c>
       <c r="G143" s="25">
         <v>3</v>
       </c>
       <c r="H143" s="14">
         <f t="shared" si="2"/>
-        <v>78</v>
+        <v>777</v>
       </c>
     </row>
     <row r="144" spans="1:255" ht="28.35" customHeight="1">
@@ -5925,7 +5925,7 @@
     <row r="147" spans="1:8" ht="48.75" customHeight="1">
       <c r="H147" s="47">
         <f>SUM(H3:H146)</f>
-        <v>19563.002</v>
+        <v>39990.002000000008</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="29.1" customHeight="1"/>

</xml_diff>

<commit_message>
new new 10 maggio
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="232">
   <si>
     <t>PRODOTTO</t>
   </si>
@@ -708,6 +708,12 @@
   </si>
   <si>
     <t>4/5/2018</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>,</t>
   </si>
 </sst>
 </file>
@@ -1863,8 +1869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IU149"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -2361,14 +2367,14 @@
         <v>151</v>
       </c>
       <c r="F11" s="17">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="G11" s="13">
         <v>0.5</v>
       </c>
       <c r="H11" s="14">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>31.5</v>
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
@@ -3621,14 +3627,14 @@
         <v>12</v>
       </c>
       <c r="F58" s="24">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G58" s="25">
         <v>4.8499999999999996</v>
       </c>
       <c r="H58" s="14">
         <f t="shared" si="1"/>
-        <v>58.199999999999996</v>
+        <v>53.349999999999994</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4406,14 +4412,14 @@
         <v>21</v>
       </c>
       <c r="F93" s="20">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G93" s="43">
         <v>2.9</v>
       </c>
       <c r="H93" s="46">
         <f t="shared" si="2"/>
-        <v>292.89999999999998</v>
+        <v>287.09999999999997</v>
       </c>
       <c r="I93" s="42"/>
     </row>
@@ -4434,14 +4440,14 @@
         <v>21</v>
       </c>
       <c r="F94" s="20">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G94" s="43">
         <v>4.8</v>
       </c>
       <c r="H94" s="46">
         <f t="shared" si="2"/>
-        <v>220.79999999999998</v>
+        <v>192</v>
       </c>
       <c r="I94" s="42"/>
     </row>
@@ -4825,15 +4831,15 @@
       <c r="E109" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F109" s="20">
-        <v>1116</v>
+      <c r="F109" s="20" t="s">
+        <v>231</v>
       </c>
       <c r="G109" s="21">
         <v>0.66</v>
       </c>
-      <c r="H109" s="14">
-        <f t="shared" si="2"/>
-        <v>736.56000000000006</v>
+      <c r="H109" s="14" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="110" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -5214,14 +5220,14 @@
         <v>12</v>
       </c>
       <c r="F125" s="20">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="G125" s="21">
         <v>2.21</v>
       </c>
       <c r="H125" s="14">
         <f t="shared" si="2"/>
-        <v>442</v>
+        <v>331.5</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="28.35" customHeight="1">
@@ -5249,7 +5255,9 @@
       <c r="A127" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="B127" s="19"/>
+      <c r="B127" s="19" t="s">
+        <v>230</v>
+      </c>
       <c r="C127" s="19"/>
       <c r="D127" s="19"/>
       <c r="E127" s="11" t="s">
@@ -5694,14 +5702,14 @@
         <v>21</v>
       </c>
       <c r="F136" s="24">
-        <v>3625</v>
+        <v>17</v>
       </c>
       <c r="G136" s="25">
         <v>5.5</v>
       </c>
       <c r="H136" s="14">
         <f t="shared" si="2"/>
-        <v>19937.5</v>
+        <v>93.5</v>
       </c>
     </row>
     <row r="137" spans="1:255" ht="28.35" customHeight="1">
@@ -5710,21 +5718,19 @@
       </c>
       <c r="B137" s="29"/>
       <c r="C137" s="11"/>
-      <c r="D137" s="11">
-        <v>47</v>
-      </c>
+      <c r="D137" s="11"/>
       <c r="E137" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F137" s="24">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="G137" s="25">
         <v>0.4</v>
       </c>
       <c r="H137" s="14">
         <f t="shared" si="2"/>
-        <v>8.4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="138" spans="1:255" ht="28.35" customHeight="1">
@@ -5822,14 +5828,14 @@
         <v>21</v>
       </c>
       <c r="F142" s="24">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G142" s="25">
         <v>3.4</v>
       </c>
       <c r="H142" s="14">
         <f t="shared" si="2"/>
-        <v>40.799999999999997</v>
+        <v>30.599999999999998</v>
       </c>
     </row>
     <row r="143" spans="1:255" ht="28.35" customHeight="1">
@@ -5843,14 +5849,14 @@
         <v>21</v>
       </c>
       <c r="F143" s="24">
-        <v>259</v>
+        <v>23</v>
       </c>
       <c r="G143" s="25">
         <v>3</v>
       </c>
       <c r="H143" s="14">
         <f t="shared" si="2"/>
-        <v>777</v>
+        <v>69</v>
       </c>
     </row>
     <row r="144" spans="1:255" ht="28.35" customHeight="1">
@@ -5923,9 +5929,9 @@
       </c>
     </row>
     <row r="147" spans="1:8" ht="48.75" customHeight="1">
-      <c r="H147" s="47">
+      <c r="H147" s="47" t="e">
         <f>SUM(H3:H146)</f>
-        <v>39990.002000000008</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="29.1" customHeight="1"/>

</xml_diff>

<commit_message>
new new 11 maggio
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -1233,10 +1233,10 @@
     <xf numFmtId="165" fontId="13" fillId="0" borderId="6" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="13" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="21" fillId="13" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1897,8 +1897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IU154"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A142" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="E160" sqref="E160"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -1914,16 +1914,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="5" customFormat="1" ht="60.75" customHeight="1">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:35" ht="29.1" customHeight="1">
       <c r="A2" s="6" t="s">
@@ -2187,14 +2187,14 @@
         <v>12</v>
       </c>
       <c r="F7" s="17">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G7" s="13">
         <v>3</v>
       </c>
       <c r="H7" s="14">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
@@ -2241,14 +2241,14 @@
         <v>12</v>
       </c>
       <c r="F8" s="17">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G8" s="13">
         <v>3</v>
       </c>
       <c r="H8" s="14">
         <f t="shared" si="0"/>
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -2345,14 +2345,14 @@
         <v>12</v>
       </c>
       <c r="F10" s="17">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G10" s="13">
         <v>2.35</v>
       </c>
       <c r="H10" s="14">
         <f t="shared" si="0"/>
-        <v>129.25</v>
+        <v>117.5</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -4123,14 +4123,14 @@
         <v>21</v>
       </c>
       <c r="F73" s="20">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G73" s="21">
         <v>33.5</v>
       </c>
       <c r="H73" s="14">
         <f t="shared" si="2"/>
-        <v>2043.5</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="74" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4690,14 +4690,14 @@
         <v>21</v>
       </c>
       <c r="F98" s="20">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G98" s="43">
         <v>2.9</v>
       </c>
       <c r="H98" s="46">
         <f t="shared" si="2"/>
-        <v>287.09999999999997</v>
+        <v>284.2</v>
       </c>
       <c r="I98" s="42"/>
     </row>
@@ -4718,14 +4718,14 @@
         <v>21</v>
       </c>
       <c r="F99" s="20">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G99" s="43">
         <v>4.8</v>
       </c>
       <c r="H99" s="46">
         <f t="shared" si="2"/>
-        <v>192</v>
+        <v>182.4</v>
       </c>
       <c r="I99" s="42"/>
     </row>
@@ -5980,14 +5980,14 @@
         <v>21</v>
       </c>
       <c r="F141" s="24">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G141" s="25">
         <v>5.5</v>
       </c>
       <c r="H141" s="14">
         <f t="shared" si="2"/>
-        <v>93.5</v>
+        <v>88</v>
       </c>
     </row>
     <row r="142" spans="1:255" ht="28.35" customHeight="1">
@@ -6207,9 +6207,9 @@
       </c>
     </row>
     <row r="152" spans="1:8" ht="48.75" customHeight="1">
-      <c r="H152" s="48">
+      <c r="H152" s="47">
         <f>SUM(H3:H151)</f>
-        <v>19153.452000000001</v>
+        <v>19145.202000000001</v>
       </c>
     </row>
     <row r="153" spans="1:8" ht="29.1" customHeight="1"/>

</xml_diff>

<commit_message>
new new 11 maggio carichi
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -10,15 +10,15 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$151</definedName>
-    <definedName name="Excel_BuiltIn_Print_Area" localSheetId="0">Sheet1!$A$1:$H$135</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$152</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area" localSheetId="0">Sheet1!$A$1:$H$136</definedName>
   </definedNames>
   <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="240">
   <si>
     <t>PRODOTTO</t>
   </si>
@@ -668,9 +668,6 @@
     <t>4</t>
   </si>
   <si>
-    <t>85</t>
-  </si>
-  <si>
     <t>850</t>
   </si>
   <si>
@@ -729,6 +726,18 @@
   </si>
   <si>
     <t>ATI</t>
+  </si>
+  <si>
+    <t>Fogli per lavagna</t>
+  </si>
+  <si>
+    <t>11/5/2018</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>130</t>
   </si>
 </sst>
 </file>
@@ -1895,10 +1904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IU154"/>
+  <dimension ref="A1:IU155"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -2439,7 +2448,7 @@
       <c r="B12" s="10"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>151</v>
@@ -2484,12 +2493,12 @@
     </row>
     <row r="13" spans="1:35" ht="28.35" customHeight="1">
       <c r="A13" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>151</v>
@@ -2534,12 +2543,12 @@
     </row>
     <row r="14" spans="1:35" ht="28.35" customHeight="1">
       <c r="A14" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E14" s="16" t="s">
         <v>151</v>
@@ -2584,12 +2593,12 @@
     </row>
     <row r="15" spans="1:35" ht="28.35" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E15" s="16" t="s">
         <v>151</v>
@@ -2634,12 +2643,12 @@
     </row>
     <row r="16" spans="1:35" ht="28.35" customHeight="1">
       <c r="A16" s="15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>151</v>
@@ -2684,12 +2693,12 @@
     </row>
     <row r="17" spans="1:35" ht="27.75" customHeight="1">
       <c r="A17" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>151</v>
@@ -3009,7 +3018,7 @@
         <v>3</v>
       </c>
       <c r="H23" s="14">
-        <f t="shared" ref="H23:H71" si="1">F23*G23</f>
+        <f t="shared" ref="H23:H72" si="1">F23*G23</f>
         <v>6</v>
       </c>
     </row>
@@ -3021,7 +3030,7 @@
         <v>214</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D24" s="19"/>
       <c r="E24" s="19" t="s">
@@ -3110,10 +3119,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C28" s="19" t="s">
         <v>223</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>224</v>
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="19" t="s">
@@ -3183,10 +3192,10 @@
         <v>31</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>214</v>
+        <v>237</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>28</v>
@@ -3195,14 +3204,14 @@
         <v>26</v>
       </c>
       <c r="F31" s="20">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G31" s="21">
         <v>2.76</v>
       </c>
       <c r="H31" s="14">
         <f t="shared" si="1"/>
-        <v>41.4</v>
+        <v>55.199999999999996</v>
       </c>
     </row>
     <row r="32" spans="1:35" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3871,208 +3880,214 @@
     </row>
     <row r="62" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A62" s="18" t="s">
-        <v>63</v>
+        <v>236</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>214</v>
+        <v>237</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="D62" s="19"/>
+        <v>179</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E62" s="11" t="s">
-        <v>21</v>
+        <v>151</v>
       </c>
       <c r="F62" s="20">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G62" s="21">
-        <v>0.44</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="H62" s="14">
         <f t="shared" si="1"/>
-        <v>3.08</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A63" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
+      <c r="A63" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="C63" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="D63" s="19"/>
       <c r="E63" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F63" s="24">
-        <v>11</v>
-      </c>
-      <c r="G63" s="25">
-        <v>4.8499999999999996</v>
+        <v>21</v>
+      </c>
+      <c r="F63" s="20">
+        <v>7</v>
+      </c>
+      <c r="G63" s="21">
+        <v>0.44</v>
       </c>
       <c r="H63" s="14">
         <f t="shared" si="1"/>
-        <v>53.349999999999994</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A64" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="B64" s="29"/>
+        <v>64</v>
+      </c>
+      <c r="B64" s="11"/>
       <c r="C64" s="11"/>
       <c r="D64" s="11"/>
       <c r="E64" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F64" s="24">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="G64" s="25">
-        <v>5.04</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="H64" s="14">
         <f t="shared" si="1"/>
-        <v>151.19999999999999</v>
+        <v>53.349999999999994</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A65" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B65" s="19"/>
-      <c r="C65" s="19"/>
-      <c r="D65" s="19"/>
+      <c r="A65" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" s="29"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
       <c r="E65" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F65" s="20">
-        <v>25</v>
-      </c>
-      <c r="G65" s="21">
-        <v>8.3000000000000007</v>
+      <c r="F65" s="24">
+        <v>30</v>
+      </c>
+      <c r="G65" s="25">
+        <v>5.04</v>
       </c>
       <c r="H65" s="14">
         <f t="shared" si="1"/>
-        <v>207.50000000000003</v>
+        <v>151.19999999999999</v>
       </c>
     </row>
     <row r="66" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A66" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B66" s="19"/>
       <c r="C66" s="19"/>
       <c r="D66" s="19"/>
-      <c r="E66" s="19" t="s">
-        <v>21</v>
+      <c r="E66" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="F66" s="20">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="G66" s="21">
-        <v>0.75</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="H66" s="14">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>207.50000000000003</v>
       </c>
     </row>
     <row r="67" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A67" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B67" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="C67" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="D67" s="19" t="s">
-        <v>156</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="B67" s="19"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="19"/>
       <c r="E67" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F67" s="20">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="G67" s="21">
-        <v>3</v>
+        <v>0.75</v>
       </c>
       <c r="H67" s="14">
         <f t="shared" si="1"/>
-        <v>168</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A68" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B68" s="19"/>
-      <c r="C68" s="19"/>
-      <c r="D68" s="19"/>
+        <v>68</v>
+      </c>
+      <c r="B68" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="C68" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="D68" s="19" t="s">
+        <v>156</v>
+      </c>
       <c r="E68" s="19" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F68" s="20">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="G68" s="21">
         <v>3</v>
       </c>
       <c r="H68" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>168</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A69" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B69" s="19"/>
       <c r="C69" s="19"/>
-      <c r="D69" s="19" t="s">
-        <v>149</v>
-      </c>
+      <c r="D69" s="19"/>
       <c r="E69" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F69" s="20">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="G69" s="21">
         <v>3</v>
       </c>
       <c r="H69" s="14">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A70" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" s="19"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="E70" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F70" s="20">
+        <v>35</v>
+      </c>
+      <c r="G70" s="21">
+        <v>3</v>
+      </c>
+      <c r="H70" s="14">
+        <f t="shared" si="1"/>
         <v>105</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A70" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="B70" s="31"/>
-      <c r="C70" s="31"/>
-      <c r="D70" s="31"/>
-      <c r="E70" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="F70" s="20">
-        <v>18</v>
-      </c>
-      <c r="G70" s="32">
-        <v>3</v>
-      </c>
-      <c r="H70" s="33">
-        <f t="shared" si="1"/>
-        <v>54</v>
       </c>
     </row>
     <row r="71" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A71" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B71" s="31"/>
       <c r="C71" s="31"/>
@@ -4081,61 +4096,61 @@
         <v>12</v>
       </c>
       <c r="F71" s="20">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G71" s="32">
         <v>3</v>
       </c>
       <c r="H71" s="33">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>54</v>
       </c>
     </row>
     <row r="72" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A72" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B72" s="19"/>
-      <c r="C72" s="19"/>
-      <c r="D72" s="19"/>
-      <c r="E72" s="19" t="s">
+      <c r="A72" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" s="31"/>
+      <c r="C72" s="31"/>
+      <c r="D72" s="31"/>
+      <c r="E72" s="31" t="s">
         <v>12</v>
       </c>
       <c r="F72" s="20">
-        <v>43</v>
-      </c>
-      <c r="G72" s="21">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="H72" s="14">
-        <f t="shared" ref="H72:H151" si="2">F72*G72</f>
-        <v>210.70000000000002</v>
+        <v>7</v>
+      </c>
+      <c r="G72" s="32">
+        <v>3</v>
+      </c>
+      <c r="H72" s="33">
+        <f t="shared" si="1"/>
+        <v>21</v>
       </c>
     </row>
     <row r="73" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A73" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B73" s="19"/>
       <c r="C73" s="19"/>
       <c r="D73" s="19"/>
       <c r="E73" s="19" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F73" s="20">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="G73" s="21">
-        <v>33.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="H73" s="14">
-        <f t="shared" si="2"/>
-        <v>2077</v>
+        <f t="shared" ref="H73:H152" si="2">F73*G73</f>
+        <v>210.70000000000002</v>
       </c>
     </row>
     <row r="74" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A74" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B74" s="19"/>
       <c r="C74" s="19"/>
@@ -4144,19 +4159,19 @@
         <v>21</v>
       </c>
       <c r="F74" s="20">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="G74" s="21">
-        <v>2</v>
+        <v>33.5</v>
       </c>
       <c r="H74" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="75" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A75" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B75" s="19"/>
       <c r="C75" s="19"/>
@@ -4165,46 +4180,44 @@
         <v>21</v>
       </c>
       <c r="F75" s="20">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="G75" s="21">
-        <v>4.3</v>
+        <v>2</v>
       </c>
       <c r="H75" s="14">
         <f t="shared" si="2"/>
-        <v>81.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A76" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="B76" s="19" t="s">
-        <v>229</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B76" s="19"/>
       <c r="C76" s="19"/>
-      <c r="D76" s="19" t="s">
-        <v>49</v>
-      </c>
+      <c r="D76" s="19"/>
       <c r="E76" s="19" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F76" s="20">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G76" s="21">
-        <v>8.5</v>
+        <v>4.3</v>
       </c>
       <c r="H76" s="14">
         <f t="shared" si="2"/>
-        <v>204</v>
+        <v>81.7</v>
       </c>
     </row>
     <row r="77" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A77" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="B77" s="19"/>
+        <v>227</v>
+      </c>
+      <c r="B77" s="19" t="s">
+        <v>228</v>
+      </c>
       <c r="C77" s="19"/>
       <c r="D77" s="19" t="s">
         <v>49</v>
@@ -4213,19 +4226,19 @@
         <v>12</v>
       </c>
       <c r="F77" s="20">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="G77" s="21">
         <v>8.5</v>
       </c>
       <c r="H77" s="14">
         <f t="shared" si="2"/>
-        <v>102</v>
+        <v>204</v>
       </c>
     </row>
     <row r="78" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A78" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B78" s="19"/>
       <c r="C78" s="19"/>
@@ -4236,40 +4249,42 @@
         <v>12</v>
       </c>
       <c r="F78" s="20">
-        <v>1.5</v>
+        <v>12</v>
       </c>
       <c r="G78" s="21">
-        <v>5</v>
+        <v>8.5</v>
       </c>
       <c r="H78" s="14">
         <f t="shared" si="2"/>
-        <v>7.5</v>
+        <v>102</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A79" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B79" s="19"/>
       <c r="C79" s="19"/>
-      <c r="D79" s="19"/>
+      <c r="D79" s="19" t="s">
+        <v>49</v>
+      </c>
       <c r="E79" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F79" s="20">
-        <v>20</v>
+        <v>1.5</v>
       </c>
       <c r="G79" s="21">
         <v>5</v>
       </c>
       <c r="H79" s="14">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A80" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B80" s="19"/>
       <c r="C80" s="19"/>
@@ -4278,40 +4293,40 @@
         <v>12</v>
       </c>
       <c r="F80" s="20">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="G80" s="21">
         <v>5</v>
       </c>
       <c r="H80" s="14">
         <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A81" s="18" t="s">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="B81" s="19"/>
       <c r="C81" s="19"/>
-      <c r="D81" s="19" t="s">
-        <v>13</v>
-      </c>
+      <c r="D81" s="19"/>
       <c r="E81" s="19" t="s">
-        <v>151</v>
+        <v>12</v>
       </c>
       <c r="F81" s="20">
+        <v>3</v>
+      </c>
+      <c r="G81" s="21">
+        <v>5</v>
+      </c>
+      <c r="H81" s="14">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A82" s="18" t="s">
         <v>150</v>
-      </c>
-      <c r="G81" s="21"/>
-      <c r="H81" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A82" s="18" t="s">
-        <v>152</v>
       </c>
       <c r="B82" s="19"/>
       <c r="C82" s="19"/>
@@ -4330,78 +4345,78 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
+    <row r="83" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A83" s="18" t="s">
-        <v>81</v>
+        <v>152</v>
       </c>
       <c r="B83" s="19"/>
       <c r="C83" s="19"/>
-      <c r="D83" s="19"/>
+      <c r="D83" s="19" t="s">
+        <v>13</v>
+      </c>
       <c r="E83" s="19" t="s">
-        <v>21</v>
+        <v>151</v>
       </c>
       <c r="F83" s="20">
+        <v>150</v>
+      </c>
+      <c r="G83" s="21"/>
+      <c r="H83" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A84" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B84" s="19"/>
+      <c r="C84" s="19"/>
+      <c r="D84" s="19"/>
+      <c r="E84" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F84" s="20">
         <v>8</v>
       </c>
-      <c r="G83" s="21">
+      <c r="G84" s="21">
         <v>0.8</v>
       </c>
-      <c r="H83" s="14">
+      <c r="H84" s="14">
         <f t="shared" si="2"/>
         <v>6.4</v>
       </c>
     </row>
-    <row r="84" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A84" s="18" t="s">
+    <row r="85" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A85" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="B84" s="19" t="s">
+      <c r="B85" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="C84" s="19" t="s">
+      <c r="C85" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="D84" s="19" t="s">
+      <c r="D85" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E84" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F84" s="20">
+      <c r="E85" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F85" s="20">
         <v>12</v>
       </c>
-      <c r="G84" s="21">
+      <c r="G85" s="21">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H84" s="14">
+      <c r="H85" s="14">
         <f t="shared" si="2"/>
         <v>13.200000000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A85" s="18" t="s">
+    <row r="86" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A86" s="18" t="s">
         <v>83</v>
-      </c>
-      <c r="B85" s="19"/>
-      <c r="C85" s="19"/>
-      <c r="D85" s="19"/>
-      <c r="E85" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F85" s="20">
-        <v>4</v>
-      </c>
-      <c r="G85" s="21">
-        <v>0.9</v>
-      </c>
-      <c r="H85" s="14">
-        <f t="shared" si="2"/>
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A86" s="18" t="s">
-        <v>84</v>
       </c>
       <c r="B86" s="19"/>
       <c r="C86" s="19"/>
@@ -4410,19 +4425,19 @@
         <v>21</v>
       </c>
       <c r="F86" s="20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G86" s="21">
-        <v>1.5</v>
+        <v>0.9</v>
       </c>
       <c r="H86" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A87" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B87" s="19"/>
       <c r="C87" s="19"/>
@@ -4431,67 +4446,67 @@
         <v>21</v>
       </c>
       <c r="F87" s="20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G87" s="21">
         <v>1.5</v>
       </c>
       <c r="H87" s="14">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A88" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B88" s="19"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="19"/>
+      <c r="E88" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F88" s="20">
+        <v>3</v>
+      </c>
+      <c r="G88" s="21">
+        <v>1.5</v>
+      </c>
+      <c r="H88" s="14">
+        <f t="shared" si="2"/>
         <v>4.5</v>
       </c>
     </row>
-    <row r="88" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A88" s="18" t="s">
+    <row r="89" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A89" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="B88" s="19" t="s">
+      <c r="B89" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="C88" s="19" t="s">
+      <c r="C89" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="D88" s="19" t="s">
+      <c r="D89" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="E88" s="19" t="s">
+      <c r="E89" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="F88" s="20">
+      <c r="F89" s="20">
         <v>4</v>
       </c>
-      <c r="G88" s="21">
+      <c r="G89" s="21">
         <v>12.5</v>
       </c>
-      <c r="H88" s="14">
+      <c r="H89" s="14">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
     </row>
-    <row r="89" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A89" s="18" t="s">
+    <row r="90" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A90" s="18" t="s">
         <v>87</v>
-      </c>
-      <c r="B89" s="19"/>
-      <c r="C89" s="19"/>
-      <c r="D89" s="19"/>
-      <c r="E89" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F89" s="20">
-        <v>2</v>
-      </c>
-      <c r="G89" s="21">
-        <v>2.5</v>
-      </c>
-      <c r="H89" s="14">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A90" s="18" t="s">
-        <v>88</v>
       </c>
       <c r="B90" s="19"/>
       <c r="C90" s="19"/>
@@ -4500,19 +4515,19 @@
         <v>21</v>
       </c>
       <c r="F90" s="20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G90" s="21">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="H90" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A91" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B91" s="19"/>
       <c r="C91" s="19"/>
@@ -4531,37 +4546,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
+    <row r="92" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A92" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="B92" s="19" t="s">
-        <v>211</v>
-      </c>
-      <c r="C92" s="19" t="s">
-        <v>180</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="B92" s="19"/>
+      <c r="C92" s="19"/>
       <c r="D92" s="19"/>
       <c r="E92" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F92" s="20">
-        <v>50</v>
-      </c>
-      <c r="G92" s="38">
-        <v>0.19</v>
-      </c>
-      <c r="H92" s="44">
-        <f t="shared" si="2"/>
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
+        <v>0</v>
+      </c>
+      <c r="G92" s="21">
+        <v>1</v>
+      </c>
+      <c r="H92" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A93" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B93" s="19" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C93" s="19" t="s">
         <v>180</v>
@@ -4570,41 +4581,45 @@
       <c r="E93" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F93" s="37">
+      <c r="F93" s="20">
         <v>50</v>
       </c>
-      <c r="G93" s="40">
+      <c r="G93" s="38">
         <v>0.19</v>
       </c>
-      <c r="H93" s="46">
+      <c r="H93" s="44">
         <f t="shared" si="2"/>
         <v>9.5</v>
       </c>
     </row>
-    <row r="94" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
+    <row r="94" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A94" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="B94" s="19"/>
-      <c r="C94" s="19"/>
+        <v>91</v>
+      </c>
+      <c r="B94" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="C94" s="19" t="s">
+        <v>180</v>
+      </c>
       <c r="D94" s="19"/>
       <c r="E94" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F94" s="20">
-        <v>3</v>
-      </c>
-      <c r="G94" s="39">
-        <v>1.2</v>
-      </c>
-      <c r="H94" s="45">
-        <f t="shared" si="2"/>
-        <v>3.5999999999999996</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="F94" s="37">
+        <v>50</v>
+      </c>
+      <c r="G94" s="40">
+        <v>0.19</v>
+      </c>
+      <c r="H94" s="46">
+        <f t="shared" si="2"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A95" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B95" s="19"/>
       <c r="C95" s="19"/>
@@ -4613,19 +4628,19 @@
         <v>21</v>
       </c>
       <c r="F95" s="20">
-        <v>0</v>
-      </c>
-      <c r="G95" s="21">
-        <v>0.2</v>
-      </c>
-      <c r="H95" s="44">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
+        <v>3</v>
+      </c>
+      <c r="G95" s="39">
+        <v>1.2</v>
+      </c>
+      <c r="H95" s="45">
+        <f t="shared" si="2"/>
+        <v>3.5999999999999996</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A96" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B96" s="19"/>
       <c r="C96" s="19"/>
@@ -4634,54 +4649,47 @@
         <v>21</v>
       </c>
       <c r="F96" s="20">
-        <v>10</v>
-      </c>
-      <c r="G96" s="43">
-        <v>1</v>
-      </c>
-      <c r="H96" s="46">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="I96" s="41"/>
+        <v>0</v>
+      </c>
+      <c r="G96" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="H96" s="44">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="97" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A97" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="B97" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="C97" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="D97" s="19" t="s">
-        <v>183</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="B97" s="19"/>
+      <c r="C97" s="19"/>
+      <c r="D97" s="19"/>
       <c r="E97" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F97" s="20">
-        <v>104</v>
+        <v>10</v>
       </c>
       <c r="G97" s="43">
-        <v>3.45</v>
+        <v>1</v>
       </c>
       <c r="H97" s="46">
-        <f>F97*G97</f>
-        <v>358.8</v>
-      </c>
-      <c r="I97" s="42"/>
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="I97" s="41"/>
     </row>
     <row r="98" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A98" s="18" t="s">
-        <v>95</v>
+        <v>190</v>
       </c>
       <c r="B98" s="19" t="s">
         <v>182</v>
       </c>
       <c r="C98" s="19" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D98" s="19" t="s">
         <v>183</v>
@@ -4690,26 +4698,26 @@
         <v>21</v>
       </c>
       <c r="F98" s="20">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="G98" s="43">
-        <v>2.9</v>
+        <v>3.45</v>
       </c>
       <c r="H98" s="46">
-        <f t="shared" si="2"/>
-        <v>284.2</v>
+        <f>F98*G98</f>
+        <v>358.8</v>
       </c>
       <c r="I98" s="42"/>
     </row>
     <row r="99" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A99" s="18" t="s">
-        <v>225</v>
+        <v>95</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>227</v>
+        <v>182</v>
       </c>
       <c r="C99" s="19" t="s">
-        <v>226</v>
+        <v>180</v>
       </c>
       <c r="D99" s="19" t="s">
         <v>183</v>
@@ -4718,26 +4726,26 @@
         <v>21</v>
       </c>
       <c r="F99" s="20">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="G99" s="43">
-        <v>4.8</v>
+        <v>2.9</v>
       </c>
       <c r="H99" s="46">
         <f t="shared" si="2"/>
-        <v>182.4</v>
+        <v>284.2</v>
       </c>
       <c r="I99" s="42"/>
     </row>
     <row r="100" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A100" s="18" t="s">
-        <v>96</v>
+        <v>224</v>
       </c>
       <c r="B100" s="19" t="s">
-        <v>182</v>
+        <v>226</v>
       </c>
       <c r="C100" s="19" t="s">
-        <v>180</v>
+        <v>225</v>
       </c>
       <c r="D100" s="19" t="s">
         <v>183</v>
@@ -4746,20 +4754,20 @@
         <v>21</v>
       </c>
       <c r="F100" s="20">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="G100" s="43">
-        <v>3.45</v>
+        <v>4.8</v>
       </c>
       <c r="H100" s="46">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>182.4</v>
       </c>
       <c r="I100" s="42"/>
     </row>
     <row r="101" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A101" s="18" t="s">
-        <v>189</v>
+        <v>96</v>
       </c>
       <c r="B101" s="19" t="s">
         <v>182</v>
@@ -4774,388 +4782,389 @@
         <v>21</v>
       </c>
       <c r="F101" s="20">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="G101" s="43">
-        <v>3.75</v>
+        <v>3.45</v>
       </c>
       <c r="H101" s="46">
         <f t="shared" si="2"/>
-        <v>183.75</v>
+        <v>0</v>
       </c>
       <c r="I101" s="42"/>
     </row>
     <row r="102" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A102" s="18" t="s">
-        <v>97</v>
+        <v>189</v>
       </c>
       <c r="B102" s="19" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C102" s="19" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="D102" s="19" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="E102" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F102" s="20">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="G102" s="43">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="H102" s="46">
         <f t="shared" si="2"/>
-        <v>48</v>
+        <v>183.75</v>
       </c>
       <c r="I102" s="42"/>
     </row>
     <row r="103" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A103" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B103" s="19" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C103" s="19" t="s">
         <v>170</v>
       </c>
       <c r="D103" s="19" t="s">
-        <v>28</v>
+        <v>200</v>
       </c>
       <c r="E103" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F103" s="20">
+        <v>12</v>
+      </c>
+      <c r="G103" s="43">
+        <v>4</v>
+      </c>
+      <c r="H103" s="46">
+        <f t="shared" si="2"/>
         <v>48</v>
-      </c>
-      <c r="G103" s="43">
-        <v>0.8</v>
-      </c>
-      <c r="H103" s="46">
-        <f t="shared" si="2"/>
-        <v>38.400000000000006</v>
       </c>
       <c r="I103" s="42"/>
     </row>
     <row r="104" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A104" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B104" s="19" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C104" s="19" t="s">
-        <v>197</v>
+        <v>170</v>
       </c>
       <c r="D104" s="19" t="s">
-        <v>196</v>
+        <v>28</v>
       </c>
       <c r="E104" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F104" s="20">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="G104" s="43">
-        <v>11.7</v>
+        <v>0.8</v>
       </c>
       <c r="H104" s="46">
         <f t="shared" si="2"/>
-        <v>117</v>
-      </c>
+        <v>38.400000000000006</v>
+      </c>
+      <c r="I104" s="42"/>
     </row>
     <row r="105" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A105" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="B105" s="19"/>
-      <c r="C105" s="19"/>
+        <v>99</v>
+      </c>
+      <c r="B105" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="C105" s="19" t="s">
+        <v>197</v>
+      </c>
       <c r="D105" s="19" t="s">
-        <v>15</v>
+        <v>196</v>
       </c>
       <c r="E105" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F105" s="20">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="G105" s="43">
-        <v>2.4</v>
+        <v>11.7</v>
       </c>
       <c r="H105" s="46">
         <f t="shared" si="2"/>
-        <v>408</v>
+        <v>117</v>
       </c>
     </row>
     <row r="106" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A106" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="B106" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="C106" s="19" t="s">
-        <v>195</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="B106" s="19"/>
+      <c r="C106" s="19"/>
       <c r="D106" s="19" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="E106" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F106" s="20">
-        <v>30</v>
-      </c>
-      <c r="G106" s="21">
-        <v>0.83</v>
-      </c>
-      <c r="H106" s="45">
-        <f t="shared" si="2"/>
-        <v>24.9</v>
+        <v>170</v>
+      </c>
+      <c r="G106" s="43">
+        <v>2.4</v>
+      </c>
+      <c r="H106" s="46">
+        <f t="shared" si="2"/>
+        <v>408</v>
       </c>
     </row>
     <row r="107" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A107" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B107" s="19" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
       <c r="C107" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="D107" s="19"/>
+        <v>195</v>
+      </c>
+      <c r="D107" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E107" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F107" s="20">
-        <v>139</v>
+        <v>30</v>
       </c>
       <c r="G107" s="21">
-        <v>4.7</v>
-      </c>
-      <c r="H107" s="14">
-        <f t="shared" si="2"/>
-        <v>653.30000000000007</v>
+        <v>0.83</v>
+      </c>
+      <c r="H107" s="45">
+        <f t="shared" si="2"/>
+        <v>24.9</v>
       </c>
     </row>
     <row r="108" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A108" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B108" s="19" t="s">
-        <v>178</v>
+        <v>217</v>
       </c>
       <c r="C108" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="D108" s="19" t="s">
-        <v>156</v>
-      </c>
+      <c r="D108" s="19"/>
       <c r="E108" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F108" s="20">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="G108" s="21">
-        <v>2.5</v>
+        <v>4.7</v>
       </c>
       <c r="H108" s="14">
         <f t="shared" si="2"/>
-        <v>262.5</v>
+        <v>653.30000000000007</v>
       </c>
     </row>
     <row r="109" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A109" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="B109" s="19"/>
-      <c r="C109" s="19"/>
-      <c r="D109" s="34"/>
+        <v>103</v>
+      </c>
+      <c r="B109" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="C109" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="D109" s="19" t="s">
+        <v>156</v>
+      </c>
       <c r="E109" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F109" s="20">
-        <v>6</v>
+        <v>105</v>
       </c>
       <c r="G109" s="21">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="H109" s="14">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>262.5</v>
       </c>
     </row>
     <row r="110" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A110" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B110" s="19"/>
       <c r="C110" s="19"/>
-      <c r="D110" s="19"/>
+      <c r="D110" s="34"/>
       <c r="E110" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F110" s="20">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="G110" s="21">
         <v>2</v>
       </c>
       <c r="H110" s="14">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="111" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A111" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="B111" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="C111" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="D111" s="19" t="s">
-        <v>173</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B111" s="19"/>
+      <c r="C111" s="19"/>
+      <c r="D111" s="19"/>
       <c r="E111" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F111" s="20">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="G111" s="21">
-        <v>41.34</v>
+        <v>2</v>
       </c>
       <c r="H111" s="14">
         <f t="shared" si="2"/>
-        <v>289.38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A112" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="B112" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C112" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="D112" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="E112" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F112" s="20">
+        <v>7</v>
+      </c>
+      <c r="G112" s="21">
+        <v>41.34</v>
+      </c>
+      <c r="H112" s="14">
+        <f t="shared" si="2"/>
+        <v>289.38</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A113" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B112" s="19" t="s">
+      <c r="B113" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="C112" s="19" t="s">
+      <c r="C113" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="D112" s="19" t="s">
+      <c r="D113" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="E112" s="19" t="s">
+      <c r="E113" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F112" s="20">
+      <c r="F113" s="20">
         <v>30</v>
       </c>
-      <c r="G112" s="21">
+      <c r="G113" s="21">
         <v>2.7</v>
       </c>
-      <c r="H112" s="14">
+      <c r="H113" s="14">
         <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
-    <row r="113" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A113" s="23" t="s">
+    <row r="114" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A114" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="B113" s="29">
+      <c r="B114" s="29">
         <v>43140</v>
       </c>
-      <c r="C113" s="11">
+      <c r="C114" s="11">
         <v>36</v>
       </c>
-      <c r="D113" s="11" t="s">
+      <c r="D114" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="E113" s="11" t="s">
+      <c r="E114" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="F113" s="24">
+      <c r="F114" s="24">
         <v>15</v>
       </c>
-      <c r="G113" s="14">
+      <c r="G114" s="14">
         <v>6</v>
       </c>
-      <c r="H113" s="14">
+      <c r="H114" s="14">
         <f t="shared" si="2"/>
         <v>90</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A114" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="B114" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="C114" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="D114" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="E114" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F114" s="20">
-        <v>901</v>
-      </c>
-      <c r="G114" s="21">
-        <v>0.66</v>
-      </c>
-      <c r="H114" s="14">
-        <f t="shared" si="2"/>
-        <v>594.66000000000008</v>
       </c>
     </row>
     <row r="115" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A115" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B115" s="19" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="C115" s="19" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="D115" s="19" t="s">
-        <v>28</v>
+        <v>186</v>
       </c>
       <c r="E115" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F115" s="20">
-        <v>5</v>
+        <v>901</v>
       </c>
       <c r="G115" s="21">
-        <v>2.85</v>
+        <v>0.66</v>
       </c>
       <c r="H115" s="14">
         <f t="shared" si="2"/>
-        <v>14.25</v>
+        <v>594.66000000000008</v>
       </c>
     </row>
     <row r="116" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A116" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>210</v>
+        <v>168</v>
       </c>
       <c r="C116" s="19" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="D116" s="19" t="s">
         <v>28</v>
@@ -5164,50 +5173,52 @@
         <v>21</v>
       </c>
       <c r="F116" s="20">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G116" s="21">
-        <v>1.72</v>
+        <v>2.85</v>
       </c>
       <c r="H116" s="14">
         <f t="shared" si="2"/>
-        <v>12.04</v>
+        <v>14.25</v>
       </c>
     </row>
     <row r="117" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A117" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B117" s="19" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="C117" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="D117" s="19"/>
+        <v>181</v>
+      </c>
+      <c r="D117" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E117" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F117" s="20">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G117" s="21">
-        <v>2.9</v>
+        <v>1.72</v>
       </c>
       <c r="H117" s="14">
         <f t="shared" si="2"/>
-        <v>17.399999999999999</v>
+        <v>12.04</v>
       </c>
     </row>
     <row r="118" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A118" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B118" s="19" t="s">
-        <v>192</v>
+        <v>237</v>
       </c>
       <c r="C118" s="19" t="s">
-        <v>179</v>
+        <v>238</v>
       </c>
       <c r="D118" s="19" t="s">
         <v>28</v>
@@ -5216,94 +5227,94 @@
         <v>21</v>
       </c>
       <c r="F118" s="20">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G118" s="21">
-        <v>1.72</v>
+        <v>2.9</v>
       </c>
       <c r="H118" s="14">
         <f t="shared" si="2"/>
-        <v>5.16</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="119" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A119" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="B119" s="19"/>
-      <c r="C119" s="19"/>
-      <c r="D119" s="35"/>
+        <v>113</v>
+      </c>
+      <c r="B119" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="C119" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="D119" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E119" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F119" s="20">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G119" s="21">
-        <v>5</v>
+        <v>1.72</v>
       </c>
       <c r="H119" s="14">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>5.16</v>
       </c>
     </row>
     <row r="120" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A120" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B120" s="19"/>
       <c r="C120" s="19"/>
-      <c r="D120" s="19"/>
+      <c r="D120" s="35"/>
       <c r="E120" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F120" s="20">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G120" s="21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H120" s="14">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="121" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A121" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="B121" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="C121" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="D121" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B121" s="19"/>
+      <c r="C121" s="19"/>
+      <c r="D121" s="19"/>
+      <c r="E121" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F121" s="20">
         <v>9</v>
       </c>
-      <c r="E121" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F121" s="20">
-        <v>169</v>
-      </c>
       <c r="G121" s="21">
-        <v>2.69</v>
+        <v>1</v>
       </c>
       <c r="H121" s="14">
         <f t="shared" si="2"/>
-        <v>454.61</v>
+        <v>9</v>
       </c>
     </row>
     <row r="122" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A122" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B122" s="19" t="s">
         <v>172</v>
       </c>
       <c r="C122" s="19" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D122" s="19" t="s">
         <v>9</v>
@@ -5312,88 +5323,94 @@
         <v>12</v>
       </c>
       <c r="F122" s="20">
-        <v>113</v>
+        <v>169</v>
       </c>
       <c r="G122" s="21">
-        <v>3.3</v>
+        <v>2.69</v>
       </c>
       <c r="H122" s="14">
         <f t="shared" si="2"/>
-        <v>372.9</v>
+        <v>454.61</v>
       </c>
     </row>
     <row r="123" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A123" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="B123" s="19"/>
-      <c r="C123" s="19"/>
-      <c r="D123" s="19"/>
+        <v>117</v>
+      </c>
+      <c r="B123" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C123" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="D123" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="E123" s="19" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F123" s="20">
-        <v>5</v>
+        <v>113</v>
       </c>
       <c r="G123" s="21">
-        <v>2.87</v>
+        <v>3.3</v>
       </c>
       <c r="H123" s="14">
         <f t="shared" si="2"/>
-        <v>14.350000000000001</v>
+        <v>372.9</v>
       </c>
     </row>
     <row r="124" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A124" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B124" s="19"/>
+      <c r="C124" s="19"/>
+      <c r="D124" s="19"/>
+      <c r="E124" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F124" s="20">
+        <v>5</v>
+      </c>
+      <c r="G124" s="21">
+        <v>2.87</v>
+      </c>
+      <c r="H124" s="14">
+        <f t="shared" si="2"/>
+        <v>14.350000000000001</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A125" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="B124" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="C124" s="19" t="s">
+      <c r="B125" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="C125" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="D124" s="19" t="s">
+      <c r="D125" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="E124" s="19" t="s">
+      <c r="E125" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="F124" s="20">
+      <c r="F125" s="20">
         <v>6</v>
       </c>
-      <c r="G124" s="21">
+      <c r="G125" s="21">
         <v>7</v>
       </c>
-      <c r="H124" s="14">
+      <c r="H125" s="14">
         <f t="shared" si="2"/>
         <v>42</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" s="36" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A125" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="B125" s="19"/>
-      <c r="C125" s="19"/>
-      <c r="D125" s="19"/>
-      <c r="E125" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F125" s="20">
-        <v>582</v>
-      </c>
-      <c r="G125" s="21">
-        <v>3</v>
-      </c>
-      <c r="H125" s="14">
-        <f t="shared" si="2"/>
-        <v>1746</v>
       </c>
     </row>
     <row r="126" spans="1:8" s="36" customFormat="1" ht="28.35" customHeight="1">
       <c r="A126" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B126" s="19"/>
       <c r="C126" s="19"/>
@@ -5402,94 +5419,88 @@
         <v>21</v>
       </c>
       <c r="F126" s="20">
+        <v>582</v>
+      </c>
+      <c r="G126" s="21">
+        <v>3</v>
+      </c>
+      <c r="H126" s="14">
+        <f t="shared" si="2"/>
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" s="36" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A127" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B127" s="19"/>
+      <c r="C127" s="19"/>
+      <c r="D127" s="19"/>
+      <c r="E127" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F127" s="20">
         <v>1</v>
       </c>
-      <c r="G126" s="21">
+      <c r="G127" s="21">
         <v>1.96</v>
       </c>
-      <c r="H126" s="14">
+      <c r="H127" s="14">
         <f t="shared" si="2"/>
         <v>1.96</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="28.35" customHeight="1">
-      <c r="A127" s="23" t="s">
+    <row r="128" spans="1:8" ht="28.35" customHeight="1">
+      <c r="A128" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="B127" s="11"/>
-      <c r="C127" s="11"/>
-      <c r="D127" s="11"/>
-      <c r="E127" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F127" s="24">
-        <v>7</v>
-      </c>
-      <c r="G127" s="25">
-        <v>1.97</v>
-      </c>
-      <c r="H127" s="14">
-        <f t="shared" si="2"/>
-        <v>13.79</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" ht="28.35" customHeight="1">
-      <c r="A128" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="B128" s="19"/>
-      <c r="C128" s="19"/>
-      <c r="D128" s="19"/>
+      <c r="B128" s="11"/>
+      <c r="C128" s="11"/>
+      <c r="D128" s="11"/>
       <c r="E128" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F128" s="20">
-        <v>95</v>
-      </c>
-      <c r="G128" s="21">
+      <c r="F128" s="24">
         <v>7</v>
       </c>
+      <c r="G128" s="25">
+        <v>1.97</v>
+      </c>
       <c r="H128" s="14">
         <f t="shared" si="2"/>
-        <v>665</v>
+        <v>13.79</v>
       </c>
     </row>
     <row r="129" spans="1:255" ht="28.35" customHeight="1">
       <c r="A129" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="B129" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="C129" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="D129" s="19" t="s">
-        <v>13</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="B129" s="19"/>
+      <c r="C129" s="19"/>
+      <c r="D129" s="19"/>
       <c r="E129" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F129" s="20">
-        <v>250</v>
+        <v>95</v>
       </c>
       <c r="G129" s="21">
-        <v>2.69</v>
+        <v>7</v>
       </c>
       <c r="H129" s="14">
         <f t="shared" si="2"/>
-        <v>672.5</v>
+        <v>665</v>
       </c>
     </row>
     <row r="130" spans="1:255" ht="28.35" customHeight="1">
       <c r="A130" s="18" t="s">
-        <v>177</v>
+        <v>126</v>
       </c>
       <c r="B130" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C130" s="19" t="s">
         <v>220</v>
-      </c>
-      <c r="C130" s="19" t="s">
-        <v>222</v>
       </c>
       <c r="D130" s="19" t="s">
         <v>13</v>
@@ -5498,438 +5509,444 @@
         <v>12</v>
       </c>
       <c r="F130" s="20">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="G130" s="21">
-        <v>2.21</v>
+        <v>2.69</v>
       </c>
       <c r="H130" s="14">
         <f t="shared" si="2"/>
-        <v>331.5</v>
+        <v>672.5</v>
       </c>
     </row>
     <row r="131" spans="1:255" ht="28.35" customHeight="1">
-      <c r="A131" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="B131" s="11"/>
-      <c r="C131" s="11"/>
-      <c r="D131" s="11"/>
+      <c r="A131" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B131" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C131" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="D131" s="19" t="s">
+        <v>13</v>
+      </c>
       <c r="E131" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F131" s="24">
-        <v>100</v>
-      </c>
-      <c r="G131" s="25">
-        <v>1.43</v>
+      <c r="F131" s="20">
+        <v>150</v>
+      </c>
+      <c r="G131" s="21">
+        <v>2.21</v>
       </c>
       <c r="H131" s="14">
         <f t="shared" si="2"/>
-        <v>143</v>
+        <v>331.5</v>
       </c>
     </row>
     <row r="132" spans="1:255" ht="28.35" customHeight="1">
-      <c r="A132" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="B132" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="C132" s="19"/>
-      <c r="D132" s="19"/>
+      <c r="A132" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="B132" s="11"/>
+      <c r="C132" s="11"/>
+      <c r="D132" s="11"/>
       <c r="E132" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F132" s="20">
-        <v>4</v>
-      </c>
-      <c r="G132" s="21">
-        <v>8.5</v>
+      <c r="F132" s="24">
+        <v>100</v>
+      </c>
+      <c r="G132" s="25">
+        <v>1.43</v>
       </c>
       <c r="H132" s="14">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>143</v>
       </c>
     </row>
     <row r="133" spans="1:255" ht="28.35" customHeight="1">
       <c r="A133" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="B133" s="19"/>
+        <v>128</v>
+      </c>
+      <c r="B133" s="19" t="s">
+        <v>229</v>
+      </c>
       <c r="C133" s="19"/>
       <c r="D133" s="19"/>
       <c r="E133" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F133" s="20">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="G133" s="21">
-        <v>5</v>
+        <v>8.5</v>
       </c>
       <c r="H133" s="14">
         <f t="shared" si="2"/>
-        <v>85</v>
+        <v>34</v>
       </c>
     </row>
     <row r="134" spans="1:255" ht="28.35" customHeight="1">
       <c r="A134" s="18" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="B134" s="19"/>
       <c r="C134" s="19"/>
-      <c r="D134" s="19" t="s">
-        <v>155</v>
-      </c>
+      <c r="D134" s="19"/>
       <c r="E134" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F134" s="20">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G134" s="21">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="H134" s="14">
         <f t="shared" si="2"/>
-        <v>564</v>
+        <v>85</v>
       </c>
     </row>
     <row r="135" spans="1:255" ht="28.35" customHeight="1">
-      <c r="A135" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="B135" s="11"/>
-      <c r="C135" s="11"/>
-      <c r="D135" s="11"/>
+      <c r="A135" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B135" s="19"/>
+      <c r="C135" s="19"/>
+      <c r="D135" s="19" t="s">
+        <v>155</v>
+      </c>
       <c r="E135" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F135" s="24">
+      <c r="F135" s="20">
+        <v>12</v>
+      </c>
+      <c r="G135" s="21">
+        <v>47</v>
+      </c>
+      <c r="H135" s="14">
+        <f t="shared" si="2"/>
+        <v>564</v>
+      </c>
+    </row>
+    <row r="136" spans="1:255" ht="28.35" customHeight="1">
+      <c r="A136" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="B136" s="11"/>
+      <c r="C136" s="11"/>
+      <c r="D136" s="11"/>
+      <c r="E136" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F136" s="24">
         <v>22</v>
       </c>
-      <c r="G135" s="25">
+      <c r="G136" s="25">
         <v>2.97</v>
       </c>
-      <c r="H135" s="14">
+      <c r="H136" s="14">
         <f t="shared" si="2"/>
         <v>65.34</v>
       </c>
     </row>
-    <row r="136" spans="1:255" ht="28.35" customHeight="1">
-      <c r="A136" s="18" t="s">
+    <row r="137" spans="1:255" ht="28.35" customHeight="1">
+      <c r="A137" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="B136" s="19"/>
-      <c r="C136" s="19"/>
-      <c r="D136" s="19"/>
-      <c r="E136" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F136" s="20">
+      <c r="B137" s="19"/>
+      <c r="C137" s="19"/>
+      <c r="D137" s="19"/>
+      <c r="E137" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F137" s="20">
         <v>140</v>
       </c>
-      <c r="G136" s="21">
+      <c r="G137" s="21">
         <v>1.1299999999999999</v>
       </c>
-      <c r="H136" s="14">
+      <c r="H137" s="14">
         <f t="shared" si="2"/>
         <v>158.19999999999999</v>
       </c>
-      <c r="I136"/>
-      <c r="J136"/>
-      <c r="K136"/>
-      <c r="L136"/>
-      <c r="M136"/>
-      <c r="N136"/>
-      <c r="O136"/>
-      <c r="P136"/>
-      <c r="Q136"/>
-      <c r="R136"/>
-      <c r="S136"/>
-      <c r="T136"/>
-      <c r="U136"/>
-      <c r="V136"/>
-      <c r="W136"/>
-      <c r="X136"/>
-      <c r="Y136"/>
-      <c r="Z136"/>
-      <c r="AA136"/>
-      <c r="AB136"/>
-      <c r="AC136"/>
-      <c r="AD136"/>
-      <c r="AE136"/>
-      <c r="AF136"/>
-      <c r="AG136"/>
-      <c r="AH136"/>
-      <c r="AI136"/>
-      <c r="AJ136"/>
-      <c r="AK136"/>
-      <c r="AL136"/>
-      <c r="AM136"/>
-      <c r="AN136"/>
-      <c r="AO136"/>
-      <c r="AP136"/>
-      <c r="AQ136"/>
-      <c r="AR136"/>
-      <c r="AS136"/>
-      <c r="AT136"/>
-      <c r="AU136"/>
-      <c r="AV136"/>
-      <c r="AW136"/>
-      <c r="AX136"/>
-      <c r="AY136"/>
-      <c r="AZ136"/>
-      <c r="BA136"/>
-      <c r="BB136"/>
-      <c r="BC136"/>
-      <c r="BD136"/>
-      <c r="BE136"/>
-      <c r="BF136"/>
-      <c r="BG136"/>
-      <c r="BH136"/>
-      <c r="BI136"/>
-      <c r="BJ136"/>
-      <c r="BK136"/>
-      <c r="BL136"/>
-      <c r="BM136"/>
-      <c r="BN136"/>
-      <c r="BO136"/>
-      <c r="BP136"/>
-      <c r="BQ136"/>
-      <c r="BR136"/>
-      <c r="BS136"/>
-      <c r="BT136"/>
-      <c r="BU136"/>
-      <c r="BV136"/>
-      <c r="BW136"/>
-      <c r="BX136"/>
-      <c r="BY136"/>
-      <c r="BZ136"/>
-      <c r="CA136"/>
-      <c r="CB136"/>
-      <c r="CC136"/>
-      <c r="CD136"/>
-      <c r="CE136"/>
-      <c r="CF136"/>
-      <c r="CG136"/>
-      <c r="CH136"/>
-      <c r="CI136"/>
-      <c r="CJ136"/>
-      <c r="CK136"/>
-      <c r="CL136"/>
-      <c r="CM136"/>
-      <c r="CN136"/>
-      <c r="CO136"/>
-      <c r="CP136"/>
-      <c r="CQ136"/>
-      <c r="CR136"/>
-      <c r="CS136"/>
-      <c r="CT136"/>
-      <c r="CU136"/>
-      <c r="CV136"/>
-      <c r="CW136"/>
-      <c r="CX136"/>
-      <c r="CY136"/>
-      <c r="CZ136"/>
-      <c r="DA136"/>
-      <c r="DB136"/>
-      <c r="DC136"/>
-      <c r="DD136"/>
-      <c r="DE136"/>
-      <c r="DF136"/>
-      <c r="DG136"/>
-      <c r="DH136"/>
-      <c r="DI136"/>
-      <c r="DJ136"/>
-      <c r="DK136"/>
-      <c r="DL136"/>
-      <c r="DM136"/>
-      <c r="DN136"/>
-      <c r="DO136"/>
-      <c r="DP136"/>
-      <c r="DQ136"/>
-      <c r="DR136"/>
-      <c r="DS136"/>
-      <c r="DT136"/>
-      <c r="DU136"/>
-      <c r="DV136"/>
-      <c r="DW136"/>
-      <c r="DX136"/>
-      <c r="DY136"/>
-      <c r="DZ136"/>
-      <c r="EA136"/>
-      <c r="EB136"/>
-      <c r="EC136"/>
-      <c r="ED136"/>
-      <c r="EE136"/>
-      <c r="EF136"/>
-      <c r="EG136"/>
-      <c r="EH136"/>
-      <c r="EI136"/>
-      <c r="EJ136"/>
-      <c r="EK136"/>
-      <c r="EL136"/>
-      <c r="EM136"/>
-      <c r="EN136"/>
-      <c r="EO136"/>
-      <c r="EP136"/>
-      <c r="EQ136"/>
-      <c r="ER136"/>
-      <c r="ES136"/>
-      <c r="ET136"/>
-      <c r="EU136"/>
-      <c r="EV136"/>
-      <c r="EW136"/>
-      <c r="EX136"/>
-      <c r="EY136"/>
-      <c r="EZ136"/>
-      <c r="FA136"/>
-      <c r="FB136"/>
-      <c r="FC136"/>
-      <c r="FD136"/>
-      <c r="FE136"/>
-      <c r="FF136"/>
-      <c r="FG136"/>
-      <c r="FH136"/>
-      <c r="FI136"/>
-      <c r="FJ136"/>
-      <c r="FK136"/>
-      <c r="FL136"/>
-      <c r="FM136"/>
-      <c r="FN136"/>
-      <c r="FO136"/>
-      <c r="FP136"/>
-      <c r="FQ136"/>
-      <c r="FR136"/>
-      <c r="FS136"/>
-      <c r="FT136"/>
-      <c r="FU136"/>
-      <c r="FV136"/>
-      <c r="FW136"/>
-      <c r="FX136"/>
-      <c r="FY136"/>
-      <c r="FZ136"/>
-      <c r="GA136"/>
-      <c r="GB136"/>
-      <c r="GC136"/>
-      <c r="GD136"/>
-      <c r="GE136"/>
-      <c r="GF136"/>
-      <c r="GG136"/>
-      <c r="GH136"/>
-      <c r="GI136"/>
-      <c r="GJ136"/>
-      <c r="GK136"/>
-      <c r="GL136"/>
-      <c r="GM136"/>
-      <c r="GN136"/>
-      <c r="GO136"/>
-      <c r="GP136"/>
-      <c r="GQ136"/>
-      <c r="GR136"/>
-      <c r="GS136"/>
-      <c r="GT136"/>
-      <c r="GU136"/>
-      <c r="GV136"/>
-      <c r="GW136"/>
-      <c r="GX136"/>
-      <c r="GY136"/>
-      <c r="GZ136"/>
-      <c r="HA136"/>
-      <c r="HB136"/>
-      <c r="HC136"/>
-      <c r="HD136"/>
-      <c r="HE136"/>
-      <c r="HF136"/>
-      <c r="HG136"/>
-      <c r="HH136"/>
-      <c r="HI136"/>
-      <c r="HJ136"/>
-      <c r="HK136"/>
-      <c r="HL136"/>
-      <c r="HM136"/>
-      <c r="HN136"/>
-      <c r="HO136"/>
-      <c r="HP136"/>
-      <c r="HQ136"/>
-      <c r="HR136"/>
-      <c r="HS136"/>
-      <c r="HT136"/>
-      <c r="HU136"/>
-      <c r="HV136"/>
-      <c r="HW136"/>
-      <c r="HX136"/>
-      <c r="HY136"/>
-      <c r="HZ136"/>
-      <c r="IA136"/>
-      <c r="IB136"/>
-      <c r="IC136"/>
-      <c r="ID136"/>
-      <c r="IE136"/>
-      <c r="IF136"/>
-      <c r="IG136"/>
-      <c r="IH136"/>
-      <c r="II136"/>
-      <c r="IJ136"/>
-      <c r="IK136"/>
-      <c r="IL136"/>
-      <c r="IM136"/>
-      <c r="IN136"/>
-      <c r="IO136"/>
-      <c r="IP136"/>
-      <c r="IQ136"/>
-      <c r="IR136"/>
-      <c r="IS136"/>
-      <c r="IT136"/>
-      <c r="IU136"/>
-    </row>
-    <row r="137" spans="1:255" ht="28.35" customHeight="1">
-      <c r="A137" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="B137" s="11"/>
-      <c r="C137" s="11"/>
-      <c r="D137" s="11"/>
-      <c r="E137" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F137" s="24">
-        <v>25</v>
-      </c>
-      <c r="G137" s="25">
-        <v>5</v>
-      </c>
-      <c r="H137" s="14">
-        <f t="shared" si="2"/>
-        <v>125</v>
-      </c>
+      <c r="I137"/>
+      <c r="J137"/>
+      <c r="K137"/>
+      <c r="L137"/>
+      <c r="M137"/>
+      <c r="N137"/>
+      <c r="O137"/>
+      <c r="P137"/>
+      <c r="Q137"/>
+      <c r="R137"/>
+      <c r="S137"/>
+      <c r="T137"/>
+      <c r="U137"/>
+      <c r="V137"/>
+      <c r="W137"/>
+      <c r="X137"/>
+      <c r="Y137"/>
+      <c r="Z137"/>
+      <c r="AA137"/>
+      <c r="AB137"/>
+      <c r="AC137"/>
+      <c r="AD137"/>
+      <c r="AE137"/>
+      <c r="AF137"/>
+      <c r="AG137"/>
+      <c r="AH137"/>
+      <c r="AI137"/>
+      <c r="AJ137"/>
+      <c r="AK137"/>
+      <c r="AL137"/>
+      <c r="AM137"/>
+      <c r="AN137"/>
+      <c r="AO137"/>
+      <c r="AP137"/>
+      <c r="AQ137"/>
+      <c r="AR137"/>
+      <c r="AS137"/>
+      <c r="AT137"/>
+      <c r="AU137"/>
+      <c r="AV137"/>
+      <c r="AW137"/>
+      <c r="AX137"/>
+      <c r="AY137"/>
+      <c r="AZ137"/>
+      <c r="BA137"/>
+      <c r="BB137"/>
+      <c r="BC137"/>
+      <c r="BD137"/>
+      <c r="BE137"/>
+      <c r="BF137"/>
+      <c r="BG137"/>
+      <c r="BH137"/>
+      <c r="BI137"/>
+      <c r="BJ137"/>
+      <c r="BK137"/>
+      <c r="BL137"/>
+      <c r="BM137"/>
+      <c r="BN137"/>
+      <c r="BO137"/>
+      <c r="BP137"/>
+      <c r="BQ137"/>
+      <c r="BR137"/>
+      <c r="BS137"/>
+      <c r="BT137"/>
+      <c r="BU137"/>
+      <c r="BV137"/>
+      <c r="BW137"/>
+      <c r="BX137"/>
+      <c r="BY137"/>
+      <c r="BZ137"/>
+      <c r="CA137"/>
+      <c r="CB137"/>
+      <c r="CC137"/>
+      <c r="CD137"/>
+      <c r="CE137"/>
+      <c r="CF137"/>
+      <c r="CG137"/>
+      <c r="CH137"/>
+      <c r="CI137"/>
+      <c r="CJ137"/>
+      <c r="CK137"/>
+      <c r="CL137"/>
+      <c r="CM137"/>
+      <c r="CN137"/>
+      <c r="CO137"/>
+      <c r="CP137"/>
+      <c r="CQ137"/>
+      <c r="CR137"/>
+      <c r="CS137"/>
+      <c r="CT137"/>
+      <c r="CU137"/>
+      <c r="CV137"/>
+      <c r="CW137"/>
+      <c r="CX137"/>
+      <c r="CY137"/>
+      <c r="CZ137"/>
+      <c r="DA137"/>
+      <c r="DB137"/>
+      <c r="DC137"/>
+      <c r="DD137"/>
+      <c r="DE137"/>
+      <c r="DF137"/>
+      <c r="DG137"/>
+      <c r="DH137"/>
+      <c r="DI137"/>
+      <c r="DJ137"/>
+      <c r="DK137"/>
+      <c r="DL137"/>
+      <c r="DM137"/>
+      <c r="DN137"/>
+      <c r="DO137"/>
+      <c r="DP137"/>
+      <c r="DQ137"/>
+      <c r="DR137"/>
+      <c r="DS137"/>
+      <c r="DT137"/>
+      <c r="DU137"/>
+      <c r="DV137"/>
+      <c r="DW137"/>
+      <c r="DX137"/>
+      <c r="DY137"/>
+      <c r="DZ137"/>
+      <c r="EA137"/>
+      <c r="EB137"/>
+      <c r="EC137"/>
+      <c r="ED137"/>
+      <c r="EE137"/>
+      <c r="EF137"/>
+      <c r="EG137"/>
+      <c r="EH137"/>
+      <c r="EI137"/>
+      <c r="EJ137"/>
+      <c r="EK137"/>
+      <c r="EL137"/>
+      <c r="EM137"/>
+      <c r="EN137"/>
+      <c r="EO137"/>
+      <c r="EP137"/>
+      <c r="EQ137"/>
+      <c r="ER137"/>
+      <c r="ES137"/>
+      <c r="ET137"/>
+      <c r="EU137"/>
+      <c r="EV137"/>
+      <c r="EW137"/>
+      <c r="EX137"/>
+      <c r="EY137"/>
+      <c r="EZ137"/>
+      <c r="FA137"/>
+      <c r="FB137"/>
+      <c r="FC137"/>
+      <c r="FD137"/>
+      <c r="FE137"/>
+      <c r="FF137"/>
+      <c r="FG137"/>
+      <c r="FH137"/>
+      <c r="FI137"/>
+      <c r="FJ137"/>
+      <c r="FK137"/>
+      <c r="FL137"/>
+      <c r="FM137"/>
+      <c r="FN137"/>
+      <c r="FO137"/>
+      <c r="FP137"/>
+      <c r="FQ137"/>
+      <c r="FR137"/>
+      <c r="FS137"/>
+      <c r="FT137"/>
+      <c r="FU137"/>
+      <c r="FV137"/>
+      <c r="FW137"/>
+      <c r="FX137"/>
+      <c r="FY137"/>
+      <c r="FZ137"/>
+      <c r="GA137"/>
+      <c r="GB137"/>
+      <c r="GC137"/>
+      <c r="GD137"/>
+      <c r="GE137"/>
+      <c r="GF137"/>
+      <c r="GG137"/>
+      <c r="GH137"/>
+      <c r="GI137"/>
+      <c r="GJ137"/>
+      <c r="GK137"/>
+      <c r="GL137"/>
+      <c r="GM137"/>
+      <c r="GN137"/>
+      <c r="GO137"/>
+      <c r="GP137"/>
+      <c r="GQ137"/>
+      <c r="GR137"/>
+      <c r="GS137"/>
+      <c r="GT137"/>
+      <c r="GU137"/>
+      <c r="GV137"/>
+      <c r="GW137"/>
+      <c r="GX137"/>
+      <c r="GY137"/>
+      <c r="GZ137"/>
+      <c r="HA137"/>
+      <c r="HB137"/>
+      <c r="HC137"/>
+      <c r="HD137"/>
+      <c r="HE137"/>
+      <c r="HF137"/>
+      <c r="HG137"/>
+      <c r="HH137"/>
+      <c r="HI137"/>
+      <c r="HJ137"/>
+      <c r="HK137"/>
+      <c r="HL137"/>
+      <c r="HM137"/>
+      <c r="HN137"/>
+      <c r="HO137"/>
+      <c r="HP137"/>
+      <c r="HQ137"/>
+      <c r="HR137"/>
+      <c r="HS137"/>
+      <c r="HT137"/>
+      <c r="HU137"/>
+      <c r="HV137"/>
+      <c r="HW137"/>
+      <c r="HX137"/>
+      <c r="HY137"/>
+      <c r="HZ137"/>
+      <c r="IA137"/>
+      <c r="IB137"/>
+      <c r="IC137"/>
+      <c r="ID137"/>
+      <c r="IE137"/>
+      <c r="IF137"/>
+      <c r="IG137"/>
+      <c r="IH137"/>
+      <c r="II137"/>
+      <c r="IJ137"/>
+      <c r="IK137"/>
+      <c r="IL137"/>
+      <c r="IM137"/>
+      <c r="IN137"/>
+      <c r="IO137"/>
+      <c r="IP137"/>
+      <c r="IQ137"/>
+      <c r="IR137"/>
+      <c r="IS137"/>
+      <c r="IT137"/>
+      <c r="IU137"/>
     </row>
     <row r="138" spans="1:255" ht="28.35" customHeight="1">
       <c r="A138" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B138" s="11"/>
       <c r="C138" s="11"/>
       <c r="D138" s="11"/>
       <c r="E138" s="11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F138" s="24">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="G138" s="25">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H138" s="14">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>125</v>
       </c>
     </row>
     <row r="139" spans="1:255" ht="28.35" customHeight="1">
       <c r="A139" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B139" s="11"/>
       <c r="C139" s="11"/>
@@ -5938,40 +5955,40 @@
         <v>21</v>
       </c>
       <c r="F139" s="24">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G139" s="25">
-        <v>1.36</v>
+        <v>12</v>
       </c>
       <c r="H139" s="14">
         <f t="shared" si="2"/>
-        <v>10.88</v>
+        <v>12</v>
       </c>
     </row>
     <row r="140" spans="1:255" ht="28.35" customHeight="1">
       <c r="A140" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="B140" s="29"/>
+        <v>134</v>
+      </c>
+      <c r="B140" s="11"/>
       <c r="C140" s="11"/>
       <c r="D140" s="11"/>
       <c r="E140" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F140" s="24">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="G140" s="25">
-        <v>2.2000000000000002</v>
+        <v>1.36</v>
       </c>
       <c r="H140" s="14">
         <f t="shared" si="2"/>
-        <v>48.400000000000006</v>
+        <v>10.88</v>
       </c>
     </row>
     <row r="141" spans="1:255" ht="28.35" customHeight="1">
       <c r="A141" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B141" s="29"/>
       <c r="C141" s="11"/>
@@ -5980,19 +5997,19 @@
         <v>21</v>
       </c>
       <c r="F141" s="24">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G141" s="25">
-        <v>5.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H141" s="14">
         <f t="shared" si="2"/>
-        <v>88</v>
+        <v>48.400000000000006</v>
       </c>
     </row>
     <row r="142" spans="1:255" ht="28.35" customHeight="1">
       <c r="A142" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B142" s="29"/>
       <c r="C142" s="11"/>
@@ -6001,61 +6018,61 @@
         <v>21</v>
       </c>
       <c r="F142" s="24">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="G142" s="25">
-        <v>0.4</v>
+        <v>5.5</v>
       </c>
       <c r="H142" s="14">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>88</v>
       </c>
     </row>
     <row r="143" spans="1:255" ht="28.35" customHeight="1">
       <c r="A143" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="B143" s="11"/>
+        <v>137</v>
+      </c>
+      <c r="B143" s="29"/>
       <c r="C143" s="11"/>
       <c r="D143" s="11"/>
       <c r="E143" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F143" s="24">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G143" s="25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H143" s="14">
         <f t="shared" si="2"/>
-        <v>3.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="144" spans="1:255" ht="28.35" customHeight="1">
       <c r="A144" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="B144" s="29"/>
+        <v>138</v>
+      </c>
+      <c r="B144" s="11"/>
       <c r="C144" s="11"/>
       <c r="D144" s="11"/>
       <c r="E144" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F144" s="24">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="G144" s="25">
-        <v>1.1000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="H144" s="14">
         <f t="shared" si="2"/>
-        <v>31.900000000000002</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="145" spans="1:8" ht="28.35" customHeight="1">
       <c r="A145" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B145" s="29"/>
       <c r="C145" s="11"/>
@@ -6064,19 +6081,19 @@
         <v>21</v>
       </c>
       <c r="F145" s="24">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="G145" s="25">
-        <v>0.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H145" s="14">
         <f t="shared" si="2"/>
-        <v>54</v>
+        <v>31.900000000000002</v>
       </c>
     </row>
     <row r="146" spans="1:8" ht="28.35" customHeight="1">
       <c r="A146" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B146" s="29"/>
       <c r="C146" s="11"/>
@@ -6085,19 +6102,19 @@
         <v>21</v>
       </c>
       <c r="F146" s="24">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="G146" s="25">
-        <v>2.85</v>
+        <v>0.9</v>
       </c>
       <c r="H146" s="14">
         <f t="shared" si="2"/>
-        <v>85.5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="147" spans="1:8" ht="28.35" customHeight="1">
       <c r="A147" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B147" s="29"/>
       <c r="C147" s="11"/>
@@ -6106,86 +6123,84 @@
         <v>21</v>
       </c>
       <c r="F147" s="24">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="G147" s="25">
-        <v>3.4</v>
+        <v>2.85</v>
       </c>
       <c r="H147" s="14">
         <f t="shared" si="2"/>
-        <v>30.599999999999998</v>
+        <v>85.5</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="28.35" customHeight="1">
       <c r="A148" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="B148" s="11"/>
+        <v>142</v>
+      </c>
+      <c r="B148" s="29"/>
       <c r="C148" s="11"/>
       <c r="D148" s="11"/>
       <c r="E148" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F148" s="24">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="G148" s="25">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="H148" s="14">
         <f t="shared" si="2"/>
-        <v>69</v>
+        <v>30.599999999999998</v>
       </c>
     </row>
     <row r="149" spans="1:8" ht="28.35" customHeight="1">
       <c r="A149" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="B149" s="29"/>
+        <v>143</v>
+      </c>
+      <c r="B149" s="11"/>
       <c r="C149" s="11"/>
-      <c r="D149" s="11" t="s">
-        <v>145</v>
-      </c>
+      <c r="D149" s="11"/>
       <c r="E149" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F149" s="24">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G149" s="25">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="H149" s="14">
         <f t="shared" si="2"/>
-        <v>357</v>
+        <v>69</v>
       </c>
     </row>
     <row r="150" spans="1:8" ht="28.35" customHeight="1">
       <c r="A150" s="23" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B150" s="29"/>
       <c r="C150" s="11"/>
       <c r="D150" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E150" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F150" s="24">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="G150" s="25">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H150" s="14">
         <f t="shared" si="2"/>
-        <v>1000</v>
+        <v>357</v>
       </c>
     </row>
     <row r="151" spans="1:8" ht="28.35" customHeight="1">
       <c r="A151" s="23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B151" s="29"/>
       <c r="C151" s="11"/>
@@ -6196,35 +6211,58 @@
         <v>21</v>
       </c>
       <c r="F151" s="24">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="G151" s="25">
         <v>10</v>
       </c>
       <c r="H151" s="14">
         <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" ht="28.35" customHeight="1">
+      <c r="A152" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="B152" s="29"/>
+      <c r="C152" s="11"/>
+      <c r="D152" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="E152" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F152" s="24">
+        <v>9</v>
+      </c>
+      <c r="G152" s="25">
+        <v>10</v>
+      </c>
+      <c r="H152" s="14">
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
     </row>
-    <row r="152" spans="1:8" ht="48.75" customHeight="1">
-      <c r="H152" s="47">
-        <f>SUM(H3:H151)</f>
-        <v>19145.202000000001</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" ht="29.1" customHeight="1"/>
-    <row r="154" spans="1:8" ht="30" customHeight="1"/>
+    <row r="153" spans="1:8" ht="48.75" customHeight="1">
+      <c r="H153" s="47">
+        <f>SUM(H3:H152)</f>
+        <v>19178.602000000003</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" ht="29.1" customHeight="1"/>
+    <row r="155" spans="1:8" ht="30" customHeight="1"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="F115:F117 F84 F26:F29 F23:F24">
+  <conditionalFormatting sqref="F116:F118 F85 F26:F29 F23:F24">
     <cfRule type="cellIs" dxfId="21" priority="2" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F30:F31 F40:F41 F87:F89">
+  <conditionalFormatting sqref="F30:F31 F40:F41 F88:F90">
     <cfRule type="cellIs" dxfId="20" priority="4" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>25</formula>
     </cfRule>
@@ -6254,7 +6292,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F49 F85:F86 F105 F90:F91">
+  <conditionalFormatting sqref="F49 F86:F87 F106 F91:F92">
     <cfRule type="cellIs" dxfId="14" priority="12" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>1</formula>
     </cfRule>
@@ -6264,67 +6302,67 @@
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F58 F73:F83">
+  <conditionalFormatting sqref="F58 F74:F84">
     <cfRule type="cellIs" dxfId="12" priority="14" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F62">
+  <conditionalFormatting sqref="F63">
     <cfRule type="cellIs" dxfId="11" priority="15" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F67">
+  <conditionalFormatting sqref="F68">
     <cfRule type="cellIs" dxfId="10" priority="16" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>35</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F68">
+  <conditionalFormatting sqref="F69">
     <cfRule type="cellIs" dxfId="9" priority="17" stopIfTrue="1" operator="lessThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F101 F96:F97">
+  <conditionalFormatting sqref="F102 F97:F98">
     <cfRule type="cellIs" dxfId="8" priority="24" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F118 F106">
+  <conditionalFormatting sqref="F119 F107">
     <cfRule type="cellIs" dxfId="7" priority="25" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>150</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F108:F111">
+  <conditionalFormatting sqref="F109:F112">
     <cfRule type="cellIs" dxfId="6" priority="28" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F104">
+  <conditionalFormatting sqref="F105">
     <cfRule type="cellIs" dxfId="5" priority="31" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F100">
+  <conditionalFormatting sqref="F101">
     <cfRule type="cellIs" dxfId="4" priority="33" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F98:F99">
+  <conditionalFormatting sqref="F99:F100">
     <cfRule type="cellIs" dxfId="3" priority="34" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F95">
+  <conditionalFormatting sqref="F96">
     <cfRule type="cellIs" dxfId="2" priority="36" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F93:F94">
+  <conditionalFormatting sqref="F94:F95">
     <cfRule type="cellIs" dxfId="1" priority="38" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F97">
+  <conditionalFormatting sqref="F98">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>10</formula>
     </cfRule>

</xml_diff>

<commit_message>
new new 15 maggio
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="238">
   <si>
     <t>PRODOTTO</t>
   </si>
@@ -614,12 +614,6 @@
     <t>8</t>
   </si>
   <si>
-    <t>31/1/2018</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -656,12 +650,6 @@
     <t>12//3/2018</t>
   </si>
   <si>
-    <t>15/3/2018</t>
-  </si>
-  <si>
-    <t>175</t>
-  </si>
-  <si>
     <t>27/3/2018</t>
   </si>
   <si>
@@ -738,6 +726,12 @@
   </si>
   <si>
     <t>130</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>150</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1108,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="7" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
@@ -1246,6 +1240,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1906,8 +1906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IU155"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -2089,7 +2089,7 @@
     </row>
     <row r="5" spans="1:35" ht="24.95" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -2137,7 +2137,7 @@
     </row>
     <row r="6" spans="1:35" ht="24.2" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
@@ -2185,7 +2185,7 @@
     </row>
     <row r="7" spans="1:35" ht="25.35" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="16"/>
@@ -2300,14 +2300,14 @@
         <v>12</v>
       </c>
       <c r="F9" s="17">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="G9" s="13">
         <v>3</v>
       </c>
       <c r="H9" s="14">
         <f t="shared" si="0"/>
-        <v>84</v>
+        <v>30</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -2339,7 +2339,7 @@
     </row>
     <row r="10" spans="1:35" ht="28.35" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B10" s="10">
         <v>43174</v>
@@ -2354,14 +2354,14 @@
         <v>12</v>
       </c>
       <c r="F10" s="17">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G10" s="13">
         <v>2.35</v>
       </c>
       <c r="H10" s="14">
         <f t="shared" si="0"/>
-        <v>117.5</v>
+        <v>115.15</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -2448,7 +2448,7 @@
       <c r="B12" s="10"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>151</v>
@@ -2493,12 +2493,12 @@
     </row>
     <row r="13" spans="1:35" ht="28.35" customHeight="1">
       <c r="A13" s="15" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>151</v>
@@ -2543,12 +2543,12 @@
     </row>
     <row r="14" spans="1:35" ht="28.35" customHeight="1">
       <c r="A14" s="15" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E14" s="16" t="s">
         <v>151</v>
@@ -2593,12 +2593,12 @@
     </row>
     <row r="15" spans="1:35" ht="28.35" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E15" s="16" t="s">
         <v>151</v>
@@ -2643,12 +2643,12 @@
     </row>
     <row r="16" spans="1:35" ht="28.35" customHeight="1">
       <c r="A16" s="15" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>151</v>
@@ -2693,12 +2693,12 @@
     </row>
     <row r="17" spans="1:35" ht="27.75" customHeight="1">
       <c r="A17" s="15" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>151</v>
@@ -2945,55 +2945,55 @@
       <c r="AH21" s="8"/>
       <c r="AI21" s="8"/>
     </row>
-    <row r="22" spans="1:35" ht="28.35" customHeight="1">
-      <c r="A22" s="15" t="s">
+    <row r="22" spans="1:35" s="50" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A22" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16" t="s">
+      <c r="B22" s="29"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="12">
         <v>5</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="21">
         <v>2</v>
       </c>
       <c r="H22" s="14">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
-      <c r="T22" s="8"/>
-      <c r="U22" s="8"/>
-      <c r="V22" s="8"/>
-      <c r="W22" s="8"/>
-      <c r="X22" s="8"/>
-      <c r="Y22" s="8"/>
-      <c r="Z22" s="8"/>
-      <c r="AA22" s="8"/>
-      <c r="AB22" s="8"/>
-      <c r="AC22" s="8"/>
-      <c r="AD22" s="8"/>
-      <c r="AE22" s="8"/>
-      <c r="AF22" s="8"/>
-      <c r="AG22" s="8"/>
-      <c r="AH22" s="8"/>
-      <c r="AI22" s="8"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="49"/>
+      <c r="O22" s="49"/>
+      <c r="P22" s="49"/>
+      <c r="Q22" s="49"/>
+      <c r="R22" s="49"/>
+      <c r="S22" s="49"/>
+      <c r="T22" s="49"/>
+      <c r="U22" s="49"/>
+      <c r="V22" s="49"/>
+      <c r="W22" s="49"/>
+      <c r="X22" s="49"/>
+      <c r="Y22" s="49"/>
+      <c r="Z22" s="49"/>
+      <c r="AA22" s="49"/>
+      <c r="AB22" s="49"/>
+      <c r="AC22" s="49"/>
+      <c r="AD22" s="49"/>
+      <c r="AE22" s="49"/>
+      <c r="AF22" s="49"/>
+      <c r="AG22" s="49"/>
+      <c r="AH22" s="49"/>
+      <c r="AI22" s="49"/>
     </row>
     <row r="23" spans="1:35" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A23" s="18" t="s">
@@ -3027,10 +3027,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D24" s="19"/>
       <c r="E24" s="19" t="s">
@@ -3092,10 +3092,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>28</v>
@@ -3119,10 +3119,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="19" t="s">
@@ -3144,7 +3144,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C29" s="19" t="s">
         <v>171</v>
@@ -3192,10 +3192,10 @@
         <v>31</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>28</v>
@@ -3240,10 +3240,10 @@
         <v>33</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>212</v>
+        <v>233</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="D33" s="19" t="s">
         <v>173</v>
@@ -3252,14 +3252,14 @@
         <v>34</v>
       </c>
       <c r="F33" s="20">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="G33" s="21">
         <v>2.6</v>
       </c>
       <c r="H33" s="14">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3499,7 +3499,7 @@
       </c>
       <c r="B45" s="19"/>
       <c r="C45" s="19" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D45" s="19"/>
       <c r="E45" s="28" t="s">
@@ -3521,10 +3521,10 @@
         <v>46</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D46" s="19" t="s">
         <v>28</v>
@@ -3880,10 +3880,10 @@
     </row>
     <row r="62" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A62" s="18" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C62" s="19" t="s">
         <v>179</v>
@@ -3910,7 +3910,7 @@
         <v>63</v>
       </c>
       <c r="B63" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C63" s="19" t="s">
         <v>181</v>
@@ -4213,10 +4213,10 @@
     </row>
     <row r="77" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A77" s="18" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C77" s="19"/>
       <c r="D77" s="19" t="s">
@@ -4392,7 +4392,7 @@
         <v>82</v>
       </c>
       <c r="B85" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C85" s="19" t="s">
         <v>195</v>
@@ -4572,7 +4572,7 @@
         <v>90</v>
       </c>
       <c r="B93" s="19" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C93" s="19" t="s">
         <v>180</v>
@@ -4597,7 +4597,7 @@
         <v>91</v>
       </c>
       <c r="B94" s="19" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C94" s="19" t="s">
         <v>180</v>
@@ -4739,13 +4739,13 @@
     </row>
     <row r="100" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A100" s="18" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B100" s="19" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C100" s="19" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D100" s="19" t="s">
         <v>183</v>
@@ -4832,7 +4832,7 @@
         <v>170</v>
       </c>
       <c r="D103" s="19" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E103" s="19" t="s">
         <v>21</v>
@@ -4959,7 +4959,7 @@
         <v>102</v>
       </c>
       <c r="B108" s="19" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C108" s="19" t="s">
         <v>175</v>
@@ -4996,14 +4996,14 @@
         <v>21</v>
       </c>
       <c r="F109" s="20">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G109" s="21">
         <v>2.5</v>
       </c>
       <c r="H109" s="14">
         <f t="shared" si="2"/>
-        <v>262.5</v>
+        <v>260</v>
       </c>
     </row>
     <row r="110" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -5050,10 +5050,10 @@
     </row>
     <row r="112" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A112" s="18" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B112" s="19" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C112" s="19" t="s">
         <v>169</v>
@@ -5080,10 +5080,10 @@
         <v>106</v>
       </c>
       <c r="B113" s="19" t="s">
-        <v>198</v>
+        <v>233</v>
       </c>
       <c r="C113" s="19" t="s">
-        <v>199</v>
+        <v>237</v>
       </c>
       <c r="D113" s="19" t="s">
         <v>157</v>
@@ -5092,14 +5092,14 @@
         <v>34</v>
       </c>
       <c r="F113" s="20">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="G113" s="21">
         <v>2.7</v>
       </c>
       <c r="H113" s="14">
         <f t="shared" si="2"/>
-        <v>81</v>
+        <v>162</v>
       </c>
     </row>
     <row r="114" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -5118,7 +5118,7 @@
       <c r="E114" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="F114" s="24">
+      <c r="F114" s="12">
         <v>15</v>
       </c>
       <c r="G114" s="14">
@@ -5146,14 +5146,14 @@
         <v>21</v>
       </c>
       <c r="F115" s="20">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="G115" s="21">
         <v>0.66</v>
       </c>
       <c r="H115" s="14">
         <f t="shared" si="2"/>
-        <v>594.66000000000008</v>
+        <v>594</v>
       </c>
     </row>
     <row r="116" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -5188,7 +5188,7 @@
         <v>111</v>
       </c>
       <c r="B117" s="19" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C117" s="19" t="s">
         <v>181</v>
@@ -5215,10 +5215,10 @@
         <v>112</v>
       </c>
       <c r="B118" s="19" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C118" s="19" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D118" s="19" t="s">
         <v>28</v>
@@ -5386,7 +5386,7 @@
         <v>119</v>
       </c>
       <c r="B125" s="19" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C125" s="19" t="s">
         <v>170</v>
@@ -5497,10 +5497,10 @@
         <v>126</v>
       </c>
       <c r="B130" s="19" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C130" s="19" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D130" s="19" t="s">
         <v>13</v>
@@ -5524,10 +5524,10 @@
         <v>177</v>
       </c>
       <c r="B131" s="19" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C131" s="19" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D131" s="19" t="s">
         <v>13</v>
@@ -5572,7 +5572,7 @@
         <v>128</v>
       </c>
       <c r="B133" s="19" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C133" s="19"/>
       <c r="D133" s="19"/>
@@ -6247,7 +6247,7 @@
     <row r="153" spans="1:8" ht="48.75" customHeight="1">
       <c r="H153" s="47">
         <f>SUM(H3:H152)</f>
-        <v>19178.602000000003</v>
+        <v>19265.092000000001</v>
       </c>
     </row>
     <row r="154" spans="1:8" ht="29.1" customHeight="1"/>

</xml_diff>

<commit_message>
new new 16 maggio
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -10,15 +10,15 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$152</definedName>
-    <definedName name="Excel_BuiltIn_Print_Area" localSheetId="0">Sheet1!$A$1:$H$136</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$151</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area" localSheetId="0">Sheet1!$A$1:$H$135</definedName>
   </definedNames>
   <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="236">
   <si>
     <t>PRODOTTO</t>
   </si>
@@ -140,15 +140,9 @@
     <t>Cartellette leggere con alette</t>
   </si>
   <si>
-    <t>Cartuccia toner  per E260</t>
-  </si>
-  <si>
     <t>Cartuccia toner per sig Tiziana</t>
   </si>
   <si>
-    <t>Cartuccia toner segret. M310</t>
-  </si>
-  <si>
     <t>CD  700 MB  con logo</t>
   </si>
   <si>
@@ -584,9 +578,6 @@
     <t>5/2/2018</t>
   </si>
   <si>
-    <t>Lyreco</t>
-  </si>
-  <si>
     <t xml:space="preserve">Porta abiti sposa </t>
   </si>
   <si>
@@ -732,6 +723,9 @@
   </si>
   <si>
     <t>150</t>
+  </si>
+  <si>
+    <t>Cartuccia toner segret. M312</t>
   </si>
 </sst>
 </file>
@@ -1239,13 +1233,13 @@
     <xf numFmtId="165" fontId="21" fillId="13" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1306,15 +1300,7 @@
     <cellStyle name="Text" xfId="53"/>
     <cellStyle name="Warning" xfId="54"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="13"/>
-          <bgColor indexed="34"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="21">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1904,10 +1890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IU155"/>
+  <dimension ref="A1:IU154"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -1923,16 +1909,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="5" customFormat="1" ht="60.75" customHeight="1">
-      <c r="A1" s="48" t="s">
-        <v>164</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
+      <c r="A1" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:35" ht="29.1" customHeight="1">
       <c r="A2" s="6" t="s">
@@ -2089,11 +2075,13 @@
     </row>
     <row r="5" spans="1:35" ht="24.95" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
+      <c r="D5" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="E5" s="16" t="s">
         <v>12</v>
       </c>
@@ -2137,11 +2125,13 @@
     </row>
     <row r="6" spans="1:35" ht="24.2" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
+      <c r="D6" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="E6" s="16" t="s">
         <v>12</v>
       </c>
@@ -2185,12 +2175,12 @@
     </row>
     <row r="7" spans="1:35" ht="25.35" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="16"/>
-      <c r="D7" s="16" t="s">
-        <v>13</v>
+      <c r="D7" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>12</v>
@@ -2235,7 +2225,7 @@
     </row>
     <row r="8" spans="1:35" ht="23.25" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B8" s="10">
         <v>43174</v>
@@ -2243,8 +2233,8 @@
       <c r="C8" s="16">
         <v>50</v>
       </c>
-      <c r="D8" s="16" t="s">
-        <v>13</v>
+      <c r="D8" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>12</v>
@@ -2289,25 +2279,25 @@
     </row>
     <row r="9" spans="1:35" ht="23.25" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="16"/>
-      <c r="D9" s="16" t="s">
-        <v>13</v>
+      <c r="D9" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="17">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="G9" s="13">
         <v>3</v>
       </c>
       <c r="H9" s="14">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>141</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -2339,7 +2329,7 @@
     </row>
     <row r="10" spans="1:35" ht="28.35" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B10" s="10">
         <v>43174</v>
@@ -2347,8 +2337,8 @@
       <c r="C10" s="16">
         <v>50</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>13</v>
+      <c r="D10" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>12</v>
@@ -2393,15 +2383,15 @@
     </row>
     <row r="11" spans="1:35" ht="28.35" customHeight="1">
       <c r="A11" s="15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F11" s="17">
         <v>63</v>
@@ -2443,15 +2433,15 @@
     </row>
     <row r="12" spans="1:35" ht="28.35" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F12" s="17">
         <v>10</v>
@@ -2493,15 +2483,15 @@
     </row>
     <row r="13" spans="1:35" ht="28.35" customHeight="1">
       <c r="A13" s="15" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F13" s="17">
         <v>15</v>
@@ -2543,15 +2533,15 @@
     </row>
     <row r="14" spans="1:35" ht="28.35" customHeight="1">
       <c r="A14" s="15" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F14" s="17">
         <v>8</v>
@@ -2593,15 +2583,15 @@
     </row>
     <row r="15" spans="1:35" ht="28.35" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F15" s="17">
         <v>4</v>
@@ -2643,15 +2633,15 @@
     </row>
     <row r="16" spans="1:35" ht="28.35" customHeight="1">
       <c r="A16" s="15" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F16" s="17">
         <v>5</v>
@@ -2693,15 +2683,15 @@
     </row>
     <row r="17" spans="1:35" ht="27.75" customHeight="1">
       <c r="A17" s="15" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F17" s="17">
         <v>2</v>
@@ -2852,7 +2842,7 @@
         <v>5</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E20" s="16" t="s">
         <v>10</v>
@@ -2897,12 +2887,12 @@
     </row>
     <row r="21" spans="1:35" ht="28.35" customHeight="1">
       <c r="A21" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E21" s="16" t="s">
         <v>16</v>
@@ -2945,14 +2935,14 @@
       <c r="AH21" s="8"/>
       <c r="AI21" s="8"/>
     </row>
-    <row r="22" spans="1:35" s="50" customFormat="1" ht="28.35" customHeight="1">
+    <row r="22" spans="1:35" s="49" customFormat="1" ht="28.35" customHeight="1">
       <c r="A22" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="29"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>10</v>
@@ -2967,43 +2957,43 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="49"/>
-      <c r="P22" s="49"/>
-      <c r="Q22" s="49"/>
-      <c r="R22" s="49"/>
-      <c r="S22" s="49"/>
-      <c r="T22" s="49"/>
-      <c r="U22" s="49"/>
-      <c r="V22" s="49"/>
-      <c r="W22" s="49"/>
-      <c r="X22" s="49"/>
-      <c r="Y22" s="49"/>
-      <c r="Z22" s="49"/>
-      <c r="AA22" s="49"/>
-      <c r="AB22" s="49"/>
-      <c r="AC22" s="49"/>
-      <c r="AD22" s="49"/>
-      <c r="AE22" s="49"/>
-      <c r="AF22" s="49"/>
-      <c r="AG22" s="49"/>
-      <c r="AH22" s="49"/>
-      <c r="AI22" s="49"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="48"/>
+      <c r="S22" s="48"/>
+      <c r="T22" s="48"/>
+      <c r="U22" s="48"/>
+      <c r="V22" s="48"/>
+      <c r="W22" s="48"/>
+      <c r="X22" s="48"/>
+      <c r="Y22" s="48"/>
+      <c r="Z22" s="48"/>
+      <c r="AA22" s="48"/>
+      <c r="AB22" s="48"/>
+      <c r="AC22" s="48"/>
+      <c r="AD22" s="48"/>
+      <c r="AE22" s="48"/>
+      <c r="AF22" s="48"/>
+      <c r="AG22" s="48"/>
+      <c r="AH22" s="48"/>
+      <c r="AI22" s="48"/>
     </row>
     <row r="23" spans="1:35" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A23" s="18" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>28</v>
@@ -3018,7 +3008,7 @@
         <v>3</v>
       </c>
       <c r="H23" s="14">
-        <f t="shared" ref="H23:H72" si="1">F23*G23</f>
+        <f t="shared" ref="H23:H71" si="1">F23*G23</f>
         <v>6</v>
       </c>
     </row>
@@ -3027,10 +3017,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D24" s="19"/>
       <c r="E24" s="19" t="s">
@@ -3049,7 +3039,7 @@
     </row>
     <row r="25" spans="1:35" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A25" s="18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
@@ -3092,10 +3082,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>28</v>
@@ -3119,10 +3109,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="19" t="s">
@@ -3144,10 +3134,10 @@
         <v>29</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>28</v>
@@ -3192,10 +3182,10 @@
         <v>31</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>28</v>
@@ -3240,13 +3230,13 @@
         <v>33</v>
       </c>
       <c r="B33" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="C33" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="C33" s="19" t="s">
-        <v>236</v>
-      </c>
       <c r="D33" s="19" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E33" s="19" t="s">
         <v>34</v>
@@ -3268,7 +3258,9 @@
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
+      <c r="D34" s="19" t="s">
+        <v>171</v>
+      </c>
       <c r="E34" s="19" t="s">
         <v>10</v>
       </c>
@@ -3289,7 +3281,9 @@
       </c>
       <c r="B35" s="28"/>
       <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
+      <c r="D35" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E35" s="28" t="s">
         <v>21</v>
       </c>
@@ -3333,7 +3327,9 @@
       </c>
       <c r="B37" s="19"/>
       <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
+      <c r="D37" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E37" s="28" t="s">
         <v>21</v>
       </c>
@@ -3354,7 +3350,9 @@
       </c>
       <c r="B38" s="19"/>
       <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
+      <c r="D38" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E38" s="28" t="s">
         <v>21</v>
       </c>
@@ -3375,7 +3373,9 @@
       </c>
       <c r="B39" s="19"/>
       <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
+      <c r="D39" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E39" s="28" t="s">
         <v>21</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>0</v>
       </c>
       <c r="G39" s="21">
-        <v>85</v>
+        <v>177</v>
       </c>
       <c r="H39" s="14">
         <f t="shared" si="1"/>
@@ -3392,11 +3392,13 @@
     </row>
     <row r="40" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A40" s="18" t="s">
-        <v>41</v>
+        <v>235</v>
       </c>
       <c r="B40" s="19"/>
       <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
+      <c r="D40" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E40" s="28" t="s">
         <v>21</v>
       </c>
@@ -3404,7 +3406,7 @@
         <v>0</v>
       </c>
       <c r="G40" s="21">
-        <v>177</v>
+        <v>110</v>
       </c>
       <c r="H40" s="14">
         <f t="shared" si="1"/>
@@ -3413,7 +3415,7 @@
     </row>
     <row r="41" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A41" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="19"/>
       <c r="C41" s="19"/>
@@ -3422,19 +3424,19 @@
         <v>21</v>
       </c>
       <c r="F41" s="20">
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="G41" s="21">
-        <v>110</v>
+        <v>1.18</v>
       </c>
       <c r="H41" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>200.6</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A42" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" s="19"/>
       <c r="C42" s="19"/>
@@ -3443,89 +3445,93 @@
         <v>21</v>
       </c>
       <c r="F42" s="20">
-        <v>170</v>
+        <v>575</v>
       </c>
       <c r="G42" s="21">
-        <v>1.18</v>
+        <v>0.35</v>
       </c>
       <c r="H42" s="14">
         <f t="shared" si="1"/>
-        <v>200.6</v>
+        <v>201.25</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A43" s="18" t="s">
-        <v>44</v>
+        <v>151</v>
       </c>
       <c r="B43" s="19"/>
       <c r="C43" s="19"/>
       <c r="D43" s="19"/>
       <c r="E43" s="28" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F43" s="20">
-        <v>575</v>
-      </c>
-      <c r="G43" s="21">
-        <v>0.35</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="G43" s="21"/>
       <c r="H43" s="14">
         <f t="shared" si="1"/>
-        <v>201.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A44" s="18" t="s">
-        <v>153</v>
+        <v>43</v>
       </c>
       <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
+      <c r="C44" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E44" s="28" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F44" s="20">
-        <v>60</v>
-      </c>
-      <c r="G44" s="21"/>
+        <v>3</v>
+      </c>
+      <c r="G44" s="21">
+        <v>1</v>
+      </c>
       <c r="H44" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A45" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="19"/>
+        <v>44</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>198</v>
+      </c>
       <c r="C45" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="D45" s="19"/>
+        <v>197</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E45" s="28" t="s">
         <v>21</v>
       </c>
       <c r="F45" s="20">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="G45" s="21">
-        <v>1</v>
+        <v>1.75</v>
       </c>
       <c r="H45" s="14">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A46" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" s="19" t="s">
-        <v>201</v>
-      </c>
-      <c r="C46" s="19" t="s">
-        <v>200</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
       <c r="D46" s="19" t="s">
         <v>28</v>
       </c>
@@ -3533,35 +3539,37 @@
         <v>21</v>
       </c>
       <c r="F46" s="20">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G46" s="21">
-        <v>1.75</v>
+        <v>0.72</v>
       </c>
       <c r="H46" s="14">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A47" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47" s="19"/>
       <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
+      <c r="D47" s="19" t="s">
+        <v>47</v>
+      </c>
       <c r="E47" s="28" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F47" s="20">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="G47" s="21">
-        <v>0.72</v>
+        <v>3</v>
       </c>
       <c r="H47" s="14">
         <f t="shared" si="1"/>
-        <v>0.72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3570,26 +3578,24 @@
       </c>
       <c r="B48" s="19"/>
       <c r="C48" s="19"/>
-      <c r="D48" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E48" s="28" t="s">
+      <c r="D48" s="19"/>
+      <c r="E48" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F48" s="20">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G48" s="21">
-        <v>3</v>
+        <v>1.8</v>
       </c>
       <c r="H48" s="14">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A49" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49" s="19"/>
       <c r="C49" s="19"/>
@@ -3598,67 +3604,71 @@
         <v>12</v>
       </c>
       <c r="F49" s="20">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G49" s="21">
-        <v>1.8</v>
+        <v>1</v>
       </c>
       <c r="H49" s="14">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A50" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B50" s="19"/>
       <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19" t="s">
-        <v>12</v>
+      <c r="D50" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="F50" s="20">
-        <v>14</v>
+        <v>600</v>
       </c>
       <c r="G50" s="21">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="H50" s="14">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A51" s="18" t="s">
+      <c r="A51" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="19"/>
+      <c r="B51" s="11"/>
       <c r="C51" s="19"/>
       <c r="D51" s="19" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F51" s="20">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="G51" s="21">
-        <v>0.15</v>
+        <v>0.22</v>
       </c>
       <c r="H51" s="14">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A52" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B52" s="11"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E52" s="11" t="s">
         <v>21</v>
       </c>
@@ -3666,7 +3676,7 @@
         <v>0</v>
       </c>
       <c r="G52" s="21">
-        <v>0.22</v>
+        <v>2.13</v>
       </c>
       <c r="H52" s="14">
         <f t="shared" si="1"/>
@@ -3674,55 +3684,61 @@
       </c>
     </row>
     <row r="53" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A53" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
+      <c r="A53" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" s="19"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E53" s="11" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="F53" s="20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G53" s="21">
-        <v>2.13</v>
+        <v>5.95</v>
       </c>
       <c r="H53" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A54" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B54" s="19"/>
-      <c r="C54" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>167</v>
+      </c>
       <c r="D54" s="19" t="s">
         <v>28</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="F54" s="20">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G54" s="21">
-        <v>5.95</v>
+        <v>0.7</v>
       </c>
       <c r="H54" s="14">
         <f t="shared" si="1"/>
-        <v>11.9</v>
+        <v>4.1999999999999993</v>
       </c>
     </row>
     <row r="55" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A55" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="C55" s="19" t="s">
         <v>169</v>
@@ -3734,26 +3750,22 @@
         <v>21</v>
       </c>
       <c r="F55" s="20">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="G55" s="21">
-        <v>0.7</v>
+        <v>1.5</v>
       </c>
       <c r="H55" s="14">
         <f t="shared" si="1"/>
-        <v>4.1999999999999993</v>
+        <v>27</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A56" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B56" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="C56" s="19" t="s">
-        <v>171</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B56" s="19"/>
+      <c r="C56" s="19"/>
       <c r="D56" s="19" t="s">
         <v>28</v>
       </c>
@@ -3761,129 +3773,141 @@
         <v>21</v>
       </c>
       <c r="F56" s="20">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G56" s="21">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="H56" s="14">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A57" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B57" s="19"/>
       <c r="C57" s="19"/>
-      <c r="D57" s="19"/>
+      <c r="D57" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E57" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F57" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G57" s="21">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="H57" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="58" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A58" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B58" s="19"/>
       <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
+      <c r="D58" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E58" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F58" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G58" s="21">
-        <v>1.5</v>
+        <v>5.35</v>
       </c>
       <c r="H58" s="14">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A59" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B59" s="19"/>
       <c r="C59" s="19"/>
-      <c r="D59" s="19"/>
+      <c r="D59" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E59" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F59" s="20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G59" s="21">
-        <v>5.35</v>
+        <v>2</v>
       </c>
       <c r="H59" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A60" s="18" t="s">
-        <v>62</v>
+        <v>156</v>
       </c>
       <c r="B60" s="19"/>
       <c r="C60" s="19"/>
-      <c r="D60" s="19"/>
+      <c r="D60" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="E60" s="11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F60" s="20">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="G60" s="21">
-        <v>2</v>
+        <v>1.98</v>
       </c>
       <c r="H60" s="14">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>43.56</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A61" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="B61" s="19"/>
-      <c r="C61" s="19"/>
+        <v>229</v>
+      </c>
+      <c r="B61" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="C61" s="19" t="s">
+        <v>177</v>
+      </c>
       <c r="D61" s="19" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>12</v>
+        <v>149</v>
       </c>
       <c r="F61" s="20">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="G61" s="21">
-        <v>1.98</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="H61" s="14">
         <f t="shared" si="1"/>
-        <v>43.56</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A62" s="18" t="s">
-        <v>232</v>
+        <v>61</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>233</v>
+        <v>207</v>
       </c>
       <c r="C62" s="19" t="s">
         <v>179</v>
@@ -3892,202 +3916,198 @@
         <v>28</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>151</v>
+        <v>21</v>
       </c>
       <c r="F62" s="20">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G62" s="21">
-        <v>4.9000000000000004</v>
+        <v>0.44</v>
       </c>
       <c r="H62" s="14">
         <f t="shared" si="1"/>
-        <v>19.600000000000001</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A63" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B63" s="19" t="s">
-        <v>210</v>
-      </c>
-      <c r="C63" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="D63" s="19"/>
+      <c r="A63" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
       <c r="E63" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F63" s="20">
-        <v>7</v>
-      </c>
-      <c r="G63" s="21">
-        <v>0.44</v>
+        <v>12</v>
+      </c>
+      <c r="F63" s="24">
+        <v>11</v>
+      </c>
+      <c r="G63" s="25">
+        <v>4.8499999999999996</v>
       </c>
       <c r="H63" s="14">
         <f t="shared" si="1"/>
-        <v>3.08</v>
+        <v>53.349999999999994</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A64" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="B64" s="11"/>
+        <v>63</v>
+      </c>
+      <c r="B64" s="29"/>
       <c r="C64" s="11"/>
       <c r="D64" s="11"/>
       <c r="E64" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F64" s="24">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G64" s="25">
-        <v>4.8499999999999996</v>
+        <v>5.04</v>
       </c>
       <c r="H64" s="14">
         <f t="shared" si="1"/>
-        <v>53.349999999999994</v>
+        <v>151.19999999999999</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A65" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="B65" s="29"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
+      <c r="A65" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" s="19"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="19"/>
       <c r="E65" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F65" s="24">
-        <v>30</v>
-      </c>
-      <c r="G65" s="25">
-        <v>5.04</v>
+      <c r="F65" s="20">
+        <v>25</v>
+      </c>
+      <c r="G65" s="21">
+        <v>8.3000000000000007</v>
       </c>
       <c r="H65" s="14">
         <f t="shared" si="1"/>
-        <v>151.19999999999999</v>
+        <v>207.50000000000003</v>
       </c>
     </row>
     <row r="66" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A66" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B66" s="19"/>
       <c r="C66" s="19"/>
       <c r="D66" s="19"/>
-      <c r="E66" s="11" t="s">
+      <c r="E66" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F66" s="20">
         <v>12</v>
       </c>
-      <c r="F66" s="20">
-        <v>25</v>
-      </c>
       <c r="G66" s="21">
-        <v>8.3000000000000007</v>
+        <v>0.75</v>
       </c>
       <c r="H66" s="14">
         <f t="shared" si="1"/>
-        <v>207.50000000000003</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A67" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B67" s="19"/>
-      <c r="C67" s="19"/>
-      <c r="D67" s="19"/>
+        <v>66</v>
+      </c>
+      <c r="B67" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="D67" s="19" t="s">
+        <v>154</v>
+      </c>
       <c r="E67" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F67" s="20">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="G67" s="21">
-        <v>0.75</v>
+        <v>3</v>
       </c>
       <c r="H67" s="14">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>168</v>
       </c>
     </row>
     <row r="68" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A68" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B68" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="C68" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="D68" s="19" t="s">
-        <v>156</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="B68" s="19"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="19"/>
       <c r="E68" s="19" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F68" s="20">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="G68" s="21">
         <v>3</v>
       </c>
       <c r="H68" s="14">
         <f t="shared" si="1"/>
-        <v>168</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A69" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B69" s="19"/>
       <c r="C69" s="19"/>
-      <c r="D69" s="19"/>
+      <c r="D69" s="19" t="s">
+        <v>147</v>
+      </c>
       <c r="E69" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F69" s="20">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="G69" s="21">
         <v>3</v>
       </c>
       <c r="H69" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>105</v>
       </c>
     </row>
     <row r="70" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A70" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B70" s="19"/>
-      <c r="C70" s="19"/>
-      <c r="D70" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E70" s="19" t="s">
+      <c r="A70" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" s="31"/>
+      <c r="C70" s="31"/>
+      <c r="D70" s="31"/>
+      <c r="E70" s="31" t="s">
         <v>12</v>
       </c>
       <c r="F70" s="20">
-        <v>35</v>
-      </c>
-      <c r="G70" s="21">
+        <v>18</v>
+      </c>
+      <c r="G70" s="32">
         <v>3</v>
       </c>
-      <c r="H70" s="14">
+      <c r="H70" s="33">
         <f t="shared" si="1"/>
-        <v>105</v>
+        <v>54</v>
       </c>
     </row>
     <row r="71" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A71" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B71" s="31"/>
       <c r="C71" s="31"/>
@@ -4096,61 +4116,61 @@
         <v>12</v>
       </c>
       <c r="F71" s="20">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G71" s="32">
         <v>3</v>
       </c>
       <c r="H71" s="33">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>21</v>
       </c>
     </row>
     <row r="72" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A72" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="B72" s="31"/>
-      <c r="C72" s="31"/>
-      <c r="D72" s="31"/>
-      <c r="E72" s="31" t="s">
+      <c r="A72" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" s="19"/>
+      <c r="C72" s="19"/>
+      <c r="D72" s="19"/>
+      <c r="E72" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F72" s="20">
-        <v>7</v>
-      </c>
-      <c r="G72" s="32">
-        <v>3</v>
-      </c>
-      <c r="H72" s="33">
-        <f t="shared" si="1"/>
-        <v>21</v>
+        <v>43</v>
+      </c>
+      <c r="G72" s="21">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="H72" s="14">
+        <f t="shared" ref="H72:H151" si="2">F72*G72</f>
+        <v>210.70000000000002</v>
       </c>
     </row>
     <row r="73" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A73" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B73" s="19"/>
       <c r="C73" s="19"/>
       <c r="D73" s="19"/>
       <c r="E73" s="19" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F73" s="20">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="G73" s="21">
-        <v>4.9000000000000004</v>
+        <v>33.5</v>
       </c>
       <c r="H73" s="14">
-        <f t="shared" ref="H73:H152" si="2">F73*G73</f>
-        <v>210.70000000000002</v>
+        <f t="shared" si="2"/>
+        <v>2077</v>
       </c>
     </row>
     <row r="74" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A74" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B74" s="19"/>
       <c r="C74" s="19"/>
@@ -4159,19 +4179,19 @@
         <v>21</v>
       </c>
       <c r="F74" s="20">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="G74" s="21">
-        <v>33.5</v>
+        <v>2</v>
       </c>
       <c r="H74" s="14">
         <f t="shared" si="2"/>
-        <v>2077</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A75" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B75" s="19"/>
       <c r="C75" s="19"/>
@@ -4180,161 +4200,165 @@
         <v>21</v>
       </c>
       <c r="F75" s="20">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="G75" s="21">
-        <v>2</v>
+        <v>4.3</v>
       </c>
       <c r="H75" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>81.7</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A76" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B76" s="19"/>
+        <v>220</v>
+      </c>
+      <c r="B76" s="19" t="s">
+        <v>221</v>
+      </c>
       <c r="C76" s="19"/>
-      <c r="D76" s="19"/>
+      <c r="D76" s="19" t="s">
+        <v>47</v>
+      </c>
       <c r="E76" s="19" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F76" s="20">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G76" s="21">
-        <v>4.3</v>
+        <v>8.5</v>
       </c>
       <c r="H76" s="14">
         <f t="shared" si="2"/>
-        <v>81.7</v>
+        <v>204</v>
       </c>
     </row>
     <row r="77" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A77" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="B77" s="19" t="s">
-        <v>224</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B77" s="19"/>
       <c r="C77" s="19"/>
       <c r="D77" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E77" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F77" s="20">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="G77" s="21">
         <v>8.5</v>
       </c>
       <c r="H77" s="14">
         <f t="shared" si="2"/>
-        <v>204</v>
+        <v>102</v>
       </c>
     </row>
     <row r="78" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A78" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B78" s="19"/>
       <c r="C78" s="19"/>
       <c r="D78" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E78" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F78" s="20">
-        <v>12</v>
+        <v>1.5</v>
       </c>
       <c r="G78" s="21">
-        <v>8.5</v>
+        <v>5</v>
       </c>
       <c r="H78" s="14">
         <f t="shared" si="2"/>
-        <v>102</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A79" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79" s="19"/>
       <c r="C79" s="19"/>
       <c r="D79" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E79" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F79" s="20">
-        <v>1.5</v>
+        <v>20</v>
       </c>
       <c r="G79" s="21">
         <v>5</v>
       </c>
       <c r="H79" s="14">
         <f t="shared" si="2"/>
-        <v>7.5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A80" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80" s="19"/>
       <c r="C80" s="19"/>
-      <c r="D80" s="19"/>
+      <c r="D80" s="19" t="s">
+        <v>47</v>
+      </c>
       <c r="E80" s="19" t="s">
         <v>12</v>
       </c>
       <c r="F80" s="20">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="G80" s="21">
         <v>5</v>
       </c>
       <c r="H80" s="14">
         <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A81" s="18" t="s">
-        <v>80</v>
+        <v>148</v>
       </c>
       <c r="B81" s="19"/>
       <c r="C81" s="19"/>
-      <c r="D81" s="19"/>
+      <c r="D81" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="E81" s="19" t="s">
-        <v>12</v>
+        <v>149</v>
       </c>
       <c r="F81" s="20">
-        <v>3</v>
-      </c>
-      <c r="G81" s="21">
-        <v>5</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="G81" s="21"/>
       <c r="H81" s="14">
         <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A82" s="18" t="s">
         <v>150</v>
       </c>
       <c r="B82" s="19"/>
       <c r="C82" s="19"/>
       <c r="D82" s="19" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E82" s="19" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F82" s="20">
         <v>150</v>
@@ -4345,58 +4369,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+    <row r="83" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A83" s="18" t="s">
-        <v>152</v>
+        <v>79</v>
       </c>
       <c r="B83" s="19"/>
       <c r="C83" s="19"/>
       <c r="D83" s="19" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E83" s="19" t="s">
-        <v>151</v>
+        <v>21</v>
       </c>
       <c r="F83" s="20">
-        <v>150</v>
-      </c>
-      <c r="G83" s="21"/>
+        <v>8</v>
+      </c>
+      <c r="G83" s="21">
+        <v>0.8</v>
+      </c>
       <c r="H83" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A84" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B84" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="C84" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="D84" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E84" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F84" s="20">
+        <v>12</v>
+      </c>
+      <c r="G84" s="21">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H84" s="14">
+        <f t="shared" si="2"/>
+        <v>13.200000000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A85" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="B84" s="19"/>
-      <c r="C84" s="19"/>
-      <c r="D84" s="19"/>
-      <c r="E84" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F84" s="20">
-        <v>8</v>
-      </c>
-      <c r="G84" s="21">
-        <v>0.8</v>
-      </c>
-      <c r="H84" s="14">
-        <f t="shared" si="2"/>
-        <v>6.4</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A85" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="B85" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="C85" s="19" t="s">
-        <v>195</v>
-      </c>
+      <c r="B85" s="19"/>
+      <c r="C85" s="19"/>
       <c r="D85" s="19" t="s">
         <v>28</v>
       </c>
@@ -4404,134 +4432,144 @@
         <v>21</v>
       </c>
       <c r="F85" s="20">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G85" s="21">
-        <v>1.1000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="H85" s="14">
         <f t="shared" si="2"/>
-        <v>13.200000000000001</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A86" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B86" s="19"/>
       <c r="C86" s="19"/>
-      <c r="D86" s="19"/>
+      <c r="D86" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E86" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F86" s="20">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G86" s="21">
-        <v>0.9</v>
+        <v>1.5</v>
       </c>
       <c r="H86" s="14">
         <f t="shared" si="2"/>
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A87" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B87" s="19"/>
       <c r="C87" s="19"/>
-      <c r="D87" s="19"/>
+      <c r="D87" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E87" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F87" s="20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G87" s="21">
         <v>1.5</v>
       </c>
       <c r="H87" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A88" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B88" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="C88" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="D88" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E88" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F88" s="20">
+        <v>4</v>
+      </c>
+      <c r="G88" s="21">
+        <v>12.5</v>
+      </c>
+      <c r="H88" s="14">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A89" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="B88" s="19"/>
-      <c r="C88" s="19"/>
-      <c r="D88" s="19"/>
-      <c r="E88" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F88" s="20">
-        <v>3</v>
-      </c>
-      <c r="G88" s="21">
-        <v>1.5</v>
-      </c>
-      <c r="H88" s="14">
-        <f t="shared" si="2"/>
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A89" s="18" t="s">
+      <c r="B89" s="19"/>
+      <c r="C89" s="19"/>
+      <c r="D89" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E89" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F89" s="20">
+        <v>2</v>
+      </c>
+      <c r="G89" s="21">
+        <v>2.5</v>
+      </c>
+      <c r="H89" s="14">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A90" s="18" t="s">
         <v>86</v>
-      </c>
-      <c r="B89" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="C89" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="D89" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="E89" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F89" s="20">
-        <v>4</v>
-      </c>
-      <c r="G89" s="21">
-        <v>12.5</v>
-      </c>
-      <c r="H89" s="14">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A90" s="18" t="s">
-        <v>87</v>
       </c>
       <c r="B90" s="19"/>
       <c r="C90" s="19"/>
-      <c r="D90" s="19"/>
+      <c r="D90" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E90" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F90" s="20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G90" s="21">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="H90" s="14">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A91" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B91" s="19"/>
       <c r="C91" s="19"/>
-      <c r="D91" s="19"/>
+      <c r="D91" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E91" s="19" t="s">
         <v>21</v>
       </c>
@@ -4546,101 +4584,109 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+    <row r="92" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A92" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B92" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="C92" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="D92" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E92" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F92" s="20">
+        <v>50</v>
+      </c>
+      <c r="G92" s="38">
+        <v>0.19</v>
+      </c>
+      <c r="H92" s="44">
+        <f t="shared" si="2"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A93" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="B92" s="19"/>
-      <c r="C92" s="19"/>
-      <c r="D92" s="19"/>
-      <c r="E92" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F92" s="20">
-        <v>0</v>
-      </c>
-      <c r="G92" s="21">
-        <v>1</v>
-      </c>
-      <c r="H92" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A93" s="18" t="s">
+      <c r="B93" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="C93" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="D93" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E93" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F93" s="37">
+        <v>50</v>
+      </c>
+      <c r="G93" s="40">
+        <v>0.19</v>
+      </c>
+      <c r="H93" s="46">
+        <f t="shared" si="2"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A94" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="B93" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="C93" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="D93" s="19"/>
-      <c r="E93" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F93" s="20">
-        <v>50</v>
-      </c>
-      <c r="G93" s="38">
-        <v>0.19</v>
-      </c>
-      <c r="H93" s="44">
-        <f t="shared" si="2"/>
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A94" s="18" t="s">
+      <c r="B94" s="19"/>
+      <c r="C94" s="19"/>
+      <c r="D94" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E94" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F94" s="20">
+        <v>3</v>
+      </c>
+      <c r="G94" s="39">
+        <v>1.2</v>
+      </c>
+      <c r="H94" s="45">
+        <f t="shared" si="2"/>
+        <v>3.5999999999999996</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
+      <c r="A95" s="18" t="s">
         <v>91</v>
-      </c>
-      <c r="B94" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="C94" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="D94" s="19"/>
-      <c r="E94" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F94" s="37">
-        <v>50</v>
-      </c>
-      <c r="G94" s="40">
-        <v>0.19</v>
-      </c>
-      <c r="H94" s="46">
-        <f t="shared" si="2"/>
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A95" s="18" t="s">
-        <v>92</v>
       </c>
       <c r="B95" s="19"/>
       <c r="C95" s="19"/>
-      <c r="D95" s="19"/>
+      <c r="D95" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="E95" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F95" s="20">
-        <v>3</v>
-      </c>
-      <c r="G95" s="39">
-        <v>1.2</v>
-      </c>
-      <c r="H95" s="45">
-        <f t="shared" si="2"/>
-        <v>3.5999999999999996</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+        <v>0</v>
+      </c>
+      <c r="G95" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="H95" s="44">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A96" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B96" s="19"/>
       <c r="C96" s="19"/>
@@ -4649,522 +4695,528 @@
         <v>21</v>
       </c>
       <c r="F96" s="20">
-        <v>0</v>
-      </c>
-      <c r="G96" s="21">
-        <v>0.2</v>
-      </c>
-      <c r="H96" s="44">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G96" s="43">
+        <v>1</v>
+      </c>
+      <c r="H96" s="46">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="I96" s="41"/>
     </row>
     <row r="97" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A97" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="B97" s="19"/>
-      <c r="C97" s="19"/>
-      <c r="D97" s="19"/>
+        <v>187</v>
+      </c>
+      <c r="B97" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="C97" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="D97" s="19" t="s">
+        <v>181</v>
+      </c>
       <c r="E97" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F97" s="20">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="G97" s="43">
-        <v>1</v>
+        <v>3.45</v>
       </c>
       <c r="H97" s="46">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="I97" s="41"/>
+        <f>F97*G97</f>
+        <v>358.8</v>
+      </c>
+      <c r="I97" s="42"/>
     </row>
     <row r="98" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A98" s="18" t="s">
-        <v>190</v>
+        <v>93</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C98" s="19" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D98" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E98" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F98" s="20">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G98" s="43">
-        <v>3.45</v>
+        <v>2.9</v>
       </c>
       <c r="H98" s="46">
-        <f>F98*G98</f>
-        <v>358.8</v>
+        <f t="shared" si="2"/>
+        <v>284.2</v>
       </c>
       <c r="I98" s="42"/>
     </row>
     <row r="99" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A99" s="18" t="s">
-        <v>95</v>
+        <v>217</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>182</v>
+        <v>219</v>
       </c>
       <c r="C99" s="19" t="s">
-        <v>180</v>
+        <v>218</v>
       </c>
       <c r="D99" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E99" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F99" s="20">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="G99" s="43">
-        <v>2.9</v>
+        <v>4.8</v>
       </c>
       <c r="H99" s="46">
         <f t="shared" si="2"/>
-        <v>284.2</v>
+        <v>182.4</v>
       </c>
       <c r="I99" s="42"/>
     </row>
     <row r="100" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A100" s="18" t="s">
-        <v>220</v>
+        <v>94</v>
       </c>
       <c r="B100" s="19" t="s">
-        <v>222</v>
+        <v>180</v>
       </c>
       <c r="C100" s="19" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
       <c r="D100" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E100" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F100" s="20">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="G100" s="43">
-        <v>4.8</v>
+        <v>3.45</v>
       </c>
       <c r="H100" s="46">
         <f t="shared" si="2"/>
-        <v>182.4</v>
+        <v>0</v>
       </c>
       <c r="I100" s="42"/>
     </row>
     <row r="101" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A101" s="18" t="s">
-        <v>96</v>
+        <v>186</v>
       </c>
       <c r="B101" s="19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C101" s="19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D101" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E101" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F101" s="20">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="G101" s="43">
-        <v>3.45</v>
+        <v>3.75</v>
       </c>
       <c r="H101" s="46">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>183.75</v>
       </c>
       <c r="I101" s="42"/>
     </row>
     <row r="102" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A102" s="18" t="s">
-        <v>189</v>
+        <v>95</v>
       </c>
       <c r="B102" s="19" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C102" s="19" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="D102" s="19" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="E102" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F102" s="20">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="G102" s="43">
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="H102" s="46">
         <f t="shared" si="2"/>
-        <v>183.75</v>
+        <v>48</v>
       </c>
       <c r="I102" s="42"/>
     </row>
     <row r="103" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A103" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B103" s="19" t="s">
         <v>191</v>
       </c>
       <c r="C103" s="19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D103" s="19" t="s">
-        <v>198</v>
+        <v>28</v>
       </c>
       <c r="E103" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F103" s="20">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="G103" s="43">
-        <v>4</v>
+        <v>0.8</v>
       </c>
       <c r="H103" s="46">
         <f t="shared" si="2"/>
-        <v>48</v>
+        <v>38.400000000000006</v>
       </c>
       <c r="I103" s="42"/>
     </row>
     <row r="104" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A104" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B104" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="C104" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="C104" s="19" t="s">
-        <v>170</v>
-      </c>
       <c r="D104" s="19" t="s">
-        <v>28</v>
+        <v>193</v>
       </c>
       <c r="E104" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F104" s="20">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="G104" s="43">
-        <v>0.8</v>
+        <v>11.7</v>
       </c>
       <c r="H104" s="46">
         <f t="shared" si="2"/>
-        <v>38.400000000000006</v>
-      </c>
-      <c r="I104" s="42"/>
+        <v>117</v>
+      </c>
     </row>
     <row r="105" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A105" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="B105" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="C105" s="19" t="s">
-        <v>197</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="B105" s="19"/>
+      <c r="C105" s="19"/>
       <c r="D105" s="19" t="s">
-        <v>196</v>
+        <v>15</v>
       </c>
       <c r="E105" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F105" s="20">
-        <v>10</v>
+        <v>170</v>
       </c>
       <c r="G105" s="43">
-        <v>11.7</v>
+        <v>2.4</v>
       </c>
       <c r="H105" s="46">
         <f t="shared" si="2"/>
-        <v>117</v>
+        <v>408</v>
       </c>
     </row>
     <row r="106" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A106" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="B106" s="19"/>
-      <c r="C106" s="19"/>
+        <v>99</v>
+      </c>
+      <c r="B106" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="C106" s="19" t="s">
+        <v>192</v>
+      </c>
       <c r="D106" s="19" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E106" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F106" s="20">
-        <v>170</v>
-      </c>
-      <c r="G106" s="43">
-        <v>2.4</v>
-      </c>
-      <c r="H106" s="46">
-        <f t="shared" si="2"/>
-        <v>408</v>
+        <v>30</v>
+      </c>
+      <c r="G106" s="21">
+        <v>0.83</v>
+      </c>
+      <c r="H106" s="45">
+        <f t="shared" si="2"/>
+        <v>24.9</v>
       </c>
     </row>
     <row r="107" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A107" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B107" s="19" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="C107" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="D107" s="19" t="s">
-        <v>28</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="D107" s="19"/>
       <c r="E107" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F107" s="20">
-        <v>30</v>
+        <v>139</v>
       </c>
       <c r="G107" s="21">
-        <v>0.83</v>
-      </c>
-      <c r="H107" s="45">
-        <f t="shared" si="2"/>
-        <v>24.9</v>
+        <v>4.7</v>
+      </c>
+      <c r="H107" s="14">
+        <f t="shared" si="2"/>
+        <v>653.30000000000007</v>
       </c>
     </row>
     <row r="108" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A108" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B108" s="19" t="s">
-        <v>213</v>
+        <v>176</v>
       </c>
       <c r="C108" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="D108" s="19"/>
+        <v>173</v>
+      </c>
+      <c r="D108" s="19" t="s">
+        <v>154</v>
+      </c>
       <c r="E108" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F108" s="20">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="G108" s="21">
-        <v>4.7</v>
+        <v>2.5</v>
       </c>
       <c r="H108" s="14">
         <f t="shared" si="2"/>
-        <v>653.30000000000007</v>
+        <v>260</v>
       </c>
     </row>
     <row r="109" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A109" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="B109" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="C109" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="D109" s="19" t="s">
-        <v>156</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="B109" s="19"/>
+      <c r="C109" s="19"/>
+      <c r="D109" s="34"/>
       <c r="E109" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F109" s="20">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="G109" s="21">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="H109" s="14">
         <f t="shared" si="2"/>
-        <v>260</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A110" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B110" s="19"/>
       <c r="C110" s="19"/>
-      <c r="D110" s="34"/>
+      <c r="D110" s="19"/>
       <c r="E110" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F110" s="20">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G110" s="21">
         <v>2</v>
       </c>
       <c r="H110" s="14">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="111" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A111" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="B111" s="19"/>
-      <c r="C111" s="19"/>
-      <c r="D111" s="19"/>
+        <v>200</v>
+      </c>
+      <c r="B111" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="C111" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="D111" s="19" t="s">
+        <v>171</v>
+      </c>
       <c r="E111" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F111" s="20">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="G111" s="21">
-        <v>2</v>
+        <v>41.34</v>
       </c>
       <c r="H111" s="14">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>289.38</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A112" s="18" t="s">
-        <v>203</v>
+        <v>104</v>
       </c>
       <c r="B112" s="19" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="C112" s="19" t="s">
-        <v>169</v>
+        <v>234</v>
       </c>
       <c r="D112" s="19" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="E112" s="19" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="F112" s="20">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="G112" s="21">
-        <v>41.34</v>
+        <v>2.7</v>
       </c>
       <c r="H112" s="14">
         <f t="shared" si="2"/>
-        <v>289.38</v>
+        <v>162</v>
       </c>
     </row>
     <row r="113" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A113" s="18" t="s">
+      <c r="A113" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B113" s="29">
+        <v>43140</v>
+      </c>
+      <c r="C113" s="11">
+        <v>36</v>
+      </c>
+      <c r="D113" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="E113" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B113" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="C113" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="D113" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="E113" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="F113" s="20">
-        <v>60</v>
-      </c>
-      <c r="G113" s="21">
-        <v>2.7</v>
+      <c r="F113" s="12">
+        <v>15</v>
+      </c>
+      <c r="G113" s="14">
+        <v>6</v>
       </c>
       <c r="H113" s="14">
         <f t="shared" si="2"/>
-        <v>162</v>
+        <v>90</v>
       </c>
     </row>
     <row r="114" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A114" s="23" t="s">
+      <c r="A114" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="B114" s="29">
-        <v>43140</v>
-      </c>
-      <c r="C114" s="11">
-        <v>36</v>
-      </c>
-      <c r="D114" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="E114" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="F114" s="12">
-        <v>15</v>
-      </c>
-      <c r="G114" s="14">
-        <v>6</v>
+      <c r="B114" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="C114" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="D114" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="E114" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F114" s="20">
+        <v>900</v>
+      </c>
+      <c r="G114" s="21">
+        <v>0.66</v>
       </c>
       <c r="H114" s="14">
         <f t="shared" si="2"/>
-        <v>90</v>
+        <v>594</v>
       </c>
     </row>
     <row r="115" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A115" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B115" s="19" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="C115" s="19" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="D115" s="19" t="s">
-        <v>186</v>
+        <v>28</v>
       </c>
       <c r="E115" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F115" s="20">
-        <v>900</v>
+        <v>5</v>
       </c>
       <c r="G115" s="21">
-        <v>0.66</v>
+        <v>2.85</v>
       </c>
       <c r="H115" s="14">
         <f t="shared" si="2"/>
-        <v>594</v>
+        <v>14.25</v>
       </c>
     </row>
     <row r="116" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A116" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>168</v>
+        <v>205</v>
       </c>
       <c r="C116" s="19" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="D116" s="19" t="s">
         <v>28</v>
@@ -5173,25 +5225,25 @@
         <v>21</v>
       </c>
       <c r="F116" s="20">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G116" s="21">
-        <v>2.85</v>
+        <v>1.72</v>
       </c>
       <c r="H116" s="14">
         <f t="shared" si="2"/>
-        <v>14.25</v>
+        <v>12.04</v>
       </c>
     </row>
     <row r="117" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A117" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B117" s="19" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
       <c r="C117" s="19" t="s">
-        <v>181</v>
+        <v>231</v>
       </c>
       <c r="D117" s="19" t="s">
         <v>28</v>
@@ -5200,25 +5252,25 @@
         <v>21</v>
       </c>
       <c r="F117" s="20">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G117" s="21">
-        <v>1.72</v>
+        <v>2.9</v>
       </c>
       <c r="H117" s="14">
         <f t="shared" si="2"/>
-        <v>12.04</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="118" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A118" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B118" s="19" t="s">
-        <v>233</v>
+        <v>189</v>
       </c>
       <c r="C118" s="19" t="s">
-        <v>234</v>
+        <v>177</v>
       </c>
       <c r="D118" s="19" t="s">
         <v>28</v>
@@ -5227,94 +5279,94 @@
         <v>21</v>
       </c>
       <c r="F118" s="20">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G118" s="21">
-        <v>2.9</v>
+        <v>1.72</v>
       </c>
       <c r="H118" s="14">
         <f t="shared" si="2"/>
-        <v>17.399999999999999</v>
+        <v>5.16</v>
       </c>
     </row>
     <row r="119" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A119" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="B119" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="C119" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="D119" s="19" t="s">
-        <v>28</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="B119" s="19"/>
+      <c r="C119" s="19"/>
+      <c r="D119" s="35"/>
       <c r="E119" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F119" s="20">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G119" s="21">
-        <v>1.72</v>
+        <v>5</v>
       </c>
       <c r="H119" s="14">
         <f t="shared" si="2"/>
-        <v>5.16</v>
+        <v>35</v>
       </c>
     </row>
     <row r="120" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A120" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B120" s="19"/>
       <c r="C120" s="19"/>
-      <c r="D120" s="35"/>
+      <c r="D120" s="19"/>
       <c r="E120" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F120" s="20">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G120" s="21">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H120" s="14">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="121" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A121" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="B121" s="19"/>
-      <c r="C121" s="19"/>
-      <c r="D121" s="19"/>
+        <v>114</v>
+      </c>
+      <c r="B121" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="C121" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="D121" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="E121" s="19" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F121" s="20">
-        <v>9</v>
+        <v>169</v>
       </c>
       <c r="G121" s="21">
-        <v>1</v>
+        <v>2.69</v>
       </c>
       <c r="H121" s="14">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>454.61</v>
       </c>
     </row>
     <row r="122" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A122" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B122" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="C122" s="19" t="s">
         <v>172</v>
-      </c>
-      <c r="C122" s="19" t="s">
-        <v>176</v>
       </c>
       <c r="D122" s="19" t="s">
         <v>9</v>
@@ -5323,94 +5375,88 @@
         <v>12</v>
       </c>
       <c r="F122" s="20">
-        <v>169</v>
+        <v>113</v>
       </c>
       <c r="G122" s="21">
-        <v>2.69</v>
+        <v>3.3</v>
       </c>
       <c r="H122" s="14">
         <f t="shared" si="2"/>
-        <v>454.61</v>
+        <v>372.9</v>
       </c>
     </row>
     <row r="123" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A123" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="B123" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="C123" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="D123" s="19" t="s">
-        <v>9</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="B123" s="19"/>
+      <c r="C123" s="19"/>
+      <c r="D123" s="19"/>
       <c r="E123" s="19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F123" s="20">
-        <v>113</v>
+        <v>5</v>
       </c>
       <c r="G123" s="21">
-        <v>3.3</v>
+        <v>2.87</v>
       </c>
       <c r="H123" s="14">
         <f t="shared" si="2"/>
-        <v>372.9</v>
+        <v>14.350000000000001</v>
       </c>
     </row>
     <row r="124" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A124" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B124" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="C124" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="D124" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="B124" s="19"/>
-      <c r="C124" s="19"/>
-      <c r="D124" s="19"/>
       <c r="E124" s="19" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="F124" s="20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G124" s="21">
-        <v>2.87</v>
+        <v>7</v>
       </c>
       <c r="H124" s="14">
         <f t="shared" si="2"/>
-        <v>14.350000000000001</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" s="36" customFormat="1" ht="28.35" customHeight="1">
       <c r="A125" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="B125" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="C125" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="D125" s="19" t="s">
         <v>120</v>
       </c>
+      <c r="B125" s="19"/>
+      <c r="C125" s="19"/>
+      <c r="D125" s="19"/>
       <c r="E125" s="19" t="s">
-        <v>121</v>
+        <v>21</v>
       </c>
       <c r="F125" s="20">
-        <v>6</v>
+        <v>582</v>
       </c>
       <c r="G125" s="21">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H125" s="14">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="126" spans="1:8" s="36" customFormat="1" ht="28.35" customHeight="1">
       <c r="A126" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B126" s="19"/>
       <c r="C126" s="19"/>
@@ -5419,88 +5465,94 @@
         <v>21</v>
       </c>
       <c r="F126" s="20">
-        <v>582</v>
+        <v>1</v>
       </c>
       <c r="G126" s="21">
-        <v>3</v>
+        <v>1.96</v>
       </c>
       <c r="H126" s="14">
         <f t="shared" si="2"/>
-        <v>1746</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" s="36" customFormat="1" ht="28.35" customHeight="1">
-      <c r="A127" s="18" t="s">
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="28.35" customHeight="1">
+      <c r="A127" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B127" s="11"/>
+      <c r="C127" s="11"/>
+      <c r="D127" s="11"/>
+      <c r="E127" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F127" s="24">
+        <v>7</v>
+      </c>
+      <c r="G127" s="25">
+        <v>1.97</v>
+      </c>
+      <c r="H127" s="14">
+        <f t="shared" si="2"/>
+        <v>13.79</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="28.35" customHeight="1">
+      <c r="A128" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="B127" s="19"/>
-      <c r="C127" s="19"/>
-      <c r="D127" s="19"/>
-      <c r="E127" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F127" s="20">
-        <v>1</v>
-      </c>
-      <c r="G127" s="21">
-        <v>1.96</v>
-      </c>
-      <c r="H127" s="14">
-        <f t="shared" si="2"/>
-        <v>1.96</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" ht="28.35" customHeight="1">
-      <c r="A128" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="B128" s="11"/>
-      <c r="C128" s="11"/>
-      <c r="D128" s="11"/>
+      <c r="B128" s="19"/>
+      <c r="C128" s="19"/>
+      <c r="D128" s="19"/>
       <c r="E128" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F128" s="24">
+      <c r="F128" s="20">
+        <v>95</v>
+      </c>
+      <c r="G128" s="21">
         <v>7</v>
       </c>
-      <c r="G128" s="25">
-        <v>1.97</v>
-      </c>
       <c r="H128" s="14">
         <f t="shared" si="2"/>
-        <v>13.79</v>
+        <v>665</v>
       </c>
     </row>
     <row r="129" spans="1:255" ht="28.35" customHeight="1">
       <c r="A129" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="B129" s="19"/>
-      <c r="C129" s="19"/>
-      <c r="D129" s="19"/>
+        <v>124</v>
+      </c>
+      <c r="B129" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="C129" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="D129" s="19" t="s">
+        <v>13</v>
+      </c>
       <c r="E129" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F129" s="20">
-        <v>95</v>
+        <v>250</v>
       </c>
       <c r="G129" s="21">
-        <v>7</v>
+        <v>2.69</v>
       </c>
       <c r="H129" s="14">
         <f t="shared" si="2"/>
-        <v>665</v>
+        <v>672.5</v>
       </c>
     </row>
     <row r="130" spans="1:255" ht="28.35" customHeight="1">
       <c r="A130" s="18" t="s">
-        <v>126</v>
+        <v>175</v>
       </c>
       <c r="B130" s="19" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C130" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D130" s="19" t="s">
         <v>13</v>
@@ -5509,444 +5561,438 @@
         <v>12</v>
       </c>
       <c r="F130" s="20">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="G130" s="21">
-        <v>2.69</v>
+        <v>2.21</v>
       </c>
       <c r="H130" s="14">
         <f t="shared" si="2"/>
-        <v>672.5</v>
+        <v>331.5</v>
       </c>
     </row>
     <row r="131" spans="1:255" ht="28.35" customHeight="1">
-      <c r="A131" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="B131" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="C131" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="D131" s="19" t="s">
-        <v>13</v>
-      </c>
+      <c r="A131" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="B131" s="11"/>
+      <c r="C131" s="11"/>
+      <c r="D131" s="11"/>
       <c r="E131" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F131" s="20">
-        <v>150</v>
-      </c>
-      <c r="G131" s="21">
-        <v>2.21</v>
+      <c r="F131" s="24">
+        <v>100</v>
+      </c>
+      <c r="G131" s="25">
+        <v>1.43</v>
       </c>
       <c r="H131" s="14">
         <f t="shared" si="2"/>
-        <v>331.5</v>
+        <v>143</v>
       </c>
     </row>
     <row r="132" spans="1:255" ht="28.35" customHeight="1">
-      <c r="A132" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="B132" s="11"/>
-      <c r="C132" s="11"/>
-      <c r="D132" s="11"/>
+      <c r="A132" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B132" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C132" s="19"/>
+      <c r="D132" s="19"/>
       <c r="E132" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F132" s="24">
-        <v>100</v>
-      </c>
-      <c r="G132" s="25">
-        <v>1.43</v>
+      <c r="F132" s="20">
+        <v>4</v>
+      </c>
+      <c r="G132" s="21">
+        <v>8.5</v>
       </c>
       <c r="H132" s="14">
         <f t="shared" si="2"/>
-        <v>143</v>
+        <v>34</v>
       </c>
     </row>
     <row r="133" spans="1:255" ht="28.35" customHeight="1">
       <c r="A133" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="B133" s="19" t="s">
-        <v>225</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="B133" s="19"/>
       <c r="C133" s="19"/>
       <c r="D133" s="19"/>
       <c r="E133" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F133" s="20">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="G133" s="21">
-        <v>8.5</v>
+        <v>5</v>
       </c>
       <c r="H133" s="14">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>85</v>
       </c>
     </row>
     <row r="134" spans="1:255" ht="28.35" customHeight="1">
       <c r="A134" s="18" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="B134" s="19"/>
       <c r="C134" s="19"/>
-      <c r="D134" s="19"/>
+      <c r="D134" s="19" t="s">
+        <v>153</v>
+      </c>
       <c r="E134" s="11" t="s">
         <v>12</v>
       </c>
       <c r="F134" s="20">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G134" s="21">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="H134" s="14">
         <f t="shared" si="2"/>
-        <v>85</v>
+        <v>564</v>
       </c>
     </row>
     <row r="135" spans="1:255" ht="28.35" customHeight="1">
-      <c r="A135" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="B135" s="19"/>
-      <c r="C135" s="19"/>
-      <c r="D135" s="19" t="s">
-        <v>155</v>
-      </c>
+      <c r="A135" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="B135" s="11"/>
+      <c r="C135" s="11"/>
+      <c r="D135" s="11"/>
       <c r="E135" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F135" s="20">
+      <c r="F135" s="24">
+        <v>22</v>
+      </c>
+      <c r="G135" s="25">
+        <v>2.97</v>
+      </c>
+      <c r="H135" s="14">
+        <f t="shared" si="2"/>
+        <v>65.34</v>
+      </c>
+    </row>
+    <row r="136" spans="1:255" ht="28.35" customHeight="1">
+      <c r="A136" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="B136" s="19"/>
+      <c r="C136" s="19"/>
+      <c r="D136" s="19"/>
+      <c r="E136" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F136" s="20">
+        <v>140</v>
+      </c>
+      <c r="G136" s="21">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="H136" s="14">
+        <f t="shared" si="2"/>
+        <v>158.19999999999999</v>
+      </c>
+      <c r="I136"/>
+      <c r="J136"/>
+      <c r="K136"/>
+      <c r="L136"/>
+      <c r="M136"/>
+      <c r="N136"/>
+      <c r="O136"/>
+      <c r="P136"/>
+      <c r="Q136"/>
+      <c r="R136"/>
+      <c r="S136"/>
+      <c r="T136"/>
+      <c r="U136"/>
+      <c r="V136"/>
+      <c r="W136"/>
+      <c r="X136"/>
+      <c r="Y136"/>
+      <c r="Z136"/>
+      <c r="AA136"/>
+      <c r="AB136"/>
+      <c r="AC136"/>
+      <c r="AD136"/>
+      <c r="AE136"/>
+      <c r="AF136"/>
+      <c r="AG136"/>
+      <c r="AH136"/>
+      <c r="AI136"/>
+      <c r="AJ136"/>
+      <c r="AK136"/>
+      <c r="AL136"/>
+      <c r="AM136"/>
+      <c r="AN136"/>
+      <c r="AO136"/>
+      <c r="AP136"/>
+      <c r="AQ136"/>
+      <c r="AR136"/>
+      <c r="AS136"/>
+      <c r="AT136"/>
+      <c r="AU136"/>
+      <c r="AV136"/>
+      <c r="AW136"/>
+      <c r="AX136"/>
+      <c r="AY136"/>
+      <c r="AZ136"/>
+      <c r="BA136"/>
+      <c r="BB136"/>
+      <c r="BC136"/>
+      <c r="BD136"/>
+      <c r="BE136"/>
+      <c r="BF136"/>
+      <c r="BG136"/>
+      <c r="BH136"/>
+      <c r="BI136"/>
+      <c r="BJ136"/>
+      <c r="BK136"/>
+      <c r="BL136"/>
+      <c r="BM136"/>
+      <c r="BN136"/>
+      <c r="BO136"/>
+      <c r="BP136"/>
+      <c r="BQ136"/>
+      <c r="BR136"/>
+      <c r="BS136"/>
+      <c r="BT136"/>
+      <c r="BU136"/>
+      <c r="BV136"/>
+      <c r="BW136"/>
+      <c r="BX136"/>
+      <c r="BY136"/>
+      <c r="BZ136"/>
+      <c r="CA136"/>
+      <c r="CB136"/>
+      <c r="CC136"/>
+      <c r="CD136"/>
+      <c r="CE136"/>
+      <c r="CF136"/>
+      <c r="CG136"/>
+      <c r="CH136"/>
+      <c r="CI136"/>
+      <c r="CJ136"/>
+      <c r="CK136"/>
+      <c r="CL136"/>
+      <c r="CM136"/>
+      <c r="CN136"/>
+      <c r="CO136"/>
+      <c r="CP136"/>
+      <c r="CQ136"/>
+      <c r="CR136"/>
+      <c r="CS136"/>
+      <c r="CT136"/>
+      <c r="CU136"/>
+      <c r="CV136"/>
+      <c r="CW136"/>
+      <c r="CX136"/>
+      <c r="CY136"/>
+      <c r="CZ136"/>
+      <c r="DA136"/>
+      <c r="DB136"/>
+      <c r="DC136"/>
+      <c r="DD136"/>
+      <c r="DE136"/>
+      <c r="DF136"/>
+      <c r="DG136"/>
+      <c r="DH136"/>
+      <c r="DI136"/>
+      <c r="DJ136"/>
+      <c r="DK136"/>
+      <c r="DL136"/>
+      <c r="DM136"/>
+      <c r="DN136"/>
+      <c r="DO136"/>
+      <c r="DP136"/>
+      <c r="DQ136"/>
+      <c r="DR136"/>
+      <c r="DS136"/>
+      <c r="DT136"/>
+      <c r="DU136"/>
+      <c r="DV136"/>
+      <c r="DW136"/>
+      <c r="DX136"/>
+      <c r="DY136"/>
+      <c r="DZ136"/>
+      <c r="EA136"/>
+      <c r="EB136"/>
+      <c r="EC136"/>
+      <c r="ED136"/>
+      <c r="EE136"/>
+      <c r="EF136"/>
+      <c r="EG136"/>
+      <c r="EH136"/>
+      <c r="EI136"/>
+      <c r="EJ136"/>
+      <c r="EK136"/>
+      <c r="EL136"/>
+      <c r="EM136"/>
+      <c r="EN136"/>
+      <c r="EO136"/>
+      <c r="EP136"/>
+      <c r="EQ136"/>
+      <c r="ER136"/>
+      <c r="ES136"/>
+      <c r="ET136"/>
+      <c r="EU136"/>
+      <c r="EV136"/>
+      <c r="EW136"/>
+      <c r="EX136"/>
+      <c r="EY136"/>
+      <c r="EZ136"/>
+      <c r="FA136"/>
+      <c r="FB136"/>
+      <c r="FC136"/>
+      <c r="FD136"/>
+      <c r="FE136"/>
+      <c r="FF136"/>
+      <c r="FG136"/>
+      <c r="FH136"/>
+      <c r="FI136"/>
+      <c r="FJ136"/>
+      <c r="FK136"/>
+      <c r="FL136"/>
+      <c r="FM136"/>
+      <c r="FN136"/>
+      <c r="FO136"/>
+      <c r="FP136"/>
+      <c r="FQ136"/>
+      <c r="FR136"/>
+      <c r="FS136"/>
+      <c r="FT136"/>
+      <c r="FU136"/>
+      <c r="FV136"/>
+      <c r="FW136"/>
+      <c r="FX136"/>
+      <c r="FY136"/>
+      <c r="FZ136"/>
+      <c r="GA136"/>
+      <c r="GB136"/>
+      <c r="GC136"/>
+      <c r="GD136"/>
+      <c r="GE136"/>
+      <c r="GF136"/>
+      <c r="GG136"/>
+      <c r="GH136"/>
+      <c r="GI136"/>
+      <c r="GJ136"/>
+      <c r="GK136"/>
+      <c r="GL136"/>
+      <c r="GM136"/>
+      <c r="GN136"/>
+      <c r="GO136"/>
+      <c r="GP136"/>
+      <c r="GQ136"/>
+      <c r="GR136"/>
+      <c r="GS136"/>
+      <c r="GT136"/>
+      <c r="GU136"/>
+      <c r="GV136"/>
+      <c r="GW136"/>
+      <c r="GX136"/>
+      <c r="GY136"/>
+      <c r="GZ136"/>
+      <c r="HA136"/>
+      <c r="HB136"/>
+      <c r="HC136"/>
+      <c r="HD136"/>
+      <c r="HE136"/>
+      <c r="HF136"/>
+      <c r="HG136"/>
+      <c r="HH136"/>
+      <c r="HI136"/>
+      <c r="HJ136"/>
+      <c r="HK136"/>
+      <c r="HL136"/>
+      <c r="HM136"/>
+      <c r="HN136"/>
+      <c r="HO136"/>
+      <c r="HP136"/>
+      <c r="HQ136"/>
+      <c r="HR136"/>
+      <c r="HS136"/>
+      <c r="HT136"/>
+      <c r="HU136"/>
+      <c r="HV136"/>
+      <c r="HW136"/>
+      <c r="HX136"/>
+      <c r="HY136"/>
+      <c r="HZ136"/>
+      <c r="IA136"/>
+      <c r="IB136"/>
+      <c r="IC136"/>
+      <c r="ID136"/>
+      <c r="IE136"/>
+      <c r="IF136"/>
+      <c r="IG136"/>
+      <c r="IH136"/>
+      <c r="II136"/>
+      <c r="IJ136"/>
+      <c r="IK136"/>
+      <c r="IL136"/>
+      <c r="IM136"/>
+      <c r="IN136"/>
+      <c r="IO136"/>
+      <c r="IP136"/>
+      <c r="IQ136"/>
+      <c r="IR136"/>
+      <c r="IS136"/>
+      <c r="IT136"/>
+      <c r="IU136"/>
+    </row>
+    <row r="137" spans="1:255" ht="28.35" customHeight="1">
+      <c r="A137" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="B137" s="11"/>
+      <c r="C137" s="11"/>
+      <c r="D137" s="11"/>
+      <c r="E137" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G135" s="21">
-        <v>47</v>
-      </c>
-      <c r="H135" s="14">
-        <f t="shared" si="2"/>
-        <v>564</v>
-      </c>
-    </row>
-    <row r="136" spans="1:255" ht="28.35" customHeight="1">
-      <c r="A136" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="B136" s="11"/>
-      <c r="C136" s="11"/>
-      <c r="D136" s="11"/>
-      <c r="E136" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F136" s="24">
-        <v>22</v>
-      </c>
-      <c r="G136" s="25">
-        <v>2.97</v>
-      </c>
-      <c r="H136" s="14">
-        <f t="shared" si="2"/>
-        <v>65.34</v>
-      </c>
-    </row>
-    <row r="137" spans="1:255" ht="28.35" customHeight="1">
-      <c r="A137" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="B137" s="19"/>
-      <c r="C137" s="19"/>
-      <c r="D137" s="19"/>
-      <c r="E137" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F137" s="20">
-        <v>140</v>
-      </c>
-      <c r="G137" s="21">
-        <v>1.1299999999999999</v>
+      <c r="F137" s="24">
+        <v>25</v>
+      </c>
+      <c r="G137" s="25">
+        <v>5</v>
       </c>
       <c r="H137" s="14">
         <f t="shared" si="2"/>
-        <v>158.19999999999999</v>
-      </c>
-      <c r="I137"/>
-      <c r="J137"/>
-      <c r="K137"/>
-      <c r="L137"/>
-      <c r="M137"/>
-      <c r="N137"/>
-      <c r="O137"/>
-      <c r="P137"/>
-      <c r="Q137"/>
-      <c r="R137"/>
-      <c r="S137"/>
-      <c r="T137"/>
-      <c r="U137"/>
-      <c r="V137"/>
-      <c r="W137"/>
-      <c r="X137"/>
-      <c r="Y137"/>
-      <c r="Z137"/>
-      <c r="AA137"/>
-      <c r="AB137"/>
-      <c r="AC137"/>
-      <c r="AD137"/>
-      <c r="AE137"/>
-      <c r="AF137"/>
-      <c r="AG137"/>
-      <c r="AH137"/>
-      <c r="AI137"/>
-      <c r="AJ137"/>
-      <c r="AK137"/>
-      <c r="AL137"/>
-      <c r="AM137"/>
-      <c r="AN137"/>
-      <c r="AO137"/>
-      <c r="AP137"/>
-      <c r="AQ137"/>
-      <c r="AR137"/>
-      <c r="AS137"/>
-      <c r="AT137"/>
-      <c r="AU137"/>
-      <c r="AV137"/>
-      <c r="AW137"/>
-      <c r="AX137"/>
-      <c r="AY137"/>
-      <c r="AZ137"/>
-      <c r="BA137"/>
-      <c r="BB137"/>
-      <c r="BC137"/>
-      <c r="BD137"/>
-      <c r="BE137"/>
-      <c r="BF137"/>
-      <c r="BG137"/>
-      <c r="BH137"/>
-      <c r="BI137"/>
-      <c r="BJ137"/>
-      <c r="BK137"/>
-      <c r="BL137"/>
-      <c r="BM137"/>
-      <c r="BN137"/>
-      <c r="BO137"/>
-      <c r="BP137"/>
-      <c r="BQ137"/>
-      <c r="BR137"/>
-      <c r="BS137"/>
-      <c r="BT137"/>
-      <c r="BU137"/>
-      <c r="BV137"/>
-      <c r="BW137"/>
-      <c r="BX137"/>
-      <c r="BY137"/>
-      <c r="BZ137"/>
-      <c r="CA137"/>
-      <c r="CB137"/>
-      <c r="CC137"/>
-      <c r="CD137"/>
-      <c r="CE137"/>
-      <c r="CF137"/>
-      <c r="CG137"/>
-      <c r="CH137"/>
-      <c r="CI137"/>
-      <c r="CJ137"/>
-      <c r="CK137"/>
-      <c r="CL137"/>
-      <c r="CM137"/>
-      <c r="CN137"/>
-      <c r="CO137"/>
-      <c r="CP137"/>
-      <c r="CQ137"/>
-      <c r="CR137"/>
-      <c r="CS137"/>
-      <c r="CT137"/>
-      <c r="CU137"/>
-      <c r="CV137"/>
-      <c r="CW137"/>
-      <c r="CX137"/>
-      <c r="CY137"/>
-      <c r="CZ137"/>
-      <c r="DA137"/>
-      <c r="DB137"/>
-      <c r="DC137"/>
-      <c r="DD137"/>
-      <c r="DE137"/>
-      <c r="DF137"/>
-      <c r="DG137"/>
-      <c r="DH137"/>
-      <c r="DI137"/>
-      <c r="DJ137"/>
-      <c r="DK137"/>
-      <c r="DL137"/>
-      <c r="DM137"/>
-      <c r="DN137"/>
-      <c r="DO137"/>
-      <c r="DP137"/>
-      <c r="DQ137"/>
-      <c r="DR137"/>
-      <c r="DS137"/>
-      <c r="DT137"/>
-      <c r="DU137"/>
-      <c r="DV137"/>
-      <c r="DW137"/>
-      <c r="DX137"/>
-      <c r="DY137"/>
-      <c r="DZ137"/>
-      <c r="EA137"/>
-      <c r="EB137"/>
-      <c r="EC137"/>
-      <c r="ED137"/>
-      <c r="EE137"/>
-      <c r="EF137"/>
-      <c r="EG137"/>
-      <c r="EH137"/>
-      <c r="EI137"/>
-      <c r="EJ137"/>
-      <c r="EK137"/>
-      <c r="EL137"/>
-      <c r="EM137"/>
-      <c r="EN137"/>
-      <c r="EO137"/>
-      <c r="EP137"/>
-      <c r="EQ137"/>
-      <c r="ER137"/>
-      <c r="ES137"/>
-      <c r="ET137"/>
-      <c r="EU137"/>
-      <c r="EV137"/>
-      <c r="EW137"/>
-      <c r="EX137"/>
-      <c r="EY137"/>
-      <c r="EZ137"/>
-      <c r="FA137"/>
-      <c r="FB137"/>
-      <c r="FC137"/>
-      <c r="FD137"/>
-      <c r="FE137"/>
-      <c r="FF137"/>
-      <c r="FG137"/>
-      <c r="FH137"/>
-      <c r="FI137"/>
-      <c r="FJ137"/>
-      <c r="FK137"/>
-      <c r="FL137"/>
-      <c r="FM137"/>
-      <c r="FN137"/>
-      <c r="FO137"/>
-      <c r="FP137"/>
-      <c r="FQ137"/>
-      <c r="FR137"/>
-      <c r="FS137"/>
-      <c r="FT137"/>
-      <c r="FU137"/>
-      <c r="FV137"/>
-      <c r="FW137"/>
-      <c r="FX137"/>
-      <c r="FY137"/>
-      <c r="FZ137"/>
-      <c r="GA137"/>
-      <c r="GB137"/>
-      <c r="GC137"/>
-      <c r="GD137"/>
-      <c r="GE137"/>
-      <c r="GF137"/>
-      <c r="GG137"/>
-      <c r="GH137"/>
-      <c r="GI137"/>
-      <c r="GJ137"/>
-      <c r="GK137"/>
-      <c r="GL137"/>
-      <c r="GM137"/>
-      <c r="GN137"/>
-      <c r="GO137"/>
-      <c r="GP137"/>
-      <c r="GQ137"/>
-      <c r="GR137"/>
-      <c r="GS137"/>
-      <c r="GT137"/>
-      <c r="GU137"/>
-      <c r="GV137"/>
-      <c r="GW137"/>
-      <c r="GX137"/>
-      <c r="GY137"/>
-      <c r="GZ137"/>
-      <c r="HA137"/>
-      <c r="HB137"/>
-      <c r="HC137"/>
-      <c r="HD137"/>
-      <c r="HE137"/>
-      <c r="HF137"/>
-      <c r="HG137"/>
-      <c r="HH137"/>
-      <c r="HI137"/>
-      <c r="HJ137"/>
-      <c r="HK137"/>
-      <c r="HL137"/>
-      <c r="HM137"/>
-      <c r="HN137"/>
-      <c r="HO137"/>
-      <c r="HP137"/>
-      <c r="HQ137"/>
-      <c r="HR137"/>
-      <c r="HS137"/>
-      <c r="HT137"/>
-      <c r="HU137"/>
-      <c r="HV137"/>
-      <c r="HW137"/>
-      <c r="HX137"/>
-      <c r="HY137"/>
-      <c r="HZ137"/>
-      <c r="IA137"/>
-      <c r="IB137"/>
-      <c r="IC137"/>
-      <c r="ID137"/>
-      <c r="IE137"/>
-      <c r="IF137"/>
-      <c r="IG137"/>
-      <c r="IH137"/>
-      <c r="II137"/>
-      <c r="IJ137"/>
-      <c r="IK137"/>
-      <c r="IL137"/>
-      <c r="IM137"/>
-      <c r="IN137"/>
-      <c r="IO137"/>
-      <c r="IP137"/>
-      <c r="IQ137"/>
-      <c r="IR137"/>
-      <c r="IS137"/>
-      <c r="IT137"/>
-      <c r="IU137"/>
+        <v>125</v>
+      </c>
     </row>
     <row r="138" spans="1:255" ht="28.35" customHeight="1">
       <c r="A138" s="23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B138" s="11"/>
       <c r="C138" s="11"/>
       <c r="D138" s="11"/>
       <c r="E138" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F138" s="24">
+        <v>1</v>
+      </c>
+      <c r="G138" s="25">
         <v>12</v>
       </c>
-      <c r="F138" s="24">
-        <v>25</v>
-      </c>
-      <c r="G138" s="25">
-        <v>5</v>
-      </c>
       <c r="H138" s="14">
         <f t="shared" si="2"/>
-        <v>125</v>
+        <v>12</v>
       </c>
     </row>
     <row r="139" spans="1:255" ht="28.35" customHeight="1">
       <c r="A139" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B139" s="11"/>
       <c r="C139" s="11"/>
@@ -5955,40 +6001,40 @@
         <v>21</v>
       </c>
       <c r="F139" s="24">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G139" s="25">
-        <v>12</v>
+        <v>1.36</v>
       </c>
       <c r="H139" s="14">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>10.88</v>
       </c>
     </row>
     <row r="140" spans="1:255" ht="28.35" customHeight="1">
       <c r="A140" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="B140" s="11"/>
+        <v>133</v>
+      </c>
+      <c r="B140" s="29"/>
       <c r="C140" s="11"/>
       <c r="D140" s="11"/>
       <c r="E140" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F140" s="24">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="G140" s="25">
-        <v>1.36</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H140" s="14">
         <f t="shared" si="2"/>
-        <v>10.88</v>
+        <v>48.400000000000006</v>
       </c>
     </row>
     <row r="141" spans="1:255" ht="28.35" customHeight="1">
       <c r="A141" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B141" s="29"/>
       <c r="C141" s="11"/>
@@ -5997,19 +6043,19 @@
         <v>21</v>
       </c>
       <c r="F141" s="24">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G141" s="25">
-        <v>2.2000000000000002</v>
+        <v>5.5</v>
       </c>
       <c r="H141" s="14">
         <f t="shared" si="2"/>
-        <v>48.400000000000006</v>
+        <v>88</v>
       </c>
     </row>
     <row r="142" spans="1:255" ht="28.35" customHeight="1">
       <c r="A142" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B142" s="29"/>
       <c r="C142" s="11"/>
@@ -6018,61 +6064,61 @@
         <v>21</v>
       </c>
       <c r="F142" s="24">
+        <v>40</v>
+      </c>
+      <c r="G142" s="25">
+        <v>0.4</v>
+      </c>
+      <c r="H142" s="14">
+        <f t="shared" si="2"/>
         <v>16</v>
-      </c>
-      <c r="G142" s="25">
-        <v>5.5</v>
-      </c>
-      <c r="H142" s="14">
-        <f t="shared" si="2"/>
-        <v>88</v>
       </c>
     </row>
     <row r="143" spans="1:255" ht="28.35" customHeight="1">
       <c r="A143" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="B143" s="29"/>
+        <v>136</v>
+      </c>
+      <c r="B143" s="11"/>
       <c r="C143" s="11"/>
       <c r="D143" s="11"/>
       <c r="E143" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F143" s="24">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="G143" s="25">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H143" s="14">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="144" spans="1:255" ht="28.35" customHeight="1">
       <c r="A144" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="B144" s="11"/>
+        <v>137</v>
+      </c>
+      <c r="B144" s="29"/>
       <c r="C144" s="11"/>
       <c r="D144" s="11"/>
       <c r="E144" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F144" s="24">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="G144" s="25">
-        <v>0.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H144" s="14">
         <f t="shared" si="2"/>
-        <v>3.5</v>
+        <v>31.900000000000002</v>
       </c>
     </row>
     <row r="145" spans="1:8" ht="28.35" customHeight="1">
       <c r="A145" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B145" s="29"/>
       <c r="C145" s="11"/>
@@ -6081,19 +6127,19 @@
         <v>21</v>
       </c>
       <c r="F145" s="24">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="G145" s="25">
-        <v>1.1000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="H145" s="14">
         <f t="shared" si="2"/>
-        <v>31.900000000000002</v>
+        <v>54</v>
       </c>
     </row>
     <row r="146" spans="1:8" ht="28.35" customHeight="1">
       <c r="A146" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B146" s="29"/>
       <c r="C146" s="11"/>
@@ -6102,19 +6148,19 @@
         <v>21</v>
       </c>
       <c r="F146" s="24">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="G146" s="25">
-        <v>0.9</v>
+        <v>2.85</v>
       </c>
       <c r="H146" s="14">
         <f t="shared" si="2"/>
-        <v>54</v>
+        <v>85.5</v>
       </c>
     </row>
     <row r="147" spans="1:8" ht="28.35" customHeight="1">
       <c r="A147" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B147" s="29"/>
       <c r="C147" s="11"/>
@@ -6123,56 +6169,58 @@
         <v>21</v>
       </c>
       <c r="F147" s="24">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="G147" s="25">
-        <v>2.85</v>
+        <v>3.4</v>
       </c>
       <c r="H147" s="14">
         <f t="shared" si="2"/>
-        <v>85.5</v>
+        <v>30.599999999999998</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="28.35" customHeight="1">
       <c r="A148" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="B148" s="29"/>
+        <v>141</v>
+      </c>
+      <c r="B148" s="11"/>
       <c r="C148" s="11"/>
       <c r="D148" s="11"/>
       <c r="E148" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F148" s="24">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G148" s="25">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="H148" s="14">
         <f t="shared" si="2"/>
-        <v>30.599999999999998</v>
+        <v>69</v>
       </c>
     </row>
     <row r="149" spans="1:8" ht="28.35" customHeight="1">
       <c r="A149" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B149" s="29"/>
+      <c r="C149" s="11"/>
+      <c r="D149" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="B149" s="11"/>
-      <c r="C149" s="11"/>
-      <c r="D149" s="11"/>
       <c r="E149" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F149" s="24">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G149" s="25">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="H149" s="14">
         <f t="shared" si="2"/>
-        <v>69</v>
+        <v>357</v>
       </c>
     </row>
     <row r="150" spans="1:8" ht="28.35" customHeight="1">
@@ -6188,14 +6236,14 @@
         <v>21</v>
       </c>
       <c r="F150" s="24">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="G150" s="25">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H150" s="14">
         <f t="shared" si="2"/>
-        <v>357</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="151" spans="1:8" ht="28.35" customHeight="1">
@@ -6205,164 +6253,136 @@
       <c r="B151" s="29"/>
       <c r="C151" s="11"/>
       <c r="D151" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E151" s="11" t="s">
         <v>21</v>
       </c>
       <c r="F151" s="24">
-        <v>100</v>
+        <v>9</v>
       </c>
       <c r="G151" s="25">
         <v>10</v>
       </c>
       <c r="H151" s="14">
         <f t="shared" si="2"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" ht="28.35" customHeight="1">
-      <c r="A152" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="B152" s="29"/>
-      <c r="C152" s="11"/>
-      <c r="D152" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="E152" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F152" s="24">
-        <v>9</v>
-      </c>
-      <c r="G152" s="25">
-        <v>10</v>
-      </c>
-      <c r="H152" s="14">
-        <f t="shared" si="2"/>
         <v>90</v>
       </c>
     </row>
-    <row r="153" spans="1:8" ht="48.75" customHeight="1">
-      <c r="H153" s="47">
-        <f>SUM(H3:H152)</f>
-        <v>19265.092000000001</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" ht="29.1" customHeight="1"/>
-    <row r="155" spans="1:8" ht="30" customHeight="1"/>
+    <row r="152" spans="1:8" ht="48.75" customHeight="1">
+      <c r="H152" s="47">
+        <f>SUM(H3:H151)</f>
+        <v>19342.092000000001</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" ht="29.1" customHeight="1"/>
+    <row r="154" spans="1:8" ht="30" customHeight="1"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="F116:F118 F85 F26:F29 F23:F24">
-    <cfRule type="cellIs" dxfId="21" priority="2" stopIfTrue="1" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="F115:F117 F84 F26:F29 F23:F24">
+    <cfRule type="cellIs" dxfId="20" priority="2" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F30:F31 F40:F41 F88:F90">
-    <cfRule type="cellIs" dxfId="20" priority="4" stopIfTrue="1" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="F39:F40 F87:F89 F30:F31">
+    <cfRule type="cellIs" dxfId="19" priority="4" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32:F33">
-    <cfRule type="cellIs" dxfId="19" priority="5" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="18" priority="5" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F37:F38">
-    <cfRule type="cellIs" dxfId="18" priority="6" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="6" stopIfTrue="1" operator="lessThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F39">
-    <cfRule type="cellIs" dxfId="17" priority="8" stopIfTrue="1" operator="lessThan">
-      <formula>10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F43:F44">
+  <conditionalFormatting sqref="F42:F43">
     <cfRule type="cellIs" dxfId="16" priority="10" stopIfTrue="1" operator="lessThan">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F45">
+  <conditionalFormatting sqref="F44">
     <cfRule type="cellIs" dxfId="15" priority="11" stopIfTrue="1" operator="lessThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F49 F86:F87 F106 F91:F92">
+  <conditionalFormatting sqref="F48 F85:F86 F105 F90:F91">
     <cfRule type="cellIs" dxfId="14" priority="12" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F53">
+  <conditionalFormatting sqref="F52">
     <cfRule type="cellIs" dxfId="13" priority="13" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F58 F74:F84">
+  <conditionalFormatting sqref="F57 F73:F83">
     <cfRule type="cellIs" dxfId="12" priority="14" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F63">
+  <conditionalFormatting sqref="F62">
     <cfRule type="cellIs" dxfId="11" priority="15" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F68">
+  <conditionalFormatting sqref="F67">
     <cfRule type="cellIs" dxfId="10" priority="16" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>35</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F69">
+  <conditionalFormatting sqref="F68">
     <cfRule type="cellIs" dxfId="9" priority="17" stopIfTrue="1" operator="lessThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F102 F97:F98">
+  <conditionalFormatting sqref="F101 F96:F97">
     <cfRule type="cellIs" dxfId="8" priority="24" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F119 F107">
+  <conditionalFormatting sqref="F118 F106">
     <cfRule type="cellIs" dxfId="7" priority="25" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>150</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F109:F112">
+  <conditionalFormatting sqref="F108:F111">
     <cfRule type="cellIs" dxfId="6" priority="28" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F105">
+  <conditionalFormatting sqref="F104">
     <cfRule type="cellIs" dxfId="5" priority="31" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F101">
+  <conditionalFormatting sqref="F100">
     <cfRule type="cellIs" dxfId="4" priority="33" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F99:F100">
+  <conditionalFormatting sqref="F98:F99">
     <cfRule type="cellIs" dxfId="3" priority="34" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F96">
+  <conditionalFormatting sqref="F95">
     <cfRule type="cellIs" dxfId="2" priority="36" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F94:F95">
+  <conditionalFormatting sqref="F93:F94">
     <cfRule type="cellIs" dxfId="1" priority="38" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F98">
+  <conditionalFormatting sqref="F97">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>10</formula>
     </cfRule>

</xml_diff>

<commit_message>
new new 21 maggio
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -1892,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IU154"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -2290,14 +2290,14 @@
         <v>12</v>
       </c>
       <c r="F9" s="17">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G9" s="13">
         <v>3</v>
       </c>
       <c r="H9" s="14">
         <f t="shared" si="0"/>
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
@@ -2344,14 +2344,14 @@
         <v>12</v>
       </c>
       <c r="F10" s="17">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G10" s="13">
         <v>2.35</v>
       </c>
       <c r="H10" s="14">
         <f t="shared" si="0"/>
-        <v>115.15</v>
+        <v>108.10000000000001</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -3027,14 +3027,14 @@
         <v>28</v>
       </c>
       <c r="F24" s="20">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="G24" s="21">
         <v>0.19</v>
       </c>
       <c r="H24" s="14">
         <f t="shared" si="1"/>
-        <v>47.5</v>
+        <v>28.5</v>
       </c>
     </row>
     <row r="25" spans="1:35" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3604,14 +3604,14 @@
         <v>12</v>
       </c>
       <c r="F49" s="20">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G49" s="21">
         <v>1</v>
       </c>
       <c r="H49" s="14">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4030,14 +4030,14 @@
         <v>21</v>
       </c>
       <c r="F67" s="20">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G67" s="21">
         <v>3</v>
       </c>
       <c r="H67" s="14">
         <f t="shared" si="1"/>
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="68" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4751,14 +4751,14 @@
         <v>21</v>
       </c>
       <c r="F98" s="20">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G98" s="43">
         <v>2.9</v>
       </c>
       <c r="H98" s="46">
         <f t="shared" si="2"/>
-        <v>284.2</v>
+        <v>281.3</v>
       </c>
       <c r="I98" s="42"/>
     </row>
@@ -4779,14 +4779,14 @@
         <v>21</v>
       </c>
       <c r="F99" s="20">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="G99" s="43">
         <v>4.8</v>
       </c>
       <c r="H99" s="46">
         <f t="shared" si="2"/>
-        <v>182.4</v>
+        <v>129.6</v>
       </c>
       <c r="I99" s="42"/>
     </row>
@@ -4891,14 +4891,14 @@
         <v>21</v>
       </c>
       <c r="F103" s="20">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="G103" s="43">
         <v>0.8</v>
       </c>
       <c r="H103" s="46">
         <f t="shared" si="2"/>
-        <v>38.400000000000006</v>
+        <v>28.8</v>
       </c>
       <c r="I103" s="42"/>
     </row>
@@ -6022,14 +6022,14 @@
         <v>21</v>
       </c>
       <c r="F140" s="24">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G140" s="25">
         <v>2.2000000000000002</v>
       </c>
       <c r="H140" s="14">
         <f t="shared" si="2"/>
-        <v>48.400000000000006</v>
+        <v>46.2</v>
       </c>
     </row>
     <row r="141" spans="1:255" ht="28.35" customHeight="1">
@@ -6064,14 +6064,14 @@
         <v>21</v>
       </c>
       <c r="F142" s="24">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G142" s="25">
         <v>0.4</v>
       </c>
       <c r="H142" s="14">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>15.600000000000001</v>
       </c>
     </row>
     <row r="143" spans="1:255" ht="28.35" customHeight="1">
@@ -6272,7 +6272,7 @@
     <row r="152" spans="1:8" ht="48.75" customHeight="1">
       <c r="H152" s="47">
         <f>SUM(H3:H151)</f>
-        <v>19342.092000000001</v>
+        <v>19226.142</v>
       </c>
     </row>
     <row r="153" spans="1:8" ht="29.1" customHeight="1"/>

</xml_diff>

<commit_message>
new new 21/a maggio
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -1892,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IU154"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -2494,14 +2494,14 @@
         <v>149</v>
       </c>
       <c r="F13" s="17">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G13" s="13">
         <v>0.6</v>
       </c>
       <c r="H13" s="14">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>6.6</v>
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -6272,7 +6272,7 @@
     <row r="152" spans="1:8" ht="48.75" customHeight="1">
       <c r="H152" s="47">
         <f>SUM(H3:H151)</f>
-        <v>19226.142</v>
+        <v>19223.741999999998</v>
       </c>
     </row>
     <row r="153" spans="1:8" ht="29.1" customHeight="1"/>

</xml_diff>

<commit_message>
new new 22 maggio
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -1892,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IU154"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -3242,14 +3242,14 @@
         <v>34</v>
       </c>
       <c r="F33" s="20">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="G33" s="21">
         <v>2.6</v>
       </c>
       <c r="H33" s="14">
         <f t="shared" si="1"/>
-        <v>130</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3445,14 +3445,14 @@
         <v>21</v>
       </c>
       <c r="F42" s="20">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="G42" s="21">
         <v>0.35</v>
       </c>
       <c r="H42" s="14">
         <f t="shared" si="1"/>
-        <v>201.25</v>
+        <v>200.54999999999998</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4779,14 +4779,14 @@
         <v>21</v>
       </c>
       <c r="F99" s="20">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G99" s="43">
         <v>4.8</v>
       </c>
       <c r="H99" s="46">
         <f t="shared" si="2"/>
-        <v>129.6</v>
+        <v>100.8</v>
       </c>
       <c r="I99" s="42"/>
     </row>
@@ -5423,14 +5423,14 @@
         <v>119</v>
       </c>
       <c r="F124" s="20">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G124" s="21">
         <v>7</v>
       </c>
       <c r="H124" s="14">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>28</v>
       </c>
     </row>
     <row r="125" spans="1:8" s="36" customFormat="1" ht="28.35" customHeight="1">
@@ -6272,7 +6272,7 @@
     <row r="152" spans="1:8" ht="48.75" customHeight="1">
       <c r="H152" s="47">
         <f>SUM(H3:H151)</f>
-        <v>19223.741999999998</v>
+        <v>19115.241999999998</v>
       </c>
     </row>
     <row r="153" spans="1:8" ht="29.1" customHeight="1"/>

</xml_diff>

<commit_message>
new new 24 maggio
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -1895,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IU155"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A118" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="C130" sqref="C129:C130"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A112" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="F123" sqref="F123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -5103,14 +5103,14 @@
         <v>21</v>
       </c>
       <c r="F110" s="20">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G110" s="21">
         <v>2</v>
       </c>
       <c r="H110" s="14">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -5440,14 +5440,14 @@
         <v>12</v>
       </c>
       <c r="F123" s="20">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G123" s="21">
         <v>3.3</v>
       </c>
       <c r="H123" s="14">
         <f t="shared" si="2"/>
-        <v>330</v>
+        <v>326.7</v>
       </c>
     </row>
     <row r="124" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -6337,7 +6337,7 @@
     <row r="153" spans="1:8" ht="48.75" customHeight="1">
       <c r="H153" s="47">
         <f>SUM(H3:H152)</f>
-        <v>19016.241999999998</v>
+        <v>19002.941999999999</v>
       </c>
     </row>
     <row r="154" spans="1:8" ht="29.1" customHeight="1"/>

</xml_diff>

<commit_message>
new new 28 maggio
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="238">
   <si>
     <t>PRODOTTO</t>
   </si>
@@ -710,9 +710,6 @@
     <t>30</t>
   </si>
   <si>
-    <t>130</t>
-  </si>
-  <si>
     <t>200</t>
   </si>
   <si>
@@ -729,6 +726,12 @@
   </si>
   <si>
     <t>90</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>23/5/2018</t>
   </si>
 </sst>
 </file>
@@ -1895,8 +1898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IU155"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A112" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="F123" sqref="F123"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -2436,7 +2439,7 @@
     </row>
     <row r="12" spans="1:35" ht="28.35" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B12" s="10">
         <v>43242</v>
@@ -3166,10 +3169,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D29" s="19"/>
       <c r="E29" s="19" t="s">
@@ -3191,10 +3194,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>207</v>
+        <v>237</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>169</v>
+        <v>236</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>28</v>
@@ -3239,10 +3242,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>28</v>
@@ -3290,7 +3293,7 @@
         <v>228</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>171</v>
@@ -3449,7 +3452,7 @@
     </row>
     <row r="41" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A41" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B41" s="19"/>
       <c r="C41" s="19"/>
@@ -4780,14 +4783,14 @@
         <v>21</v>
       </c>
       <c r="F98" s="20">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G98" s="43">
         <v>3.45</v>
       </c>
       <c r="H98" s="46">
         <f>F98*G98</f>
-        <v>358.8</v>
+        <v>355.35</v>
       </c>
       <c r="I98" s="42"/>
     </row>
@@ -4836,14 +4839,14 @@
         <v>21</v>
       </c>
       <c r="F100" s="20">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G100" s="43">
         <v>4.8</v>
       </c>
       <c r="H100" s="46">
         <f t="shared" si="2"/>
-        <v>86.399999999999991</v>
+        <v>76.8</v>
       </c>
       <c r="I100" s="42"/>
     </row>
@@ -5078,14 +5081,14 @@
         <v>21</v>
       </c>
       <c r="F109" s="20">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G109" s="21">
         <v>2.5</v>
       </c>
       <c r="H109" s="14">
         <f t="shared" si="2"/>
-        <v>260</v>
+        <v>257.5</v>
       </c>
     </row>
     <row r="110" spans="1:9" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -5093,7 +5096,7 @@
         <v>102</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C110" s="19" t="s">
         <v>167</v>
@@ -5118,7 +5121,7 @@
         <v>103</v>
       </c>
       <c r="B111" s="19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C111" s="19" t="s">
         <v>192</v>
@@ -5173,7 +5176,7 @@
         <v>228</v>
       </c>
       <c r="C113" s="19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D113" s="19" t="s">
         <v>155</v>
@@ -5599,14 +5602,14 @@
         <v>12</v>
       </c>
       <c r="F130" s="20">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="G130" s="21">
         <v>2.69</v>
       </c>
       <c r="H130" s="14">
         <f t="shared" si="2"/>
-        <v>672.5</v>
+        <v>403.5</v>
       </c>
     </row>
     <row r="131" spans="1:255" ht="28.35" customHeight="1">
@@ -6324,20 +6327,20 @@
         <v>21</v>
       </c>
       <c r="F152" s="24">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G152" s="25">
         <v>10</v>
       </c>
       <c r="H152" s="14">
         <f t="shared" si="2"/>
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="153" spans="1:8" ht="48.75" customHeight="1">
       <c r="H153" s="47">
         <f>SUM(H3:H152)</f>
-        <v>19002.941999999999</v>
+        <v>18708.391999999996</v>
       </c>
     </row>
     <row r="154" spans="1:8" ht="29.1" customHeight="1"/>

</xml_diff>

<commit_message>
new new 29 maggio
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="239">
   <si>
     <t>PRODOTTO</t>
   </si>
@@ -710,9 +710,6 @@
     <t>30</t>
   </si>
   <si>
-    <t>200</t>
-  </si>
-  <si>
     <t>150</t>
   </si>
   <si>
@@ -732,6 +729,12 @@
   </si>
   <si>
     <t>23/5/2018</t>
+  </si>
+  <si>
+    <t>25/5/2018</t>
+  </si>
+  <si>
+    <t>250</t>
   </si>
 </sst>
 </file>
@@ -1898,8 +1901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IU155"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A127" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="A136" sqref="A136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -2439,7 +2442,7 @@
     </row>
     <row r="12" spans="1:35" ht="28.35" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B12" s="10">
         <v>43242</v>
@@ -3169,10 +3172,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D29" s="19"/>
       <c r="E29" s="19" t="s">
@@ -3194,10 +3197,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>28</v>
@@ -3242,10 +3245,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>28</v>
@@ -3290,10 +3293,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>171</v>
@@ -3302,14 +3305,14 @@
         <v>34</v>
       </c>
       <c r="F34" s="20">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="G34" s="21">
         <v>2.6</v>
       </c>
       <c r="H34" s="14">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -3452,7 +3455,7 @@
     </row>
     <row r="41" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
       <c r="A41" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B41" s="19"/>
       <c r="C41" s="19"/>
@@ -4811,14 +4814,14 @@
         <v>21</v>
       </c>
       <c r="F99" s="20">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G99" s="43">
         <v>2.9</v>
       </c>
       <c r="H99" s="46">
         <f t="shared" si="2"/>
-        <v>281.3</v>
+        <v>275.5</v>
       </c>
       <c r="I99" s="42"/>
     </row>
@@ -5096,7 +5099,7 @@
         <v>102</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C110" s="19" t="s">
         <v>167</v>
@@ -5121,7 +5124,7 @@
         <v>103</v>
       </c>
       <c r="B111" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C111" s="19" t="s">
         <v>192</v>
@@ -5176,7 +5179,7 @@
         <v>228</v>
       </c>
       <c r="C113" s="19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D113" s="19" t="s">
         <v>155</v>
@@ -5629,14 +5632,14 @@
         <v>12</v>
       </c>
       <c r="F131" s="20">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G131" s="21">
         <v>2.21</v>
       </c>
       <c r="H131" s="14">
         <f t="shared" si="2"/>
-        <v>331.5</v>
+        <v>221</v>
       </c>
     </row>
     <row r="132" spans="1:255" ht="28.35" customHeight="1">
@@ -6340,7 +6343,7 @@
     <row r="153" spans="1:8" ht="48.75" customHeight="1">
       <c r="H153" s="47">
         <f>SUM(H3:H152)</f>
-        <v>18708.391999999996</v>
+        <v>18722.092000000001</v>
       </c>
     </row>
     <row r="154" spans="1:8" ht="29.1" customHeight="1"/>

</xml_diff>

<commit_message>
new new 30 maggio
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -1901,8 +1901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IU155"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A127" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="A136" sqref="A136"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A145" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -3185,11 +3185,11 @@
         <v>10</v>
       </c>
       <c r="G29" s="21">
-        <v>25.13</v>
+        <v>27.44</v>
       </c>
       <c r="H29" s="14">
         <f t="shared" si="1"/>
-        <v>251.29999999999998</v>
+        <v>274.40000000000003</v>
       </c>
     </row>
     <row r="30" spans="1:35" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -5188,14 +5188,14 @@
         <v>34</v>
       </c>
       <c r="F113" s="20">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="G113" s="21">
         <v>2.7</v>
       </c>
       <c r="H113" s="14">
         <f t="shared" si="2"/>
-        <v>162</v>
+        <v>81</v>
       </c>
     </row>
     <row r="114" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -6343,7 +6343,7 @@
     <row r="153" spans="1:8" ht="48.75" customHeight="1">
       <c r="H153" s="47">
         <f>SUM(H3:H152)</f>
-        <v>18722.092000000001</v>
+        <v>18664.191999999999</v>
       </c>
     </row>
     <row r="154" spans="1:8" ht="29.1" customHeight="1"/>

</xml_diff>

<commit_message>
new new 30-a maggio
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -1901,8 +1901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IU155"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A145" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A109" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="F124" sqref="F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.42578125" defaultRowHeight="12.75" customHeight="1"/>
@@ -3090,14 +3090,14 @@
         <v>28</v>
       </c>
       <c r="F25" s="20">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="G25" s="21">
         <v>0.19</v>
       </c>
       <c r="H25" s="14">
         <f t="shared" si="1"/>
-        <v>28.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:35" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -4926,14 +4926,14 @@
         <v>21</v>
       </c>
       <c r="F103" s="20">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G103" s="43">
         <v>4</v>
       </c>
       <c r="H103" s="46">
         <f t="shared" si="2"/>
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="I103" s="42"/>
     </row>
@@ -4954,14 +4954,14 @@
         <v>21</v>
       </c>
       <c r="F104" s="20">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="G104" s="43">
         <v>0.8</v>
       </c>
       <c r="H104" s="46">
         <f t="shared" si="2"/>
-        <v>28.8</v>
+        <v>19.200000000000003</v>
       </c>
       <c r="I104" s="42"/>
     </row>
@@ -5323,14 +5323,14 @@
         <v>21</v>
       </c>
       <c r="F118" s="20">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G118" s="21">
         <v>2.9</v>
       </c>
       <c r="H118" s="14">
         <f t="shared" si="2"/>
-        <v>17.399999999999999</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="119" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -5467,14 +5467,14 @@
         <v>10</v>
       </c>
       <c r="F124" s="20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G124" s="21">
         <v>2.87</v>
       </c>
       <c r="H124" s="14">
         <f t="shared" si="2"/>
-        <v>14.350000000000001</v>
+        <v>11.48</v>
       </c>
     </row>
     <row r="125" spans="1:8" s="22" customFormat="1" ht="28.35" customHeight="1">
@@ -6343,7 +6343,7 @@
     <row r="153" spans="1:8" ht="48.75" customHeight="1">
       <c r="H153" s="47">
         <f>SUM(H3:H152)</f>
-        <v>18664.191999999999</v>
+        <v>18560.721999999998</v>
       </c>
     </row>
     <row r="154" spans="1:8" ht="29.1" customHeight="1"/>

</xml_diff>

<commit_message>
Nuovo magazzino per il 2019
</commit_message>
<xml_diff>
--- a/magazzino2018.xlsx
+++ b/magazzino2018.xlsx
@@ -1304,8 +1304,8 @@
   </sheetPr>
   <dimension ref="A1:AI160"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B117" activeCellId="0" sqref="B117"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F78" activeCellId="0" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3770,14 +3770,14 @@
         <v>44</v>
       </c>
       <c r="F78" s="25" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G78" s="20" t="n">
         <v>33.5</v>
       </c>
       <c r="H78" s="16" t="n">
         <f aca="false">F78*G78</f>
-        <v>67</v>
+        <v>301.5</v>
       </c>
     </row>
     <row r="79" s="26" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3791,14 +3791,14 @@
         <v>44</v>
       </c>
       <c r="F79" s="25" t="n">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="G79" s="20" t="n">
         <v>33.5</v>
       </c>
       <c r="H79" s="16" t="n">
         <f aca="false">F79*G79</f>
-        <v>67</v>
+        <v>971.5</v>
       </c>
     </row>
     <row r="80" s="26" customFormat="true" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5684,7 +5684,7 @@
     <row r="158" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="H158" s="47" t="n">
         <f aca="false">SUM(H3:H157)</f>
-        <v>15593.47</v>
+        <v>16732.47</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>